<commit_message>
Report 16/17 02 2025.
</commit_message>
<xml_diff>
--- a/price_history_gold.xlsx
+++ b/price_history_gold.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1808"/>
+  <dimension ref="A1:E1947"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34200,7 +34200,7 @@
     </row>
     <row r="1670">
       <c r="A1670" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1670" t="inlineStr">
         <is>
@@ -34221,7 +34221,7 @@
     </row>
     <row r="1671">
       <c r="A1671" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1671" t="inlineStr">
         <is>
@@ -34242,7 +34242,7 @@
     </row>
     <row r="1672">
       <c r="A1672" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1672" t="inlineStr">
         <is>
@@ -34263,7 +34263,7 @@
     </row>
     <row r="1673">
       <c r="A1673" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1673" t="inlineStr">
         <is>
@@ -34284,7 +34284,7 @@
     </row>
     <row r="1674">
       <c r="A1674" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1674" t="inlineStr">
         <is>
@@ -34303,7 +34303,7 @@
     </row>
     <row r="1675">
       <c r="A1675" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1675" t="inlineStr">
         <is>
@@ -34324,7 +34324,7 @@
     </row>
     <row r="1676">
       <c r="A1676" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1676" t="inlineStr">
         <is>
@@ -34345,7 +34345,7 @@
     </row>
     <row r="1677">
       <c r="A1677" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1677" t="inlineStr">
         <is>
@@ -34366,7 +34366,7 @@
     </row>
     <row r="1678">
       <c r="A1678" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1678" t="inlineStr">
         <is>
@@ -34387,7 +34387,7 @@
     </row>
     <row r="1679">
       <c r="A1679" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1679" t="inlineStr">
         <is>
@@ -34408,7 +34408,7 @@
     </row>
     <row r="1680">
       <c r="A1680" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1680" t="inlineStr">
         <is>
@@ -34429,7 +34429,7 @@
     </row>
     <row r="1681">
       <c r="A1681" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1681" t="inlineStr">
         <is>
@@ -34450,7 +34450,7 @@
     </row>
     <row r="1682">
       <c r="A1682" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1682" t="inlineStr">
         <is>
@@ -34471,7 +34471,7 @@
     </row>
     <row r="1683">
       <c r="A1683" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1683" t="inlineStr">
         <is>
@@ -34492,7 +34492,7 @@
     </row>
     <row r="1684">
       <c r="A1684" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1684" t="inlineStr">
         <is>
@@ -34513,7 +34513,7 @@
     </row>
     <row r="1685">
       <c r="A1685" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1685" t="inlineStr">
         <is>
@@ -34534,7 +34534,7 @@
     </row>
     <row r="1686">
       <c r="A1686" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1686" t="inlineStr">
         <is>
@@ -34555,7 +34555,7 @@
     </row>
     <row r="1687">
       <c r="A1687" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1687" t="inlineStr">
         <is>
@@ -34576,7 +34576,7 @@
     </row>
     <row r="1688">
       <c r="A1688" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1688" t="inlineStr">
         <is>
@@ -34595,7 +34595,7 @@
     </row>
     <row r="1689">
       <c r="A1689" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1689" t="inlineStr">
         <is>
@@ -34616,7 +34616,7 @@
     </row>
     <row r="1690">
       <c r="A1690" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1690" t="inlineStr">
         <is>
@@ -34637,7 +34637,7 @@
     </row>
     <row r="1691">
       <c r="A1691" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1691" t="inlineStr">
         <is>
@@ -34658,7 +34658,7 @@
     </row>
     <row r="1692">
       <c r="A1692" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1692" t="inlineStr">
         <is>
@@ -34679,7 +34679,7 @@
     </row>
     <row r="1693">
       <c r="A1693" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1693" t="inlineStr">
         <is>
@@ -34700,7 +34700,7 @@
     </row>
     <row r="1694">
       <c r="A1694" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1694" t="inlineStr">
         <is>
@@ -34721,7 +34721,7 @@
     </row>
     <row r="1695">
       <c r="A1695" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1695" t="inlineStr">
         <is>
@@ -34742,7 +34742,7 @@
     </row>
     <row r="1696">
       <c r="A1696" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1696" t="inlineStr">
         <is>
@@ -34763,7 +34763,7 @@
     </row>
     <row r="1697">
       <c r="A1697" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1697" t="inlineStr">
         <is>
@@ -34784,7 +34784,7 @@
     </row>
     <row r="1698">
       <c r="A1698" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1698" t="inlineStr">
         <is>
@@ -34805,7 +34805,7 @@
     </row>
     <row r="1699">
       <c r="A1699" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1699" t="inlineStr">
         <is>
@@ -34826,7 +34826,7 @@
     </row>
     <row r="1700">
       <c r="A1700" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1700" t="inlineStr">
         <is>
@@ -34847,7 +34847,7 @@
     </row>
     <row r="1701">
       <c r="A1701" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1701" t="inlineStr">
         <is>
@@ -34868,7 +34868,7 @@
     </row>
     <row r="1702">
       <c r="A1702" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1702" t="inlineStr">
         <is>
@@ -34889,7 +34889,7 @@
     </row>
     <row r="1703">
       <c r="A1703" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1703" t="inlineStr">
         <is>
@@ -34910,7 +34910,7 @@
     </row>
     <row r="1704">
       <c r="A1704" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1704" t="inlineStr">
         <is>
@@ -34931,7 +34931,7 @@
     </row>
     <row r="1705">
       <c r="A1705" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1705" t="inlineStr">
         <is>
@@ -34952,7 +34952,7 @@
     </row>
     <row r="1706">
       <c r="A1706" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1706" t="inlineStr">
         <is>
@@ -34973,7 +34973,7 @@
     </row>
     <row r="1707">
       <c r="A1707" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1707" t="inlineStr">
         <is>
@@ -34994,7 +34994,7 @@
     </row>
     <row r="1708">
       <c r="A1708" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1708" t="inlineStr">
         <is>
@@ -35015,7 +35015,7 @@
     </row>
     <row r="1709">
       <c r="A1709" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1709" t="inlineStr">
         <is>
@@ -35036,7 +35036,7 @@
     </row>
     <row r="1710">
       <c r="A1710" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1710" t="inlineStr">
         <is>
@@ -35057,7 +35057,7 @@
     </row>
     <row r="1711">
       <c r="A1711" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1711" t="inlineStr">
         <is>
@@ -35078,7 +35078,7 @@
     </row>
     <row r="1712">
       <c r="A1712" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1712" t="inlineStr">
         <is>
@@ -35099,7 +35099,7 @@
     </row>
     <row r="1713">
       <c r="A1713" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1713" t="inlineStr">
         <is>
@@ -35120,7 +35120,7 @@
     </row>
     <row r="1714">
       <c r="A1714" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1714" t="inlineStr">
         <is>
@@ -35141,7 +35141,7 @@
     </row>
     <row r="1715">
       <c r="A1715" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1715" t="inlineStr">
         <is>
@@ -35162,7 +35162,7 @@
     </row>
     <row r="1716">
       <c r="A1716" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1716" t="inlineStr">
         <is>
@@ -35183,7 +35183,7 @@
     </row>
     <row r="1717">
       <c r="A1717" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1717" t="inlineStr">
         <is>
@@ -35204,7 +35204,7 @@
     </row>
     <row r="1718">
       <c r="A1718" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1718" t="inlineStr">
         <is>
@@ -35225,7 +35225,7 @@
     </row>
     <row r="1719">
       <c r="A1719" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1719" t="inlineStr">
         <is>
@@ -35246,7 +35246,7 @@
     </row>
     <row r="1720">
       <c r="A1720" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1720" t="inlineStr">
         <is>
@@ -35267,7 +35267,7 @@
     </row>
     <row r="1721">
       <c r="A1721" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1721" t="inlineStr">
         <is>
@@ -35288,7 +35288,7 @@
     </row>
     <row r="1722">
       <c r="A1722" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1722" t="inlineStr">
         <is>
@@ -35309,7 +35309,7 @@
     </row>
     <row r="1723">
       <c r="A1723" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1723" t="inlineStr">
         <is>
@@ -35330,7 +35330,7 @@
     </row>
     <row r="1724">
       <c r="A1724" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1724" t="inlineStr">
         <is>
@@ -35351,7 +35351,7 @@
     </row>
     <row r="1725">
       <c r="A1725" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1725" t="inlineStr">
         <is>
@@ -35372,7 +35372,7 @@
     </row>
     <row r="1726">
       <c r="A1726" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1726" t="inlineStr">
         <is>
@@ -35393,7 +35393,7 @@
     </row>
     <row r="1727">
       <c r="A1727" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1727" t="inlineStr">
         <is>
@@ -35414,7 +35414,7 @@
     </row>
     <row r="1728">
       <c r="A1728" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1728" t="inlineStr">
         <is>
@@ -35435,7 +35435,7 @@
     </row>
     <row r="1729">
       <c r="A1729" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1729" t="inlineStr">
         <is>
@@ -35456,7 +35456,7 @@
     </row>
     <row r="1730">
       <c r="A1730" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1730" t="inlineStr">
         <is>
@@ -35477,7 +35477,7 @@
     </row>
     <row r="1731">
       <c r="A1731" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1731" t="inlineStr">
         <is>
@@ -35498,7 +35498,7 @@
     </row>
     <row r="1732">
       <c r="A1732" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1732" t="inlineStr">
         <is>
@@ -35519,7 +35519,7 @@
     </row>
     <row r="1733">
       <c r="A1733" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1733" t="inlineStr">
         <is>
@@ -35540,7 +35540,7 @@
     </row>
     <row r="1734">
       <c r="A1734" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1734" t="inlineStr">
         <is>
@@ -35561,7 +35561,7 @@
     </row>
     <row r="1735">
       <c r="A1735" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1735" t="inlineStr">
         <is>
@@ -35582,7 +35582,7 @@
     </row>
     <row r="1736">
       <c r="A1736" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1736" t="inlineStr">
         <is>
@@ -35603,7 +35603,7 @@
     </row>
     <row r="1737">
       <c r="A1737" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1737" t="inlineStr">
         <is>
@@ -35624,7 +35624,7 @@
     </row>
     <row r="1738">
       <c r="A1738" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1738" t="inlineStr">
         <is>
@@ -35645,7 +35645,7 @@
     </row>
     <row r="1739">
       <c r="A1739" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1739" t="inlineStr">
         <is>
@@ -35666,7 +35666,7 @@
     </row>
     <row r="1740">
       <c r="A1740" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1740" t="inlineStr">
         <is>
@@ -35687,7 +35687,7 @@
     </row>
     <row r="1741">
       <c r="A1741" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1741" t="inlineStr">
         <is>
@@ -35708,7 +35708,7 @@
     </row>
     <row r="1742">
       <c r="A1742" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1742" t="inlineStr">
         <is>
@@ -35729,7 +35729,7 @@
     </row>
     <row r="1743">
       <c r="A1743" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1743" t="inlineStr">
         <is>
@@ -35750,7 +35750,7 @@
     </row>
     <row r="1744">
       <c r="A1744" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1744" t="inlineStr">
         <is>
@@ -35771,7 +35771,7 @@
     </row>
     <row r="1745">
       <c r="A1745" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1745" t="inlineStr">
         <is>
@@ -35792,7 +35792,7 @@
     </row>
     <row r="1746">
       <c r="A1746" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1746" t="inlineStr">
         <is>
@@ -35813,7 +35813,7 @@
     </row>
     <row r="1747">
       <c r="A1747" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1747" t="inlineStr">
         <is>
@@ -35832,7 +35832,7 @@
     </row>
     <row r="1748">
       <c r="A1748" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1748" t="inlineStr">
         <is>
@@ -35853,7 +35853,7 @@
     </row>
     <row r="1749">
       <c r="A1749" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1749" t="inlineStr">
         <is>
@@ -35874,7 +35874,7 @@
     </row>
     <row r="1750">
       <c r="A1750" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1750" t="inlineStr">
         <is>
@@ -35895,7 +35895,7 @@
     </row>
     <row r="1751">
       <c r="A1751" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1751" t="inlineStr">
         <is>
@@ -35916,7 +35916,7 @@
     </row>
     <row r="1752">
       <c r="A1752" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1752" t="inlineStr">
         <is>
@@ -35937,7 +35937,7 @@
     </row>
     <row r="1753">
       <c r="A1753" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1753" t="inlineStr">
         <is>
@@ -35958,7 +35958,7 @@
     </row>
     <row r="1754">
       <c r="A1754" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1754" t="inlineStr">
         <is>
@@ -35979,7 +35979,7 @@
     </row>
     <row r="1755">
       <c r="A1755" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1755" t="inlineStr">
         <is>
@@ -36000,7 +36000,7 @@
     </row>
     <row r="1756">
       <c r="A1756" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1756" t="inlineStr">
         <is>
@@ -36021,7 +36021,7 @@
     </row>
     <row r="1757">
       <c r="A1757" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1757" t="inlineStr">
         <is>
@@ -36042,7 +36042,7 @@
     </row>
     <row r="1758">
       <c r="A1758" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1758" t="inlineStr">
         <is>
@@ -36063,7 +36063,7 @@
     </row>
     <row r="1759">
       <c r="A1759" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1759" t="inlineStr">
         <is>
@@ -36084,7 +36084,7 @@
     </row>
     <row r="1760">
       <c r="A1760" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1760" t="inlineStr">
         <is>
@@ -36105,7 +36105,7 @@
     </row>
     <row r="1761">
       <c r="A1761" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1761" t="inlineStr">
         <is>
@@ -36126,7 +36126,7 @@
     </row>
     <row r="1762">
       <c r="A1762" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1762" t="inlineStr">
         <is>
@@ -36147,7 +36147,7 @@
     </row>
     <row r="1763">
       <c r="A1763" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1763" t="inlineStr">
         <is>
@@ -36168,7 +36168,7 @@
     </row>
     <row r="1764">
       <c r="A1764" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1764" t="inlineStr">
         <is>
@@ -36189,7 +36189,7 @@
     </row>
     <row r="1765">
       <c r="A1765" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1765" t="inlineStr">
         <is>
@@ -36210,7 +36210,7 @@
     </row>
     <row r="1766">
       <c r="A1766" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1766" t="inlineStr">
         <is>
@@ -36231,7 +36231,7 @@
     </row>
     <row r="1767">
       <c r="A1767" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1767" t="inlineStr">
         <is>
@@ -36252,7 +36252,7 @@
     </row>
     <row r="1768">
       <c r="A1768" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1768" t="inlineStr">
         <is>
@@ -36273,7 +36273,7 @@
     </row>
     <row r="1769">
       <c r="A1769" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1769" t="inlineStr">
         <is>
@@ -36294,7 +36294,7 @@
     </row>
     <row r="1770">
       <c r="A1770" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1770" t="inlineStr">
         <is>
@@ -36315,7 +36315,7 @@
     </row>
     <row r="1771">
       <c r="A1771" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1771" t="inlineStr">
         <is>
@@ -36334,7 +36334,7 @@
     </row>
     <row r="1772">
       <c r="A1772" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1772" t="inlineStr">
         <is>
@@ -36355,7 +36355,7 @@
     </row>
     <row r="1773">
       <c r="A1773" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1773" t="inlineStr">
         <is>
@@ -36376,7 +36376,7 @@
     </row>
     <row r="1774">
       <c r="A1774" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1774" t="inlineStr">
         <is>
@@ -36397,7 +36397,7 @@
     </row>
     <row r="1775">
       <c r="A1775" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1775" t="inlineStr">
         <is>
@@ -36416,7 +36416,7 @@
     </row>
     <row r="1776">
       <c r="A1776" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1776" t="inlineStr">
         <is>
@@ -36435,7 +36435,7 @@
     </row>
     <row r="1777">
       <c r="A1777" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1777" t="inlineStr">
         <is>
@@ -36454,7 +36454,7 @@
     </row>
     <row r="1778">
       <c r="A1778" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1778" t="inlineStr">
         <is>
@@ -36473,7 +36473,7 @@
     </row>
     <row r="1779">
       <c r="A1779" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1779" t="inlineStr">
         <is>
@@ -36492,7 +36492,7 @@
     </row>
     <row r="1780">
       <c r="A1780" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1780" t="inlineStr">
         <is>
@@ -36511,7 +36511,7 @@
     </row>
     <row r="1781">
       <c r="A1781" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1781" t="inlineStr">
         <is>
@@ -36530,7 +36530,7 @@
     </row>
     <row r="1782">
       <c r="A1782" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1782" t="inlineStr">
         <is>
@@ -36549,7 +36549,7 @@
     </row>
     <row r="1783">
       <c r="A1783" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1783" t="inlineStr">
         <is>
@@ -36568,7 +36568,7 @@
     </row>
     <row r="1784">
       <c r="A1784" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1784" t="inlineStr">
         <is>
@@ -36587,7 +36587,7 @@
     </row>
     <row r="1785">
       <c r="A1785" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1785" t="inlineStr">
         <is>
@@ -36606,7 +36606,7 @@
     </row>
     <row r="1786">
       <c r="A1786" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1786" t="inlineStr">
         <is>
@@ -36625,7 +36625,7 @@
     </row>
     <row r="1787">
       <c r="A1787" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1787" t="inlineStr">
         <is>
@@ -36644,7 +36644,7 @@
     </row>
     <row r="1788">
       <c r="A1788" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1788" t="inlineStr">
         <is>
@@ -36663,7 +36663,7 @@
     </row>
     <row r="1789">
       <c r="A1789" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1789" t="inlineStr">
         <is>
@@ -36682,7 +36682,7 @@
     </row>
     <row r="1790">
       <c r="A1790" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1790" t="inlineStr">
         <is>
@@ -36701,7 +36701,7 @@
     </row>
     <row r="1791">
       <c r="A1791" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1791" t="inlineStr">
         <is>
@@ -36720,7 +36720,7 @@
     </row>
     <row r="1792">
       <c r="A1792" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1792" t="inlineStr">
         <is>
@@ -36739,7 +36739,7 @@
     </row>
     <row r="1793">
       <c r="A1793" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1793" t="inlineStr">
         <is>
@@ -36758,7 +36758,7 @@
     </row>
     <row r="1794">
       <c r="A1794" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1794" t="inlineStr">
         <is>
@@ -36777,7 +36777,7 @@
     </row>
     <row r="1795">
       <c r="A1795" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1795" t="inlineStr">
         <is>
@@ -36796,7 +36796,7 @@
     </row>
     <row r="1796">
       <c r="A1796" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1796" t="inlineStr">
         <is>
@@ -36815,7 +36815,7 @@
     </row>
     <row r="1797">
       <c r="A1797" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1797" t="inlineStr">
         <is>
@@ -36834,7 +36834,7 @@
     </row>
     <row r="1798">
       <c r="A1798" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1798" t="inlineStr">
         <is>
@@ -36853,7 +36853,7 @@
     </row>
     <row r="1799">
       <c r="A1799" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1799" t="inlineStr">
         <is>
@@ -36872,7 +36872,7 @@
     </row>
     <row r="1800">
       <c r="A1800" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1800" t="inlineStr">
         <is>
@@ -36891,7 +36891,7 @@
     </row>
     <row r="1801">
       <c r="A1801" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1801" t="inlineStr">
         <is>
@@ -36910,7 +36910,7 @@
     </row>
     <row r="1802">
       <c r="A1802" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1802" t="inlineStr">
         <is>
@@ -36929,7 +36929,7 @@
     </row>
     <row r="1803">
       <c r="A1803" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1803" t="inlineStr">
         <is>
@@ -36948,7 +36948,7 @@
     </row>
     <row r="1804">
       <c r="A1804" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1804" t="inlineStr">
         <is>
@@ -36967,7 +36967,7 @@
     </row>
     <row r="1805">
       <c r="A1805" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1805" t="inlineStr">
         <is>
@@ -36986,7 +36986,7 @@
     </row>
     <row r="1806">
       <c r="A1806" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1806" t="inlineStr">
         <is>
@@ -37005,7 +37005,7 @@
     </row>
     <row r="1807">
       <c r="A1807" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1807" t="inlineStr">
         <is>
@@ -37024,7 +37024,7 @@
     </row>
     <row r="1808">
       <c r="A1808" s="2" t="n">
-        <v>45701.8873072424</v>
+        <v>45701.88730724537</v>
       </c>
       <c r="B1808" t="inlineStr">
         <is>
@@ -37036,6 +37036,2847 @@
       </c>
       <c r="D1808" t="inlineStr"/>
       <c r="E1808" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-kilogram-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1809">
+      <c r="A1809" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1809" t="inlineStr">
+        <is>
+          <t>1 грам абонаментно златно кюлче Tavex</t>
+        </is>
+      </c>
+      <c r="C1809" t="n">
+        <v>179</v>
+      </c>
+      <c r="D1809" t="n">
+        <v>197</v>
+      </c>
+      <c r="E1809" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-abonamentno-zlatno-kulche-tavex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1810">
+      <c r="A1810" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1810" t="inlineStr">
+        <is>
+          <t>0,25 грама златно кюлче Tavex</t>
+        </is>
+      </c>
+      <c r="C1810" t="n">
+        <v>48</v>
+      </c>
+      <c r="D1810" t="n">
+        <v>52</v>
+      </c>
+      <c r="E1810" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/0-25-gr-zlatno-kyulche-tavex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1811">
+      <c r="A1811" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1811" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Британия</t>
+        </is>
+      </c>
+      <c r="C1811" t="n">
+        <v>5519</v>
+      </c>
+      <c r="D1811" t="n">
+        <v>5576</v>
+      </c>
+      <c r="E1811" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-britaniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1812">
+      <c r="A1812" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1812" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Виенска Филхармония</t>
+        </is>
+      </c>
+      <c r="C1812" t="n">
+        <v>5519</v>
+      </c>
+      <c r="D1812" t="n">
+        <v>5603</v>
+      </c>
+      <c r="E1812" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-vienska-filharmoniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1813">
+      <c r="A1813" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1813" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Британия</t>
+        </is>
+      </c>
+      <c r="C1813" t="n">
+        <v>5519</v>
+      </c>
+      <c r="D1813" t="inlineStr"/>
+      <c r="E1813" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlatna-moneta-britaniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1814">
+      <c r="A1814" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1814" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Виенска Филхармония</t>
+        </is>
+      </c>
+      <c r="C1814" t="n">
+        <v>571</v>
+      </c>
+      <c r="D1814" t="n">
+        <v>626</v>
+      </c>
+      <c r="E1814" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-%d1%83%d0%bd%d1%86%d0%b8%d1%8f-%d0%b7%d0%bb%d0%b0%d1%82%d0%bd%d0%b0-%d0%b0%d0%b2%d1%81%d1%82%d1%80%d0%b8%d0%b9%d1%81%d0%ba%d0%b0-%d1%84%d0%b8%d0%bb%d1%85%d0%b0%d1%80%d0%bc%d0%be%d0%bd%d0%b8%d1%8f/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1815">
+      <c r="A1815" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1815" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Канадски кленов лист</t>
+        </is>
+      </c>
+      <c r="C1815" t="n">
+        <v>5519</v>
+      </c>
+      <c r="D1815" t="n">
+        <v>5598</v>
+      </c>
+      <c r="E1815" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-kanadski-klenov-list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1816">
+      <c r="A1816" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1816" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийско кенгуру</t>
+        </is>
+      </c>
+      <c r="C1816" t="n">
+        <v>5519</v>
+      </c>
+      <c r="D1816" t="n">
+        <v>5576</v>
+      </c>
+      <c r="E1816" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliysko-kenguru/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1817">
+      <c r="A1817" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1817" t="inlineStr">
+        <is>
+          <t>100 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1817" t="n">
+        <v>17378</v>
+      </c>
+      <c r="D1817" t="n">
+        <v>17667</v>
+      </c>
+      <c r="E1817" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/100-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1818">
+      <c r="A1818" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1818" t="inlineStr">
+        <is>
+          <t>100 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1818" t="n">
+        <v>17378</v>
+      </c>
+      <c r="D1818" t="n">
+        <v>17684</v>
+      </c>
+      <c r="E1818" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/100-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1819">
+      <c r="A1819" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1819" t="inlineStr">
+        <is>
+          <t>0,25 г златно кюлче Tavex, подаръчен пакет</t>
+        </is>
+      </c>
+      <c r="C1819" t="n">
+        <v>48</v>
+      </c>
+      <c r="D1819" t="n">
+        <v>71</v>
+      </c>
+      <c r="E1819" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/0-25-gr-zlatno-kyulche-tavex-podarachen-paket/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1820">
+      <c r="A1820" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1820" t="inlineStr">
+        <is>
+          <t>50 x 1 грам комбинирано кюлче Valcambi Suisse CombiBar</t>
+        </is>
+      </c>
+      <c r="C1820" t="n">
+        <v>8837</v>
+      </c>
+      <c r="D1820" t="n">
+        <v>9155</v>
+      </c>
+      <c r="E1820" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-kombinirano-zlatno-kulche-valcambi-combibar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1821">
+      <c r="A1821" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1821" t="inlineStr">
+        <is>
+          <t>50 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1821" t="n">
+        <v>8837</v>
+      </c>
+      <c r="D1821" t="n">
+        <v>8920</v>
+      </c>
+      <c r="E1821" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1822">
+      <c r="A1822" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1822" t="inlineStr">
+        <is>
+          <t>50 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1822" t="n">
+        <v>8837</v>
+      </c>
+      <c r="D1822" t="n">
+        <v>8929</v>
+      </c>
+      <c r="E1822" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1823">
+      <c r="A1823" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1823" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1823" t="n">
+        <v>5503</v>
+      </c>
+      <c r="D1823" t="n">
+        <v>5555</v>
+      </c>
+      <c r="E1823" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1824">
+      <c r="A1824" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1824" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче PAMP Suisse</t>
+        </is>
+      </c>
+      <c r="C1824" t="n">
+        <v>5503</v>
+      </c>
+      <c r="D1824" t="n">
+        <v>5557</v>
+      </c>
+      <c r="E1824" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatno-kulche-pamp-suisse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1825">
+      <c r="A1825" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1825" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1825" t="n">
+        <v>5503</v>
+      </c>
+      <c r="D1825" t="n">
+        <v>5560</v>
+      </c>
+      <c r="E1825" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1826">
+      <c r="A1826" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1826" t="inlineStr">
+        <is>
+          <t>20 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1826" t="n">
+        <v>3583</v>
+      </c>
+      <c r="D1826" t="n">
+        <v>3634</v>
+      </c>
+      <c r="E1826" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1827">
+      <c r="A1827" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1827" t="inlineStr">
+        <is>
+          <t>20 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C1827" t="n">
+        <v>3583</v>
+      </c>
+      <c r="D1827" t="inlineStr"/>
+      <c r="E1827" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1828">
+      <c r="A1828" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1828" t="inlineStr">
+        <is>
+          <t>20 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1828" t="n">
+        <v>3583</v>
+      </c>
+      <c r="D1828" t="n">
+        <v>3641</v>
+      </c>
+      <c r="E1828" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1829">
+      <c r="A1829" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1829" t="inlineStr">
+        <is>
+          <t>10 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1829" t="n">
+        <v>1792</v>
+      </c>
+      <c r="D1829" t="n">
+        <v>1852</v>
+      </c>
+      <c r="E1829" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1830">
+      <c r="A1830" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1830" t="inlineStr">
+        <is>
+          <t>10 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C1830" t="n">
+        <v>1792</v>
+      </c>
+      <c r="D1830" t="n">
+        <v>1869</v>
+      </c>
+      <c r="E1830" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1831">
+      <c r="A1831" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1831" t="inlineStr">
+        <is>
+          <t>10 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1831" t="n">
+        <v>1792</v>
+      </c>
+      <c r="D1831" t="n">
+        <v>1854</v>
+      </c>
+      <c r="E1831" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1832">
+      <c r="A1832" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1832" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1832" t="n">
+        <v>905</v>
+      </c>
+      <c r="D1832" t="n">
+        <v>978</v>
+      </c>
+      <c r="E1832" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1833">
+      <c r="A1833" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1833" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C1833" t="n">
+        <v>905</v>
+      </c>
+      <c r="D1833" t="n">
+        <v>992</v>
+      </c>
+      <c r="E1833" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1834">
+      <c r="A1834" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1834" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1834" t="n">
+        <v>905</v>
+      </c>
+      <c r="D1834" t="n">
+        <v>979</v>
+      </c>
+      <c r="E1834" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1835">
+      <c r="A1835" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1835" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C1835" t="n">
+        <v>939</v>
+      </c>
+      <c r="D1835" t="n">
+        <v>1028</v>
+      </c>
+      <c r="E1835" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-pamp-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1836">
+      <c r="A1836" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1836" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Argor-Heraeus лунар Змия 2025</t>
+        </is>
+      </c>
+      <c r="C1836" t="n">
+        <v>913</v>
+      </c>
+      <c r="D1836" t="n">
+        <v>1015</v>
+      </c>
+      <c r="E1836" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-argor-heraeus-lunar-zmiya-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1837">
+      <c r="A1837" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1837" t="inlineStr">
+        <is>
+          <t>2,5 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1837" t="n">
+        <v>465</v>
+      </c>
+      <c r="D1837" t="n">
+        <v>520</v>
+      </c>
+      <c r="E1837" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/2-5-grama-zlatno-kyulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1838">
+      <c r="A1838" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1838" t="inlineStr">
+        <is>
+          <t>2,5 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C1838" t="n">
+        <v>465</v>
+      </c>
+      <c r="D1838" t="n">
+        <v>524</v>
+      </c>
+      <c r="E1838" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/dva-grama-i-polovina-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1839">
+      <c r="A1839" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1839" t="inlineStr">
+        <is>
+          <t>2 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1839" t="n">
+        <v>372</v>
+      </c>
+      <c r="D1839" t="n">
+        <v>416</v>
+      </c>
+      <c r="E1839" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/2-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1840">
+      <c r="A1840" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1840" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1840" t="n">
+        <v>182</v>
+      </c>
+      <c r="D1840" t="n">
+        <v>219</v>
+      </c>
+      <c r="E1840" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1841">
+      <c r="A1841" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1841" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C1841" t="n">
+        <v>182</v>
+      </c>
+      <c r="D1841" t="n">
+        <v>221</v>
+      </c>
+      <c r="E1841" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1842">
+      <c r="A1842" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1842" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1842" t="n">
+        <v>182</v>
+      </c>
+      <c r="D1842" t="n">
+        <v>217</v>
+      </c>
+      <c r="E1842" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1843">
+      <c r="A1843" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1843" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Argor-Heraeus лунар Змия 2025</t>
+        </is>
+      </c>
+      <c r="C1843" t="n">
+        <v>208</v>
+      </c>
+      <c r="D1843" t="n">
+        <v>264</v>
+      </c>
+      <c r="E1843" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kyulche-argor-heraeus-lunar-zmiya-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1844">
+      <c r="A1844" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1844" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Американски орел</t>
+        </is>
+      </c>
+      <c r="C1844" t="n">
+        <v>5519</v>
+      </c>
+      <c r="D1844" t="n">
+        <v>5743</v>
+      </c>
+      <c r="E1844" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-uncia-amerikanski-orel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1845">
+      <c r="A1845" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1845" t="inlineStr">
+        <is>
+          <t>20 долара двоен орел лейди Либърти</t>
+        </is>
+      </c>
+      <c r="C1845" t="n">
+        <v>5182</v>
+      </c>
+      <c r="D1845" t="n">
+        <v>6104</v>
+      </c>
+      <c r="E1845" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-dolara-dvoen-orel-lejdi-libarti/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1846">
+      <c r="A1846" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1846" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Американски бизон</t>
+        </is>
+      </c>
+      <c r="C1846" t="n">
+        <v>5600</v>
+      </c>
+      <c r="D1846" t="n">
+        <v>5851</v>
+      </c>
+      <c r="E1846" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-amerikanski-bizon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1847">
+      <c r="A1847" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1847" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Кругерранд, Южна Африка</t>
+        </is>
+      </c>
+      <c r="C1847" t="n">
+        <v>5443</v>
+      </c>
+      <c r="D1847" t="n">
+        <v>5555</v>
+      </c>
+      <c r="E1847" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-krugerrand-yujna-afrika/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1848">
+      <c r="A1848" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1848" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Слон Южна Африка - Големите 5</t>
+        </is>
+      </c>
+      <c r="C1848" t="n">
+        <v>5519</v>
+      </c>
+      <c r="D1848" t="n">
+        <v>5635</v>
+      </c>
+      <c r="E1848" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-slon-yuzhna-afrika-golemite-5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1849">
+      <c r="A1849" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1849" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C1849" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1849" t="n">
+        <v>6256</v>
+      </c>
+      <c r="E1849" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1850">
+      <c r="A1850" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1850" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C1850" t="n">
+        <v>5682</v>
+      </c>
+      <c r="D1850" t="n">
+        <v>5964</v>
+      </c>
+      <c r="E1850" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1851">
+      <c r="A1851" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1851" t="inlineStr">
+        <is>
+          <t>1/4 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C1851" t="n">
+        <v>1420</v>
+      </c>
+      <c r="D1851" t="n">
+        <v>1618</v>
+      </c>
+      <c r="E1851" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-4-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1852">
+      <c r="A1852" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1852" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C1852" t="n">
+        <v>568</v>
+      </c>
+      <c r="D1852" t="n">
+        <v>701</v>
+      </c>
+      <c r="E1852" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1853">
+      <c r="A1853" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1853" t="inlineStr">
+        <is>
+          <t>1/20 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C1853" t="n">
+        <v>271</v>
+      </c>
+      <c r="D1853" t="n">
+        <v>396</v>
+      </c>
+      <c r="E1853" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-20-unciya-zlaten-avstraliiski-lunar-godina-na-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1854">
+      <c r="A1854" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1854" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C1854" t="n">
+        <v>5627</v>
+      </c>
+      <c r="D1854" t="n">
+        <v>5743</v>
+      </c>
+      <c r="E1854" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1855">
+      <c r="A1855" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1855" t="inlineStr">
+        <is>
+          <t>1/2 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C1855" t="n">
+        <v>2760</v>
+      </c>
+      <c r="D1855" t="n">
+        <v>3074</v>
+      </c>
+      <c r="E1855" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-2-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1856">
+      <c r="A1856" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1856" t="inlineStr">
+        <is>
+          <t>1/4 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C1856" t="n">
+        <v>1420</v>
+      </c>
+      <c r="D1856" t="n">
+        <v>1591</v>
+      </c>
+      <c r="E1856" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-4-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1857">
+      <c r="A1857" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1857" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C1857" t="n">
+        <v>568</v>
+      </c>
+      <c r="D1857" t="n">
+        <v>691</v>
+      </c>
+      <c r="E1857" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1858">
+      <c r="A1858" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1858" t="inlineStr">
+        <is>
+          <t>1/20 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C1858" t="n">
+        <v>271</v>
+      </c>
+      <c r="D1858" t="n">
+        <v>396</v>
+      </c>
+      <c r="E1858" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-20-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1859">
+      <c r="A1859" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1859" t="inlineStr">
+        <is>
+          <t>Руска златна монета 5 рубли Николай II</t>
+        </is>
+      </c>
+      <c r="C1859" t="n">
+        <v>741</v>
+      </c>
+      <c r="D1859" t="n">
+        <v>972</v>
+      </c>
+      <c r="E1859" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-5-rubli-nikolay-iii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1860">
+      <c r="A1860" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1860" t="inlineStr">
+        <is>
+          <t>10 рубли Николай II Русия</t>
+        </is>
+      </c>
+      <c r="C1860" t="n">
+        <v>1482</v>
+      </c>
+      <c r="D1860" t="n">
+        <v>2013</v>
+      </c>
+      <c r="E1860" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-rubli-nikolai-ii-rusia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1861">
+      <c r="A1861" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1861" t="inlineStr">
+        <is>
+          <t>20 френски франка Наполеон III</t>
+        </is>
+      </c>
+      <c r="C1861" t="n">
+        <v>1031</v>
+      </c>
+      <c r="D1861" t="n">
+        <v>1060</v>
+      </c>
+      <c r="E1861" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-frenski-franka-napoleon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1862">
+      <c r="A1862" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1862" t="inlineStr">
+        <is>
+          <t>20 френски франка златна монета Наполеон III с лавров венец</t>
+        </is>
+      </c>
+      <c r="C1862" t="n">
+        <v>1031</v>
+      </c>
+      <c r="D1862" t="n">
+        <v>1060</v>
+      </c>
+      <c r="E1862" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-%d1%84%d1%80%d0%b0%d0%bd%d0%ba%d0%b0-%d1%84%d1%80%d0%b5%d0%bd%d1%81%d0%ba%d0%b8-%d0%bd%d0%b0%d0%bf%d0%be%d0%bb%d0%b5%d0%be%d0%bd-%d1%81-%d0%bb%d0%b0%d0%b2%d1%80%d0%be%d0%b2-%d0%b2%d0%b5%d0%bd%d0%b5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1863">
+      <c r="A1863" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1863" t="inlineStr">
+        <is>
+          <t>10 франка френски Наполеон III</t>
+        </is>
+      </c>
+      <c r="C1863" t="n">
+        <v>561</v>
+      </c>
+      <c r="D1863" t="n">
+        <v>642</v>
+      </c>
+      <c r="E1863" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-frenski-franka-napoleon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1864">
+      <c r="A1864" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1864" t="inlineStr">
+        <is>
+          <t>10 френски франка златна монета Наполеон III с лавров венец</t>
+        </is>
+      </c>
+      <c r="C1864" t="n">
+        <v>561</v>
+      </c>
+      <c r="D1864" t="n">
+        <v>642</v>
+      </c>
+      <c r="E1864" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-frenski-franka-zlatna-moneta-napoleon-iii-s-lavrov-venets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1865">
+      <c r="A1865" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1865" t="inlineStr">
+        <is>
+          <t>Златна монета 20 френски франка Серес</t>
+        </is>
+      </c>
+      <c r="C1865" t="n">
+        <v>1031</v>
+      </c>
+      <c r="D1865" t="n">
+        <v>1060</v>
+      </c>
+      <c r="E1865" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-frenski-franka-seres/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1866">
+      <c r="A1866" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1866" t="inlineStr">
+        <is>
+          <t>20 френски франка златна монета Гениус</t>
+        </is>
+      </c>
+      <c r="C1866" t="n">
+        <v>1031</v>
+      </c>
+      <c r="D1866" t="n">
+        <v>1060</v>
+      </c>
+      <c r="E1866" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-zlatni-frenski-franka-genius/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1867">
+      <c r="A1867" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1867" t="inlineStr">
+        <is>
+          <t>Златна монета 20 франка Мариана</t>
+        </is>
+      </c>
+      <c r="C1867" t="n">
+        <v>1031</v>
+      </c>
+      <c r="D1867" t="n">
+        <v>1060</v>
+      </c>
+      <c r="E1867" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-frenski-franka-mariana/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1868">
+      <c r="A1868" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1868" t="inlineStr">
+        <is>
+          <t>20 белгийски франка златна монета Леополд II</t>
+        </is>
+      </c>
+      <c r="C1868" t="n">
+        <v>1033</v>
+      </c>
+      <c r="D1868" t="n">
+        <v>1062</v>
+      </c>
+      <c r="E1868" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-belgiiski-franka-leopold-ii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1869">
+      <c r="A1869" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1869" t="inlineStr">
+        <is>
+          <t>20 лири Виктор Емануил II Италия</t>
+        </is>
+      </c>
+      <c r="C1869" t="n">
+        <v>1033</v>
+      </c>
+      <c r="D1869" t="n">
+        <v>1077</v>
+      </c>
+      <c r="E1869" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/italian-20lira-emanuele/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1870">
+      <c r="A1870" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1870" t="inlineStr">
+        <is>
+          <t>20 лири златна монета Умберто I, Италия</t>
+        </is>
+      </c>
+      <c r="C1870" t="n">
+        <v>1033</v>
+      </c>
+      <c r="D1870" t="n">
+        <v>1062</v>
+      </c>
+      <c r="E1870" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-liri-zlatna-moneta-umberto-i-italiya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1871">
+      <c r="A1871" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1871" t="inlineStr">
+        <is>
+          <t>4 австрийски дуката златна монета Франц Йосиф</t>
+        </is>
+      </c>
+      <c r="C1871" t="n">
+        <v>2395</v>
+      </c>
+      <c r="D1871" t="n">
+        <v>2590</v>
+      </c>
+      <c r="E1871" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-4-avstriiski-dukata-franc-iosif/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1872">
+      <c r="A1872" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1872" t="inlineStr">
+        <is>
+          <t>1 австрийски дукат златна монета Франц Йосиф</t>
+        </is>
+      </c>
+      <c r="C1872" t="n">
+        <v>616</v>
+      </c>
+      <c r="D1872" t="n">
+        <v>650</v>
+      </c>
+      <c r="E1872" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-1-avstriiski-dukat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1873">
+      <c r="A1873" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1873" t="inlineStr">
+        <is>
+          <t>8 форинта/20 франка Франц Йосиф Унгария</t>
+        </is>
+      </c>
+      <c r="C1873" t="n">
+        <v>1031</v>
+      </c>
+      <c r="D1873" t="n">
+        <v>1088</v>
+      </c>
+      <c r="E1873" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-forinta-20-franka-franc-iosif-ungariia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1874">
+      <c r="A1874" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1874" t="inlineStr">
+        <is>
+          <t>Златна монета 4 флорина/10 франка Франц Йосиф, Австрия</t>
+        </is>
+      </c>
+      <c r="C1874" t="n">
+        <v>540</v>
+      </c>
+      <c r="D1874" t="n">
+        <v>578</v>
+      </c>
+      <c r="E1874" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-4-florina-10-franka-franc-iosif-avstria/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1875">
+      <c r="A1875" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1875" t="inlineStr">
+        <is>
+          <t>20 франка златна монета Швейцария Вренели</t>
+        </is>
+      </c>
+      <c r="C1875" t="n">
+        <v>1031</v>
+      </c>
+      <c r="D1875" t="n">
+        <v>1062</v>
+      </c>
+      <c r="E1875" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-zlatni-franka-shveitsariya-vreneli/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1876">
+      <c r="A1876" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1876" t="inlineStr">
+        <is>
+          <t>10 гулдена Вилхелмина Холандия</t>
+        </is>
+      </c>
+      <c r="C1876" t="n">
+        <v>1048</v>
+      </c>
+      <c r="D1876" t="n">
+        <v>1139</v>
+      </c>
+      <c r="E1876" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-guldena-vilhemina-holandiya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1877">
+      <c r="A1877" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1877" t="inlineStr">
+        <is>
+          <t>20 германски марки Вилхелм II</t>
+        </is>
+      </c>
+      <c r="C1877" t="n">
+        <v>1259</v>
+      </c>
+      <c r="D1877" t="n">
+        <v>1354</v>
+      </c>
+      <c r="E1877" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-germanski-marki-vilhelm-ii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1878">
+      <c r="A1878" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1878" t="inlineStr">
+        <is>
+          <t>Златен Мемориален Суверен Чарлз III Великобритания 2022г.</t>
+        </is>
+      </c>
+      <c r="C1878" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D1878" t="n">
+        <v>1358</v>
+      </c>
+      <c r="E1878" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-memorialen-suveren-charles-iii-2022/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1879">
+      <c r="A1879" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1879" t="inlineStr">
+        <is>
+          <t>Златен Суверен Чарлз III Великобритания</t>
+        </is>
+      </c>
+      <c r="C1879" t="n">
+        <v>1305</v>
+      </c>
+      <c r="D1879" t="n">
+        <v>1364</v>
+      </c>
+      <c r="E1879" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-charles-iii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1880">
+      <c r="A1880" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1880" t="inlineStr">
+        <is>
+          <t>Златен суверен Елизабет II 1957-2021 Великобритания</t>
+        </is>
+      </c>
+      <c r="C1880" t="n">
+        <v>1274</v>
+      </c>
+      <c r="D1880" t="n">
+        <v>1323</v>
+      </c>
+      <c r="E1880" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/suveren-elizabet-ii-velikobritaniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1881">
+      <c r="A1881" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1881" t="inlineStr">
+        <is>
+          <t>Златен суверен Едуард VII Великобритания</t>
+        </is>
+      </c>
+      <c r="C1881" t="n">
+        <v>1274</v>
+      </c>
+      <c r="D1881" t="n">
+        <v>1345</v>
+      </c>
+      <c r="E1881" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-eduard-vii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1882">
+      <c r="A1882" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1882" t="inlineStr">
+        <is>
+          <t>Златен суверен Джордж V Великобритания</t>
+        </is>
+      </c>
+      <c r="C1882" t="n">
+        <v>1274</v>
+      </c>
+      <c r="D1882" t="n">
+        <v>1345</v>
+      </c>
+      <c r="E1882" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-jorge-v/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1883">
+      <c r="A1883" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1883" t="inlineStr">
+        <is>
+          <t>Златен суверен Виктория Великобритания</t>
+        </is>
+      </c>
+      <c r="C1883" t="n">
+        <v>1274</v>
+      </c>
+      <c r="D1883" t="n">
+        <v>1358</v>
+      </c>
+      <c r="E1883" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-viktoriya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1884">
+      <c r="A1884" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1884" t="inlineStr">
+        <is>
+          <t>Британски златен суверен Елизабет II, 2022г.</t>
+        </is>
+      </c>
+      <c r="C1884" t="n">
+        <v>1274</v>
+      </c>
+      <c r="D1884" t="inlineStr"/>
+      <c r="E1884" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-britanski-suveren-elizabet-ii-2022/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1885">
+      <c r="A1885" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1885" t="inlineStr">
+        <is>
+          <t>20 франка златна монета Тунис</t>
+        </is>
+      </c>
+      <c r="C1885" t="n">
+        <v>1026</v>
+      </c>
+      <c r="D1885" t="n">
+        <v>1118</v>
+      </c>
+      <c r="E1885" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-franka-zlatna-moneta-tunis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1886">
+      <c r="A1886" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1886" t="inlineStr">
+        <is>
+          <t>Златна монета 100 турски куруша</t>
+        </is>
+      </c>
+      <c r="C1886" t="n">
+        <v>1026</v>
+      </c>
+      <c r="D1886" t="inlineStr"/>
+      <c r="E1886" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-100-turski-kurusha/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1887">
+      <c r="A1887" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1887" t="inlineStr">
+        <is>
+          <t>50 песос Мексико</t>
+        </is>
+      </c>
+      <c r="C1887" t="n">
+        <v>6523</v>
+      </c>
+      <c r="D1887" t="n">
+        <v>6924</v>
+      </c>
+      <c r="E1887" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni38s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-8/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1888">
+      <c r="A1888" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1888" t="inlineStr">
+        <is>
+          <t>Златна монета 100 австрийски корони Франц Йосиф</t>
+        </is>
+      </c>
+      <c r="C1888" t="n">
+        <v>5224</v>
+      </c>
+      <c r="D1888" t="n">
+        <v>5603</v>
+      </c>
+      <c r="E1888" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-100-avstriyski-koroni-franc-yosif/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1889">
+      <c r="A1889" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1889" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C1889" t="n">
+        <v>5323</v>
+      </c>
+      <c r="D1889" t="n">
+        <v>5643</v>
+      </c>
+      <c r="E1889" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1890">
+      <c r="A1890" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1890" t="inlineStr">
+        <is>
+          <t>15 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C1890" t="n">
+        <v>2661</v>
+      </c>
+      <c r="D1890" t="n">
+        <v>2912</v>
+      </c>
+      <c r="E1890" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/15-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1891">
+      <c r="A1891" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1891" t="inlineStr">
+        <is>
+          <t>8 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C1891" t="n">
+        <v>1419</v>
+      </c>
+      <c r="D1891" t="n">
+        <v>1595</v>
+      </c>
+      <c r="E1891" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1892">
+      <c r="A1892" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1892" t="inlineStr">
+        <is>
+          <t>3 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C1892" t="n">
+        <v>532</v>
+      </c>
+      <c r="D1892" t="n">
+        <v>676</v>
+      </c>
+      <c r="E1892" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/3-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1893">
+      <c r="A1893" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1893" t="inlineStr">
+        <is>
+          <t>1 грам златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C1893" t="n">
+        <v>177</v>
+      </c>
+      <c r="D1893" t="n">
+        <v>269</v>
+      </c>
+      <c r="E1893" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1894">
+      <c r="A1894" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1894" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Тигъра 2022</t>
+        </is>
+      </c>
+      <c r="C1894" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1894" t="n">
+        <v>8089</v>
+      </c>
+      <c r="E1894" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-oz-australian-lunar-year-of-the-tiger-2022-gold-coin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1895">
+      <c r="A1895" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1895" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Вола 2021</t>
+        </is>
+      </c>
+      <c r="C1895" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1895" t="n">
+        <v>6471</v>
+      </c>
+      <c r="E1895" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-oz-australian-lunar-year-of-the-ox-2021-gold-coin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1896">
+      <c r="A1896" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1896" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийски лунар година на Мишката 2020</t>
+        </is>
+      </c>
+      <c r="C1896" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1896" t="n">
+        <v>6363</v>
+      </c>
+      <c r="E1896" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyski-lunar-godina-mishkata-2020/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1897">
+      <c r="A1897" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1897" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Кучето 2018</t>
+        </is>
+      </c>
+      <c r="C1897" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1897" t="n">
+        <v>6363</v>
+      </c>
+      <c r="E1897" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni38s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-22/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1898">
+      <c r="A1898" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1898" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Петела 2017</t>
+        </is>
+      </c>
+      <c r="C1898" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1898" t="n">
+        <v>6363</v>
+      </c>
+      <c r="E1898" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni40s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-24/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1899">
+      <c r="A1899" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1899" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Маймуната 2016</t>
+        </is>
+      </c>
+      <c r="C1899" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1899" t="n">
+        <v>6363</v>
+      </c>
+      <c r="E1899" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-maimunata-2016/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1900">
+      <c r="A1900" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1900" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Змията 2013</t>
+        </is>
+      </c>
+      <c r="C1900" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1900" t="n">
+        <v>6471</v>
+      </c>
+      <c r="E1900" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlaten-avstraliiski-lunar-godina-na-zmiyata-2013/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1901">
+      <c r="A1901" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1901" t="inlineStr">
+        <is>
+          <t>1 унция австралиисйки лунар година на дракона 2012</t>
+        </is>
+      </c>
+      <c r="C1901" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1901" t="n">
+        <v>6363</v>
+      </c>
+      <c r="E1901" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-drakona-2012/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1902">
+      <c r="A1902" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1902" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Заека 2011</t>
+        </is>
+      </c>
+      <c r="C1902" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1902" t="n">
+        <v>6363</v>
+      </c>
+      <c r="E1902" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-moneta-avstraliiski-lunar-zaek-2011/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1903">
+      <c r="A1903" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1903" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Вола 2009</t>
+        </is>
+      </c>
+      <c r="C1903" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1903" t="n">
+        <v>6363</v>
+      </c>
+      <c r="E1903" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-avstraliiski-lunar-godina-na-vola-2009/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1904">
+      <c r="A1904" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1904" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Мишката 2008</t>
+        </is>
+      </c>
+      <c r="C1904" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1904" t="n">
+        <v>6363</v>
+      </c>
+      <c r="E1904" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-uncia-moneta-lunar-mishka-2008/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1905">
+      <c r="A1905" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1905" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Прасето 2007</t>
+        </is>
+      </c>
+      <c r="C1905" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1905" t="n">
+        <v>6363</v>
+      </c>
+      <c r="E1905" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-avstraliiski-lunar-godina-na-praseto-2007/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1906">
+      <c r="A1906" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1906" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Петела 2005</t>
+        </is>
+      </c>
+      <c r="C1906" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1906" t="n">
+        <v>6363</v>
+      </c>
+      <c r="E1906" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-petela-2005/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1907">
+      <c r="A1907" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1907" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Маймуната 2004</t>
+        </is>
+      </c>
+      <c r="C1907" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1907" t="n">
+        <v>6363</v>
+      </c>
+      <c r="E1907" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-%d1%83%d0%bd%d1%86%d0%b8%d1%8f-%d0%b7%d0%bb%d0%b0%d1%82%d0%b5%d0%bd-%d0%b0%d0%b2%d1%81%d1%82%d1%80%d0%b0%d0%bb%d0%b8%d0%b9%d1%81%d0%ba%d0%b8-%d0%bb%d1%83%d0%bd%d0%b0%d1%80-%d0%b3%d0%be%d0%b4%d0%b8-2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1908">
+      <c r="A1908" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1908" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Козата 2003</t>
+        </is>
+      </c>
+      <c r="C1908" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1908" t="n">
+        <v>6363</v>
+      </c>
+      <c r="E1908" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni38s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-24/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1909">
+      <c r="A1909" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1909" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийки Лунар 2000 година на дракона</t>
+        </is>
+      </c>
+      <c r="C1909" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1909" t="n">
+        <v>7280</v>
+      </c>
+      <c r="E1909" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyki-lunar-2000-godina-drakona/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1910">
+      <c r="A1910" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1910" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Тигъра 2010</t>
+        </is>
+      </c>
+      <c r="C1910" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1910" t="inlineStr"/>
+      <c r="E1910" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-tigura-2010/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1911">
+      <c r="A1911" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1911" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Кучето 2006</t>
+        </is>
+      </c>
+      <c r="C1911" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1911" t="n">
+        <v>6363</v>
+      </c>
+      <c r="E1911" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-kucheto-2006/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1912">
+      <c r="A1912" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1912" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Тигъра 1998</t>
+        </is>
+      </c>
+      <c r="C1912" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1912" t="n">
+        <v>6741</v>
+      </c>
+      <c r="E1912" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliiski-lunar-godinata-na-tigara-1998/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1913">
+      <c r="A1913" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1913" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Вола 1997</t>
+        </is>
+      </c>
+      <c r="C1913" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1913" t="n">
+        <v>6741</v>
+      </c>
+      <c r="E1913" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliiski-lunar-godinata-na-vola-1997/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1914">
+      <c r="A1914" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1914" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Мишката 1996</t>
+        </is>
+      </c>
+      <c r="C1914" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1914" t="inlineStr"/>
+      <c r="E1914" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni42s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1915">
+      <c r="A1915" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1915" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Коня 2014</t>
+        </is>
+      </c>
+      <c r="C1915" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1915" t="inlineStr"/>
+      <c r="E1915" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-konq-2014/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1916">
+      <c r="A1916" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1916" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Argor-Heraeus лунар Дракон 2024</t>
+        </is>
+      </c>
+      <c r="C1916" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1916" t="inlineStr"/>
+      <c r="E1916" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-argor-heraeus-lunar-drakon-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1917">
+      <c r="A1917" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1917" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Argor-Heraeus лунар Дракон 2024</t>
+        </is>
+      </c>
+      <c r="C1917" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1917" t="inlineStr"/>
+      <c r="E1917" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kyulche-argor-heraeus-lunar-drakon-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1918">
+      <c r="A1918" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1918" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C1918" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1918" t="inlineStr"/>
+      <c r="E1918" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1919">
+      <c r="A1919" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1919" t="inlineStr">
+        <is>
+          <t>15 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C1919" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1919" t="inlineStr"/>
+      <c r="E1919" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/15-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1920">
+      <c r="A1920" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1920" t="inlineStr">
+        <is>
+          <t>8 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C1920" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1920" t="inlineStr"/>
+      <c r="E1920" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1921">
+      <c r="A1921" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1921" t="inlineStr">
+        <is>
+          <t>3 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C1921" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1921" t="inlineStr"/>
+      <c r="E1921" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/3-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1922">
+      <c r="A1922" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1922" t="inlineStr">
+        <is>
+          <t>1 грам златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C1922" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1922" t="inlineStr"/>
+      <c r="E1922" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1923">
+      <c r="A1923" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1923" t="inlineStr">
+        <is>
+          <t>1/2 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C1923" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1923" t="inlineStr"/>
+      <c r="E1923" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-2-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1924">
+      <c r="A1924" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1924" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Драконът на Тюдор 2024г.</t>
+        </is>
+      </c>
+      <c r="C1924" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1924" t="inlineStr"/>
+      <c r="E1924" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-pazitelite-na-tudorite-drakonat-na-tudor-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1925">
+      <c r="A1925" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1925" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Еднорогът на Сиймор 2024 г.</t>
+        </is>
+      </c>
+      <c r="C1925" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1925" t="inlineStr"/>
+      <c r="E1925" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-pazitelite-na-tyudorite-ednorogut-na-siimor-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1926">
+      <c r="A1926" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1926" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Бикът от Кларънс 2023 г.</t>
+        </is>
+      </c>
+      <c r="C1926" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1926" t="inlineStr"/>
+      <c r="E1926" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-pazitelite-na-tyudorite-bikut-ot-klaruns-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1927">
+      <c r="A1927" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1927" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Британия - Елизабет II</t>
+        </is>
+      </c>
+      <c r="C1927" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1927" t="inlineStr"/>
+      <c r="E1927" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-britaniya-elizabet-ii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1928">
+      <c r="A1928" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1928" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Йейлът на Бофорт 2023 г.</t>
+        </is>
+      </c>
+      <c r="C1928" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1928" t="inlineStr"/>
+      <c r="E1928" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-oz-zlatna-moneta-pazitelite-na-tyudorite-yeylut-na-bofort-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1929">
+      <c r="A1929" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1929" t="inlineStr">
+        <is>
+          <t>1/2 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C1929" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1929" t="inlineStr"/>
+      <c r="E1929" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-2-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1930">
+      <c r="A1930" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1930" t="inlineStr">
+        <is>
+          <t>1/4 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C1930" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1930" t="inlineStr"/>
+      <c r="E1930" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-4-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1931">
+      <c r="A1931" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1931" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C1931" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1931" t="inlineStr"/>
+      <c r="E1931" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-pamp-lunar-drakon-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1932">
+      <c r="A1932" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1932" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C1932" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1932" t="inlineStr"/>
+      <c r="E1932" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-pamp-lunar-zaek-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1933">
+      <c r="A1933" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1933" t="inlineStr">
+        <is>
+          <t>1/10 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C1933" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1933" t="inlineStr"/>
+      <c r="E1933" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1934">
+      <c r="A1934" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1934" t="inlineStr">
+        <is>
+          <t>15 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C1934" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1934" t="inlineStr"/>
+      <c r="E1934" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/15-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1935">
+      <c r="A1935" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1935" t="inlineStr">
+        <is>
+          <t>1/20 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C1935" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1935" t="inlineStr"/>
+      <c r="E1935" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-20-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1936">
+      <c r="A1936" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1936" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C1936" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1936" t="inlineStr"/>
+      <c r="E1936" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1937">
+      <c r="A1937" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1937" t="inlineStr">
+        <is>
+          <t>8 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C1937" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1937" t="inlineStr"/>
+      <c r="E1937" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1938">
+      <c r="A1938" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1938" t="inlineStr">
+        <is>
+          <t>3 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C1938" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1938" t="inlineStr"/>
+      <c r="E1938" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/3-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1939">
+      <c r="A1939" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1939" t="inlineStr">
+        <is>
+          <t>1 грам златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C1939" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1939" t="inlineStr"/>
+      <c r="E1939" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1940">
+      <c r="A1940" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1940" t="inlineStr">
+        <is>
+          <t>100 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C1940" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1940" t="inlineStr"/>
+      <c r="E1940" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/100-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1941">
+      <c r="A1941" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1941" t="inlineStr">
+        <is>
+          <t>50 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C1941" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1941" t="inlineStr"/>
+      <c r="E1941" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1942">
+      <c r="A1942" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1942" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C1942" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1942" t="inlineStr"/>
+      <c r="E1942" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1943">
+      <c r="A1943" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1943" t="inlineStr">
+        <is>
+          <t>10 крони Кристиян X Дания</t>
+        </is>
+      </c>
+      <c r="C1943" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1943" t="inlineStr"/>
+      <c r="E1943" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-kroni-kristiyan-x-daniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1944">
+      <c r="A1944" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1944" t="inlineStr">
+        <is>
+          <t>10 Гулдена Вилхелм III Холандия</t>
+        </is>
+      </c>
+      <c r="C1944" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1944" t="inlineStr"/>
+      <c r="E1944" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni38s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-9/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1945">
+      <c r="A1945" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1945" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2022</t>
+        </is>
+      </c>
+      <c r="C1945" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1945" t="inlineStr"/>
+      <c r="E1945" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitayska-panda-2022/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1946">
+      <c r="A1946" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1946" t="inlineStr">
+        <is>
+          <t>Златна монета 10 франка Мариана</t>
+        </is>
+      </c>
+      <c r="C1946" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1946" t="inlineStr"/>
+      <c r="E1946" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-frenski-franka-mariana/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1947">
+      <c r="A1947" s="2" t="n">
+        <v>45705.0167971608</v>
+      </c>
+      <c r="B1947" t="inlineStr">
+        <is>
+          <t>1 килограм златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1947" t="n">
+        <v>5573</v>
+      </c>
+      <c r="D1947" t="inlineStr"/>
+      <c r="E1947" t="inlineStr">
         <is>
           <t>https://tavex.bg/zlato/1-kilogram-zlatno-kulche-valcambi/</t>
         </is>

</xml_diff>

<commit_message>
Report 18 02 2025
</commit_message>
<xml_diff>
--- a/price_history_gold.xlsx
+++ b/price_history_gold.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1947"/>
+  <dimension ref="A1:E2086"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37043,7 +37043,7 @@
     </row>
     <row r="1809">
       <c r="A1809" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1809" t="inlineStr">
         <is>
@@ -37064,7 +37064,7 @@
     </row>
     <row r="1810">
       <c r="A1810" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1810" t="inlineStr">
         <is>
@@ -37085,7 +37085,7 @@
     </row>
     <row r="1811">
       <c r="A1811" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1811" t="inlineStr">
         <is>
@@ -37106,7 +37106,7 @@
     </row>
     <row r="1812">
       <c r="A1812" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1812" t="inlineStr">
         <is>
@@ -37127,7 +37127,7 @@
     </row>
     <row r="1813">
       <c r="A1813" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1813" t="inlineStr">
         <is>
@@ -37146,7 +37146,7 @@
     </row>
     <row r="1814">
       <c r="A1814" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1814" t="inlineStr">
         <is>
@@ -37167,7 +37167,7 @@
     </row>
     <row r="1815">
       <c r="A1815" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1815" t="inlineStr">
         <is>
@@ -37188,7 +37188,7 @@
     </row>
     <row r="1816">
       <c r="A1816" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1816" t="inlineStr">
         <is>
@@ -37209,7 +37209,7 @@
     </row>
     <row r="1817">
       <c r="A1817" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1817" t="inlineStr">
         <is>
@@ -37230,7 +37230,7 @@
     </row>
     <row r="1818">
       <c r="A1818" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1818" t="inlineStr">
         <is>
@@ -37251,7 +37251,7 @@
     </row>
     <row r="1819">
       <c r="A1819" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1819" t="inlineStr">
         <is>
@@ -37272,7 +37272,7 @@
     </row>
     <row r="1820">
       <c r="A1820" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1820" t="inlineStr">
         <is>
@@ -37293,7 +37293,7 @@
     </row>
     <row r="1821">
       <c r="A1821" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1821" t="inlineStr">
         <is>
@@ -37314,7 +37314,7 @@
     </row>
     <row r="1822">
       <c r="A1822" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1822" t="inlineStr">
         <is>
@@ -37335,7 +37335,7 @@
     </row>
     <row r="1823">
       <c r="A1823" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1823" t="inlineStr">
         <is>
@@ -37356,7 +37356,7 @@
     </row>
     <row r="1824">
       <c r="A1824" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1824" t="inlineStr">
         <is>
@@ -37377,7 +37377,7 @@
     </row>
     <row r="1825">
       <c r="A1825" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1825" t="inlineStr">
         <is>
@@ -37398,7 +37398,7 @@
     </row>
     <row r="1826">
       <c r="A1826" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1826" t="inlineStr">
         <is>
@@ -37419,7 +37419,7 @@
     </row>
     <row r="1827">
       <c r="A1827" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1827" t="inlineStr">
         <is>
@@ -37438,7 +37438,7 @@
     </row>
     <row r="1828">
       <c r="A1828" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1828" t="inlineStr">
         <is>
@@ -37459,7 +37459,7 @@
     </row>
     <row r="1829">
       <c r="A1829" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1829" t="inlineStr">
         <is>
@@ -37480,7 +37480,7 @@
     </row>
     <row r="1830">
       <c r="A1830" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1830" t="inlineStr">
         <is>
@@ -37501,7 +37501,7 @@
     </row>
     <row r="1831">
       <c r="A1831" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1831" t="inlineStr">
         <is>
@@ -37522,7 +37522,7 @@
     </row>
     <row r="1832">
       <c r="A1832" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1832" t="inlineStr">
         <is>
@@ -37543,7 +37543,7 @@
     </row>
     <row r="1833">
       <c r="A1833" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1833" t="inlineStr">
         <is>
@@ -37564,7 +37564,7 @@
     </row>
     <row r="1834">
       <c r="A1834" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1834" t="inlineStr">
         <is>
@@ -37585,7 +37585,7 @@
     </row>
     <row r="1835">
       <c r="A1835" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1835" t="inlineStr">
         <is>
@@ -37606,7 +37606,7 @@
     </row>
     <row r="1836">
       <c r="A1836" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1836" t="inlineStr">
         <is>
@@ -37627,7 +37627,7 @@
     </row>
     <row r="1837">
       <c r="A1837" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1837" t="inlineStr">
         <is>
@@ -37648,7 +37648,7 @@
     </row>
     <row r="1838">
       <c r="A1838" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1838" t="inlineStr">
         <is>
@@ -37669,7 +37669,7 @@
     </row>
     <row r="1839">
       <c r="A1839" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1839" t="inlineStr">
         <is>
@@ -37690,7 +37690,7 @@
     </row>
     <row r="1840">
       <c r="A1840" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1840" t="inlineStr">
         <is>
@@ -37711,7 +37711,7 @@
     </row>
     <row r="1841">
       <c r="A1841" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1841" t="inlineStr">
         <is>
@@ -37732,7 +37732,7 @@
     </row>
     <row r="1842">
       <c r="A1842" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1842" t="inlineStr">
         <is>
@@ -37753,7 +37753,7 @@
     </row>
     <row r="1843">
       <c r="A1843" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1843" t="inlineStr">
         <is>
@@ -37774,7 +37774,7 @@
     </row>
     <row r="1844">
       <c r="A1844" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1844" t="inlineStr">
         <is>
@@ -37795,7 +37795,7 @@
     </row>
     <row r="1845">
       <c r="A1845" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1845" t="inlineStr">
         <is>
@@ -37816,7 +37816,7 @@
     </row>
     <row r="1846">
       <c r="A1846" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1846" t="inlineStr">
         <is>
@@ -37837,7 +37837,7 @@
     </row>
     <row r="1847">
       <c r="A1847" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1847" t="inlineStr">
         <is>
@@ -37858,7 +37858,7 @@
     </row>
     <row r="1848">
       <c r="A1848" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1848" t="inlineStr">
         <is>
@@ -37879,7 +37879,7 @@
     </row>
     <row r="1849">
       <c r="A1849" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1849" t="inlineStr">
         <is>
@@ -37900,7 +37900,7 @@
     </row>
     <row r="1850">
       <c r="A1850" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1850" t="inlineStr">
         <is>
@@ -37921,7 +37921,7 @@
     </row>
     <row r="1851">
       <c r="A1851" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1851" t="inlineStr">
         <is>
@@ -37942,7 +37942,7 @@
     </row>
     <row r="1852">
       <c r="A1852" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1852" t="inlineStr">
         <is>
@@ -37963,7 +37963,7 @@
     </row>
     <row r="1853">
       <c r="A1853" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1853" t="inlineStr">
         <is>
@@ -37984,7 +37984,7 @@
     </row>
     <row r="1854">
       <c r="A1854" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1854" t="inlineStr">
         <is>
@@ -38005,7 +38005,7 @@
     </row>
     <row r="1855">
       <c r="A1855" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1855" t="inlineStr">
         <is>
@@ -38026,7 +38026,7 @@
     </row>
     <row r="1856">
       <c r="A1856" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1856" t="inlineStr">
         <is>
@@ -38047,7 +38047,7 @@
     </row>
     <row r="1857">
       <c r="A1857" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1857" t="inlineStr">
         <is>
@@ -38068,7 +38068,7 @@
     </row>
     <row r="1858">
       <c r="A1858" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1858" t="inlineStr">
         <is>
@@ -38089,7 +38089,7 @@
     </row>
     <row r="1859">
       <c r="A1859" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1859" t="inlineStr">
         <is>
@@ -38110,7 +38110,7 @@
     </row>
     <row r="1860">
       <c r="A1860" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1860" t="inlineStr">
         <is>
@@ -38131,7 +38131,7 @@
     </row>
     <row r="1861">
       <c r="A1861" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1861" t="inlineStr">
         <is>
@@ -38152,7 +38152,7 @@
     </row>
     <row r="1862">
       <c r="A1862" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1862" t="inlineStr">
         <is>
@@ -38173,7 +38173,7 @@
     </row>
     <row r="1863">
       <c r="A1863" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1863" t="inlineStr">
         <is>
@@ -38194,7 +38194,7 @@
     </row>
     <row r="1864">
       <c r="A1864" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1864" t="inlineStr">
         <is>
@@ -38215,7 +38215,7 @@
     </row>
     <row r="1865">
       <c r="A1865" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1865" t="inlineStr">
         <is>
@@ -38236,7 +38236,7 @@
     </row>
     <row r="1866">
       <c r="A1866" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1866" t="inlineStr">
         <is>
@@ -38257,7 +38257,7 @@
     </row>
     <row r="1867">
       <c r="A1867" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1867" t="inlineStr">
         <is>
@@ -38278,7 +38278,7 @@
     </row>
     <row r="1868">
       <c r="A1868" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1868" t="inlineStr">
         <is>
@@ -38299,7 +38299,7 @@
     </row>
     <row r="1869">
       <c r="A1869" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1869" t="inlineStr">
         <is>
@@ -38320,7 +38320,7 @@
     </row>
     <row r="1870">
       <c r="A1870" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1870" t="inlineStr">
         <is>
@@ -38341,7 +38341,7 @@
     </row>
     <row r="1871">
       <c r="A1871" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1871" t="inlineStr">
         <is>
@@ -38362,7 +38362,7 @@
     </row>
     <row r="1872">
       <c r="A1872" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1872" t="inlineStr">
         <is>
@@ -38383,7 +38383,7 @@
     </row>
     <row r="1873">
       <c r="A1873" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1873" t="inlineStr">
         <is>
@@ -38404,7 +38404,7 @@
     </row>
     <row r="1874">
       <c r="A1874" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1874" t="inlineStr">
         <is>
@@ -38425,7 +38425,7 @@
     </row>
     <row r="1875">
       <c r="A1875" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1875" t="inlineStr">
         <is>
@@ -38446,7 +38446,7 @@
     </row>
     <row r="1876">
       <c r="A1876" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1876" t="inlineStr">
         <is>
@@ -38467,7 +38467,7 @@
     </row>
     <row r="1877">
       <c r="A1877" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1877" t="inlineStr">
         <is>
@@ -38488,7 +38488,7 @@
     </row>
     <row r="1878">
       <c r="A1878" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1878" t="inlineStr">
         <is>
@@ -38509,7 +38509,7 @@
     </row>
     <row r="1879">
       <c r="A1879" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1879" t="inlineStr">
         <is>
@@ -38530,7 +38530,7 @@
     </row>
     <row r="1880">
       <c r="A1880" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1880" t="inlineStr">
         <is>
@@ -38551,7 +38551,7 @@
     </row>
     <row r="1881">
       <c r="A1881" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1881" t="inlineStr">
         <is>
@@ -38572,7 +38572,7 @@
     </row>
     <row r="1882">
       <c r="A1882" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1882" t="inlineStr">
         <is>
@@ -38593,7 +38593,7 @@
     </row>
     <row r="1883">
       <c r="A1883" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1883" t="inlineStr">
         <is>
@@ -38614,7 +38614,7 @@
     </row>
     <row r="1884">
       <c r="A1884" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1884" t="inlineStr">
         <is>
@@ -38633,7 +38633,7 @@
     </row>
     <row r="1885">
       <c r="A1885" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1885" t="inlineStr">
         <is>
@@ -38654,7 +38654,7 @@
     </row>
     <row r="1886">
       <c r="A1886" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1886" t="inlineStr">
         <is>
@@ -38673,7 +38673,7 @@
     </row>
     <row r="1887">
       <c r="A1887" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1887" t="inlineStr">
         <is>
@@ -38694,7 +38694,7 @@
     </row>
     <row r="1888">
       <c r="A1888" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1888" t="inlineStr">
         <is>
@@ -38715,7 +38715,7 @@
     </row>
     <row r="1889">
       <c r="A1889" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1889" t="inlineStr">
         <is>
@@ -38736,7 +38736,7 @@
     </row>
     <row r="1890">
       <c r="A1890" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1890" t="inlineStr">
         <is>
@@ -38757,7 +38757,7 @@
     </row>
     <row r="1891">
       <c r="A1891" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1891" t="inlineStr">
         <is>
@@ -38778,7 +38778,7 @@
     </row>
     <row r="1892">
       <c r="A1892" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1892" t="inlineStr">
         <is>
@@ -38799,7 +38799,7 @@
     </row>
     <row r="1893">
       <c r="A1893" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1893" t="inlineStr">
         <is>
@@ -38820,7 +38820,7 @@
     </row>
     <row r="1894">
       <c r="A1894" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1894" t="inlineStr">
         <is>
@@ -38841,7 +38841,7 @@
     </row>
     <row r="1895">
       <c r="A1895" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1895" t="inlineStr">
         <is>
@@ -38862,7 +38862,7 @@
     </row>
     <row r="1896">
       <c r="A1896" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1896" t="inlineStr">
         <is>
@@ -38883,7 +38883,7 @@
     </row>
     <row r="1897">
       <c r="A1897" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1897" t="inlineStr">
         <is>
@@ -38904,7 +38904,7 @@
     </row>
     <row r="1898">
       <c r="A1898" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1898" t="inlineStr">
         <is>
@@ -38925,7 +38925,7 @@
     </row>
     <row r="1899">
       <c r="A1899" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1899" t="inlineStr">
         <is>
@@ -38946,7 +38946,7 @@
     </row>
     <row r="1900">
       <c r="A1900" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1900" t="inlineStr">
         <is>
@@ -38967,7 +38967,7 @@
     </row>
     <row r="1901">
       <c r="A1901" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1901" t="inlineStr">
         <is>
@@ -38988,7 +38988,7 @@
     </row>
     <row r="1902">
       <c r="A1902" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1902" t="inlineStr">
         <is>
@@ -39009,7 +39009,7 @@
     </row>
     <row r="1903">
       <c r="A1903" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1903" t="inlineStr">
         <is>
@@ -39030,7 +39030,7 @@
     </row>
     <row r="1904">
       <c r="A1904" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1904" t="inlineStr">
         <is>
@@ -39051,7 +39051,7 @@
     </row>
     <row r="1905">
       <c r="A1905" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1905" t="inlineStr">
         <is>
@@ -39072,7 +39072,7 @@
     </row>
     <row r="1906">
       <c r="A1906" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1906" t="inlineStr">
         <is>
@@ -39093,7 +39093,7 @@
     </row>
     <row r="1907">
       <c r="A1907" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1907" t="inlineStr">
         <is>
@@ -39114,7 +39114,7 @@
     </row>
     <row r="1908">
       <c r="A1908" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1908" t="inlineStr">
         <is>
@@ -39135,7 +39135,7 @@
     </row>
     <row r="1909">
       <c r="A1909" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1909" t="inlineStr">
         <is>
@@ -39156,7 +39156,7 @@
     </row>
     <row r="1910">
       <c r="A1910" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1910" t="inlineStr">
         <is>
@@ -39175,7 +39175,7 @@
     </row>
     <row r="1911">
       <c r="A1911" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1911" t="inlineStr">
         <is>
@@ -39196,7 +39196,7 @@
     </row>
     <row r="1912">
       <c r="A1912" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1912" t="inlineStr">
         <is>
@@ -39217,7 +39217,7 @@
     </row>
     <row r="1913">
       <c r="A1913" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1913" t="inlineStr">
         <is>
@@ -39238,7 +39238,7 @@
     </row>
     <row r="1914">
       <c r="A1914" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1914" t="inlineStr">
         <is>
@@ -39257,7 +39257,7 @@
     </row>
     <row r="1915">
       <c r="A1915" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1915" t="inlineStr">
         <is>
@@ -39276,7 +39276,7 @@
     </row>
     <row r="1916">
       <c r="A1916" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1916" t="inlineStr">
         <is>
@@ -39295,7 +39295,7 @@
     </row>
     <row r="1917">
       <c r="A1917" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1917" t="inlineStr">
         <is>
@@ -39314,7 +39314,7 @@
     </row>
     <row r="1918">
       <c r="A1918" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1918" t="inlineStr">
         <is>
@@ -39333,7 +39333,7 @@
     </row>
     <row r="1919">
       <c r="A1919" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1919" t="inlineStr">
         <is>
@@ -39352,7 +39352,7 @@
     </row>
     <row r="1920">
       <c r="A1920" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1920" t="inlineStr">
         <is>
@@ -39371,7 +39371,7 @@
     </row>
     <row r="1921">
       <c r="A1921" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1921" t="inlineStr">
         <is>
@@ -39390,7 +39390,7 @@
     </row>
     <row r="1922">
       <c r="A1922" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1922" t="inlineStr">
         <is>
@@ -39409,7 +39409,7 @@
     </row>
     <row r="1923">
       <c r="A1923" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1923" t="inlineStr">
         <is>
@@ -39428,7 +39428,7 @@
     </row>
     <row r="1924">
       <c r="A1924" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1924" t="inlineStr">
         <is>
@@ -39447,7 +39447,7 @@
     </row>
     <row r="1925">
       <c r="A1925" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1925" t="inlineStr">
         <is>
@@ -39466,7 +39466,7 @@
     </row>
     <row r="1926">
       <c r="A1926" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1926" t="inlineStr">
         <is>
@@ -39485,7 +39485,7 @@
     </row>
     <row r="1927">
       <c r="A1927" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1927" t="inlineStr">
         <is>
@@ -39504,7 +39504,7 @@
     </row>
     <row r="1928">
       <c r="A1928" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1928" t="inlineStr">
         <is>
@@ -39523,7 +39523,7 @@
     </row>
     <row r="1929">
       <c r="A1929" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1929" t="inlineStr">
         <is>
@@ -39542,7 +39542,7 @@
     </row>
     <row r="1930">
       <c r="A1930" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1930" t="inlineStr">
         <is>
@@ -39561,7 +39561,7 @@
     </row>
     <row r="1931">
       <c r="A1931" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1931" t="inlineStr">
         <is>
@@ -39580,7 +39580,7 @@
     </row>
     <row r="1932">
       <c r="A1932" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1932" t="inlineStr">
         <is>
@@ -39599,7 +39599,7 @@
     </row>
     <row r="1933">
       <c r="A1933" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1933" t="inlineStr">
         <is>
@@ -39618,7 +39618,7 @@
     </row>
     <row r="1934">
       <c r="A1934" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1934" t="inlineStr">
         <is>
@@ -39637,7 +39637,7 @@
     </row>
     <row r="1935">
       <c r="A1935" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1935" t="inlineStr">
         <is>
@@ -39656,7 +39656,7 @@
     </row>
     <row r="1936">
       <c r="A1936" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1936" t="inlineStr">
         <is>
@@ -39675,7 +39675,7 @@
     </row>
     <row r="1937">
       <c r="A1937" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1937" t="inlineStr">
         <is>
@@ -39694,7 +39694,7 @@
     </row>
     <row r="1938">
       <c r="A1938" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1938" t="inlineStr">
         <is>
@@ -39713,7 +39713,7 @@
     </row>
     <row r="1939">
       <c r="A1939" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1939" t="inlineStr">
         <is>
@@ -39732,7 +39732,7 @@
     </row>
     <row r="1940">
       <c r="A1940" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1940" t="inlineStr">
         <is>
@@ -39751,7 +39751,7 @@
     </row>
     <row r="1941">
       <c r="A1941" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1941" t="inlineStr">
         <is>
@@ -39770,7 +39770,7 @@
     </row>
     <row r="1942">
       <c r="A1942" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1942" t="inlineStr">
         <is>
@@ -39789,7 +39789,7 @@
     </row>
     <row r="1943">
       <c r="A1943" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1943" t="inlineStr">
         <is>
@@ -39808,7 +39808,7 @@
     </row>
     <row r="1944">
       <c r="A1944" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1944" t="inlineStr">
         <is>
@@ -39827,7 +39827,7 @@
     </row>
     <row r="1945">
       <c r="A1945" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1945" t="inlineStr">
         <is>
@@ -39846,7 +39846,7 @@
     </row>
     <row r="1946">
       <c r="A1946" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1946" t="inlineStr">
         <is>
@@ -39865,7 +39865,7 @@
     </row>
     <row r="1947">
       <c r="A1947" s="2" t="n">
-        <v>45705.0167971608</v>
+        <v>45705.01679716435</v>
       </c>
       <c r="B1947" t="inlineStr">
         <is>
@@ -39877,6 +39877,2849 @@
       </c>
       <c r="D1947" t="inlineStr"/>
       <c r="E1947" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-kilogram-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1948">
+      <c r="A1948" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1948" t="inlineStr">
+        <is>
+          <t>1 грам абонаментно златно кюлче Tavex</t>
+        </is>
+      </c>
+      <c r="C1948" t="n">
+        <v>182</v>
+      </c>
+      <c r="D1948" t="n">
+        <v>202</v>
+      </c>
+      <c r="E1948" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-abonamentno-zlatno-kulche-tavex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1949">
+      <c r="A1949" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1949" t="inlineStr">
+        <is>
+          <t>0,25 грама златно кюлче Tavex</t>
+        </is>
+      </c>
+      <c r="C1949" t="n">
+        <v>49</v>
+      </c>
+      <c r="D1949" t="n">
+        <v>53</v>
+      </c>
+      <c r="E1949" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/0-25-gr-zlatno-kyulche-tavex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1950">
+      <c r="A1950" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1950" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Британия</t>
+        </is>
+      </c>
+      <c r="C1950" t="n">
+        <v>5637</v>
+      </c>
+      <c r="D1950" t="n">
+        <v>5694</v>
+      </c>
+      <c r="E1950" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-britaniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1951">
+      <c r="A1951" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1951" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Виенска Филхармония</t>
+        </is>
+      </c>
+      <c r="C1951" t="n">
+        <v>5637</v>
+      </c>
+      <c r="D1951" t="n">
+        <v>5721</v>
+      </c>
+      <c r="E1951" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-vienska-filharmoniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1952">
+      <c r="A1952" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1952" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Британия</t>
+        </is>
+      </c>
+      <c r="C1952" t="n">
+        <v>583</v>
+      </c>
+      <c r="D1952" t="n">
+        <v>628</v>
+      </c>
+      <c r="E1952" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlatna-moneta-britaniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1953">
+      <c r="A1953" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1953" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Виенска Филхармония</t>
+        </is>
+      </c>
+      <c r="C1953" t="n">
+        <v>583</v>
+      </c>
+      <c r="D1953" t="n">
+        <v>639</v>
+      </c>
+      <c r="E1953" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-%d1%83%d0%bd%d1%86%d0%b8%d1%8f-%d0%b7%d0%bb%d0%b0%d1%82%d0%bd%d0%b0-%d0%b0%d0%b2%d1%81%d1%82%d1%80%d0%b8%d0%b9%d1%81%d0%ba%d0%b0-%d1%84%d0%b8%d0%bb%d1%85%d0%b0%d1%80%d0%bc%d0%be%d0%bd%d0%b8%d1%8f/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1954">
+      <c r="A1954" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1954" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Канадски кленов лист</t>
+        </is>
+      </c>
+      <c r="C1954" t="n">
+        <v>5637</v>
+      </c>
+      <c r="D1954" t="n">
+        <v>5716</v>
+      </c>
+      <c r="E1954" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-kanadski-klenov-list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1955">
+      <c r="A1955" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1955" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийско кенгуру</t>
+        </is>
+      </c>
+      <c r="C1955" t="n">
+        <v>5637</v>
+      </c>
+      <c r="D1955" t="n">
+        <v>5694</v>
+      </c>
+      <c r="E1955" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliysko-kenguru/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1956">
+      <c r="A1956" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1956" t="inlineStr">
+        <is>
+          <t>100 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1956" t="n">
+        <v>17753</v>
+      </c>
+      <c r="D1956" t="n">
+        <v>18041</v>
+      </c>
+      <c r="E1956" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/100-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1957">
+      <c r="A1957" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1957" t="inlineStr">
+        <is>
+          <t>100 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1957" t="n">
+        <v>17753</v>
+      </c>
+      <c r="D1957" t="n">
+        <v>18058</v>
+      </c>
+      <c r="E1957" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/100-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1958">
+      <c r="A1958" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1958" t="inlineStr">
+        <is>
+          <t>0,25 г златно кюлче Tavex, подаръчен пакет</t>
+        </is>
+      </c>
+      <c r="C1958" t="n">
+        <v>49</v>
+      </c>
+      <c r="D1958" t="n">
+        <v>72</v>
+      </c>
+      <c r="E1958" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/0-25-gr-zlatno-kyulche-tavex-podarachen-paket/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1959">
+      <c r="A1959" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1959" t="inlineStr">
+        <is>
+          <t>50 x 1 грам комбинирано кюлче Valcambi Suisse CombiBar</t>
+        </is>
+      </c>
+      <c r="C1959" t="n">
+        <v>9027</v>
+      </c>
+      <c r="D1959" t="n">
+        <v>9345</v>
+      </c>
+      <c r="E1959" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-kombinirano-zlatno-kulche-valcambi-combibar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1960">
+      <c r="A1960" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1960" t="inlineStr">
+        <is>
+          <t>50 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1960" t="n">
+        <v>9027</v>
+      </c>
+      <c r="D1960" t="n">
+        <v>9109</v>
+      </c>
+      <c r="E1960" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1961">
+      <c r="A1961" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1961" t="inlineStr">
+        <is>
+          <t>50 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1961" t="n">
+        <v>9027</v>
+      </c>
+      <c r="D1961" t="n">
+        <v>9118</v>
+      </c>
+      <c r="E1961" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1962">
+      <c r="A1962" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1962" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1962" t="n">
+        <v>5621</v>
+      </c>
+      <c r="D1962" t="n">
+        <v>5672</v>
+      </c>
+      <c r="E1962" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1963">
+      <c r="A1963" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1963" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче PAMP Suisse</t>
+        </is>
+      </c>
+      <c r="C1963" t="n">
+        <v>5621</v>
+      </c>
+      <c r="D1963" t="n">
+        <v>5674</v>
+      </c>
+      <c r="E1963" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatno-kulche-pamp-suisse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1964">
+      <c r="A1964" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1964" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1964" t="n">
+        <v>5621</v>
+      </c>
+      <c r="D1964" t="n">
+        <v>5677</v>
+      </c>
+      <c r="E1964" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1965">
+      <c r="A1965" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1965" t="inlineStr">
+        <is>
+          <t>20 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1965" t="n">
+        <v>3661</v>
+      </c>
+      <c r="D1965" t="n">
+        <v>3711</v>
+      </c>
+      <c r="E1965" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1966">
+      <c r="A1966" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1966" t="inlineStr">
+        <is>
+          <t>20 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C1966" t="n">
+        <v>3661</v>
+      </c>
+      <c r="D1966" t="inlineStr"/>
+      <c r="E1966" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1967">
+      <c r="A1967" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1967" t="inlineStr">
+        <is>
+          <t>20 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1967" t="n">
+        <v>3661</v>
+      </c>
+      <c r="D1967" t="n">
+        <v>3718</v>
+      </c>
+      <c r="E1967" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1968">
+      <c r="A1968" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1968" t="inlineStr">
+        <is>
+          <t>10 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1968" t="n">
+        <v>1831</v>
+      </c>
+      <c r="D1968" t="n">
+        <v>1891</v>
+      </c>
+      <c r="E1968" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1969">
+      <c r="A1969" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1969" t="inlineStr">
+        <is>
+          <t>10 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C1969" t="n">
+        <v>1831</v>
+      </c>
+      <c r="D1969" t="n">
+        <v>1909</v>
+      </c>
+      <c r="E1969" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1970">
+      <c r="A1970" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1970" t="inlineStr">
+        <is>
+          <t>10 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1970" t="n">
+        <v>1831</v>
+      </c>
+      <c r="D1970" t="n">
+        <v>1893</v>
+      </c>
+      <c r="E1970" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1971">
+      <c r="A1971" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1971" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1971" t="n">
+        <v>924</v>
+      </c>
+      <c r="D1971" t="n">
+        <v>999</v>
+      </c>
+      <c r="E1971" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1972">
+      <c r="A1972" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1972" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C1972" t="n">
+        <v>924</v>
+      </c>
+      <c r="D1972" t="n">
+        <v>1014</v>
+      </c>
+      <c r="E1972" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1973">
+      <c r="A1973" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1973" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1973" t="n">
+        <v>924</v>
+      </c>
+      <c r="D1973" t="n">
+        <v>1001</v>
+      </c>
+      <c r="E1973" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1974">
+      <c r="A1974" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1974" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C1974" t="n">
+        <v>959</v>
+      </c>
+      <c r="D1974" t="n">
+        <v>1049</v>
+      </c>
+      <c r="E1974" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-pamp-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1975">
+      <c r="A1975" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1975" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Argor-Heraeus лунар Змия 2025</t>
+        </is>
+      </c>
+      <c r="C1975" t="n">
+        <v>933</v>
+      </c>
+      <c r="D1975" t="n">
+        <v>1036</v>
+      </c>
+      <c r="E1975" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-argor-heraeus-lunar-zmiya-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1976">
+      <c r="A1976" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1976" t="inlineStr">
+        <is>
+          <t>2,5 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1976" t="n">
+        <v>475</v>
+      </c>
+      <c r="D1976" t="n">
+        <v>531</v>
+      </c>
+      <c r="E1976" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/2-5-grama-zlatno-kyulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1977">
+      <c r="A1977" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1977" t="inlineStr">
+        <is>
+          <t>2,5 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C1977" t="n">
+        <v>475</v>
+      </c>
+      <c r="D1977" t="n">
+        <v>535</v>
+      </c>
+      <c r="E1977" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/dva-grama-i-polovina-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1978">
+      <c r="A1978" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1978" t="inlineStr">
+        <is>
+          <t>2 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1978" t="n">
+        <v>380</v>
+      </c>
+      <c r="D1978" t="n">
+        <v>425</v>
+      </c>
+      <c r="E1978" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/2-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1979">
+      <c r="A1979" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1979" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C1979" t="n">
+        <v>186</v>
+      </c>
+      <c r="D1979" t="n">
+        <v>224</v>
+      </c>
+      <c r="E1979" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1980">
+      <c r="A1980" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1980" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C1980" t="n">
+        <v>186</v>
+      </c>
+      <c r="D1980" t="n">
+        <v>225</v>
+      </c>
+      <c r="E1980" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1981">
+      <c r="A1981" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1981" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C1981" t="n">
+        <v>186</v>
+      </c>
+      <c r="D1981" t="n">
+        <v>222</v>
+      </c>
+      <c r="E1981" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1982">
+      <c r="A1982" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1982" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Argor-Heraeus лунар Змия 2025</t>
+        </is>
+      </c>
+      <c r="C1982" t="n">
+        <v>213</v>
+      </c>
+      <c r="D1982" t="n">
+        <v>269</v>
+      </c>
+      <c r="E1982" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kyulche-argor-heraeus-lunar-zmiya-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1983">
+      <c r="A1983" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1983" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Американски орел</t>
+        </is>
+      </c>
+      <c r="C1983" t="n">
+        <v>5637</v>
+      </c>
+      <c r="D1983" t="n">
+        <v>5865</v>
+      </c>
+      <c r="E1983" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-uncia-amerikanski-orel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1984">
+      <c r="A1984" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1984" t="inlineStr">
+        <is>
+          <t>20 долара двоен орел лейди Либърти</t>
+        </is>
+      </c>
+      <c r="C1984" t="n">
+        <v>5294</v>
+      </c>
+      <c r="D1984" t="n">
+        <v>6234</v>
+      </c>
+      <c r="E1984" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-dolara-dvoen-orel-lejdi-libarti/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1985">
+      <c r="A1985" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1985" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Американски бизон</t>
+        </is>
+      </c>
+      <c r="C1985" t="n">
+        <v>5721</v>
+      </c>
+      <c r="D1985" t="n">
+        <v>5975</v>
+      </c>
+      <c r="E1985" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-amerikanski-bizon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1986">
+      <c r="A1986" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1986" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Кругерранд, Южна Африка</t>
+        </is>
+      </c>
+      <c r="C1986" t="n">
+        <v>5560</v>
+      </c>
+      <c r="D1986" t="n">
+        <v>5672</v>
+      </c>
+      <c r="E1986" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-krugerrand-yujna-afrika/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1987">
+      <c r="A1987" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1987" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Слон Южна Африка - Големите 5</t>
+        </is>
+      </c>
+      <c r="C1987" t="n">
+        <v>5637</v>
+      </c>
+      <c r="D1987" t="n">
+        <v>5754</v>
+      </c>
+      <c r="E1987" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-slon-yuzhna-afrika-golemite-5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1988">
+      <c r="A1988" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1988" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C1988" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D1988" t="n">
+        <v>6388</v>
+      </c>
+      <c r="E1988" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1989">
+      <c r="A1989" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1989" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C1989" t="n">
+        <v>5803</v>
+      </c>
+      <c r="D1989" t="n">
+        <v>6090</v>
+      </c>
+      <c r="E1989" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1990">
+      <c r="A1990" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1990" t="inlineStr">
+        <is>
+          <t>1/4 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C1990" t="n">
+        <v>1451</v>
+      </c>
+      <c r="D1990" t="n">
+        <v>1652</v>
+      </c>
+      <c r="E1990" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-4-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1991">
+      <c r="A1991" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1991" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C1991" t="n">
+        <v>581</v>
+      </c>
+      <c r="D1991" t="n">
+        <v>716</v>
+      </c>
+      <c r="E1991" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1992">
+      <c r="A1992" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1992" t="inlineStr">
+        <is>
+          <t>1/20 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C1992" t="n">
+        <v>277</v>
+      </c>
+      <c r="D1992" t="n">
+        <v>405</v>
+      </c>
+      <c r="E1992" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-20-unciya-zlaten-avstraliiski-lunar-godina-na-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1993">
+      <c r="A1993" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1993" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C1993" t="n">
+        <v>5748</v>
+      </c>
+      <c r="D1993" t="n">
+        <v>5865</v>
+      </c>
+      <c r="E1993" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1994">
+      <c r="A1994" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1994" t="inlineStr">
+        <is>
+          <t>1/2 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C1994" t="n">
+        <v>2819</v>
+      </c>
+      <c r="D1994" t="n">
+        <v>3139</v>
+      </c>
+      <c r="E1994" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-2-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1995">
+      <c r="A1995" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1995" t="inlineStr">
+        <is>
+          <t>1/4 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C1995" t="n">
+        <v>1451</v>
+      </c>
+      <c r="D1995" t="n">
+        <v>1624</v>
+      </c>
+      <c r="E1995" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-4-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1996">
+      <c r="A1996" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1996" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C1996" t="n">
+        <v>581</v>
+      </c>
+      <c r="D1996" t="n">
+        <v>705</v>
+      </c>
+      <c r="E1996" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1997">
+      <c r="A1997" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1997" t="inlineStr">
+        <is>
+          <t>1/20 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C1997" t="n">
+        <v>277</v>
+      </c>
+      <c r="D1997" t="n">
+        <v>405</v>
+      </c>
+      <c r="E1997" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-20-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1998">
+      <c r="A1998" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1998" t="inlineStr">
+        <is>
+          <t>Руска златна монета 5 рубли Николай II</t>
+        </is>
+      </c>
+      <c r="C1998" t="n">
+        <v>756</v>
+      </c>
+      <c r="D1998" t="n">
+        <v>993</v>
+      </c>
+      <c r="E1998" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-5-rubli-nikolay-iii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1999">
+      <c r="A1999" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B1999" t="inlineStr">
+        <is>
+          <t>10 рубли Николай II Русия</t>
+        </is>
+      </c>
+      <c r="C1999" t="n">
+        <v>1514</v>
+      </c>
+      <c r="D1999" t="n">
+        <v>2056</v>
+      </c>
+      <c r="E1999" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-rubli-nikolai-ii-rusia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2000">
+      <c r="A2000" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2000" t="inlineStr">
+        <is>
+          <t>20 френски франка Наполеон III</t>
+        </is>
+      </c>
+      <c r="C2000" t="n">
+        <v>1053</v>
+      </c>
+      <c r="D2000" t="n">
+        <v>1083</v>
+      </c>
+      <c r="E2000" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-frenski-franka-napoleon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2001">
+      <c r="A2001" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2001" t="inlineStr">
+        <is>
+          <t>20 френски франка златна монета Наполеон III с лавров венец</t>
+        </is>
+      </c>
+      <c r="C2001" t="n">
+        <v>1053</v>
+      </c>
+      <c r="D2001" t="n">
+        <v>1083</v>
+      </c>
+      <c r="E2001" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-%d1%84%d1%80%d0%b0%d0%bd%d0%ba%d0%b0-%d1%84%d1%80%d0%b5%d0%bd%d1%81%d0%ba%d0%b8-%d0%bd%d0%b0%d0%bf%d0%be%d0%bb%d0%b5%d0%be%d0%bd-%d1%81-%d0%bb%d0%b0%d0%b2%d1%80%d0%be%d0%b2-%d0%b2%d0%b5%d0%bd%d0%b5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2002">
+      <c r="A2002" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2002" t="inlineStr">
+        <is>
+          <t>10 франка френски Наполеон III</t>
+        </is>
+      </c>
+      <c r="C2002" t="n">
+        <v>573</v>
+      </c>
+      <c r="D2002" t="n">
+        <v>655</v>
+      </c>
+      <c r="E2002" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-frenski-franka-napoleon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2003">
+      <c r="A2003" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2003" t="inlineStr">
+        <is>
+          <t>10 френски франка златна монета Наполеон III с лавров венец</t>
+        </is>
+      </c>
+      <c r="C2003" t="n">
+        <v>573</v>
+      </c>
+      <c r="D2003" t="n">
+        <v>655</v>
+      </c>
+      <c r="E2003" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-frenski-franka-zlatna-moneta-napoleon-iii-s-lavrov-venets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2004">
+      <c r="A2004" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2004" t="inlineStr">
+        <is>
+          <t>Златна монета 20 френски франка Серес</t>
+        </is>
+      </c>
+      <c r="C2004" t="n">
+        <v>1053</v>
+      </c>
+      <c r="D2004" t="n">
+        <v>1083</v>
+      </c>
+      <c r="E2004" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-frenski-franka-seres/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2005">
+      <c r="A2005" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2005" t="inlineStr">
+        <is>
+          <t>20 френски франка златна монета Гениус</t>
+        </is>
+      </c>
+      <c r="C2005" t="n">
+        <v>1053</v>
+      </c>
+      <c r="D2005" t="n">
+        <v>1083</v>
+      </c>
+      <c r="E2005" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-zlatni-frenski-franka-genius/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2006">
+      <c r="A2006" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2006" t="inlineStr">
+        <is>
+          <t>Златна монета 20 франка Мариана</t>
+        </is>
+      </c>
+      <c r="C2006" t="n">
+        <v>1053</v>
+      </c>
+      <c r="D2006" t="n">
+        <v>1083</v>
+      </c>
+      <c r="E2006" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-frenski-franka-mariana/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2007">
+      <c r="A2007" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2007" t="inlineStr">
+        <is>
+          <t>20 белгийски франка златна монета Леополд II</t>
+        </is>
+      </c>
+      <c r="C2007" t="n">
+        <v>1055</v>
+      </c>
+      <c r="D2007" t="n">
+        <v>1085</v>
+      </c>
+      <c r="E2007" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-belgiiski-franka-leopold-ii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2008">
+      <c r="A2008" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2008" t="inlineStr">
+        <is>
+          <t>20 лири Виктор Емануил II Италия</t>
+        </is>
+      </c>
+      <c r="C2008" t="n">
+        <v>1055</v>
+      </c>
+      <c r="D2008" t="n">
+        <v>1100</v>
+      </c>
+      <c r="E2008" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/italian-20lira-emanuele/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2009">
+      <c r="A2009" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2009" t="inlineStr">
+        <is>
+          <t>20 лири златна монета Умберто I, Италия</t>
+        </is>
+      </c>
+      <c r="C2009" t="n">
+        <v>1055</v>
+      </c>
+      <c r="D2009" t="n">
+        <v>1085</v>
+      </c>
+      <c r="E2009" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-liri-zlatna-moneta-umberto-i-italiya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2010">
+      <c r="A2010" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2010" t="inlineStr">
+        <is>
+          <t>4 австрийски дуката златна монета Франц Йосиф</t>
+        </is>
+      </c>
+      <c r="C2010" t="n">
+        <v>2447</v>
+      </c>
+      <c r="D2010" t="n">
+        <v>2646</v>
+      </c>
+      <c r="E2010" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-4-avstriiski-dukata-franc-iosif/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2011">
+      <c r="A2011" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2011" t="inlineStr">
+        <is>
+          <t>1 австрийски дукат златна монета Франц Йосиф</t>
+        </is>
+      </c>
+      <c r="C2011" t="n">
+        <v>630</v>
+      </c>
+      <c r="D2011" t="n">
+        <v>664</v>
+      </c>
+      <c r="E2011" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-1-avstriiski-dukat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2012">
+      <c r="A2012" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2012" t="inlineStr">
+        <is>
+          <t>8 форинта/20 франка Франц Йосиф Унгария</t>
+        </is>
+      </c>
+      <c r="C2012" t="n">
+        <v>1053</v>
+      </c>
+      <c r="D2012" t="n">
+        <v>1110</v>
+      </c>
+      <c r="E2012" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-forinta-20-franka-franc-iosif-ungariia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2013">
+      <c r="A2013" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2013" t="inlineStr">
+        <is>
+          <t>Златна монета 4 флорина/10 франка Франц Йосиф, Австрия</t>
+        </is>
+      </c>
+      <c r="C2013" t="n">
+        <v>552</v>
+      </c>
+      <c r="D2013" t="n">
+        <v>590</v>
+      </c>
+      <c r="E2013" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-4-florina-10-franka-franc-iosif-avstria/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2014">
+      <c r="A2014" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2014" t="inlineStr">
+        <is>
+          <t>20 франка златна монета Швейцария Вренели</t>
+        </is>
+      </c>
+      <c r="C2014" t="n">
+        <v>1053</v>
+      </c>
+      <c r="D2014" t="n">
+        <v>1085</v>
+      </c>
+      <c r="E2014" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-zlatni-franka-shveitsariya-vreneli/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2015">
+      <c r="A2015" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2015" t="inlineStr">
+        <is>
+          <t>10 гулдена Вилхелмина Холандия</t>
+        </is>
+      </c>
+      <c r="C2015" t="n">
+        <v>1071</v>
+      </c>
+      <c r="D2015" t="n">
+        <v>1163</v>
+      </c>
+      <c r="E2015" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-guldena-vilhemina-holandiya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2016">
+      <c r="A2016" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2016" t="inlineStr">
+        <is>
+          <t>20 германски марки Вилхелм II</t>
+        </is>
+      </c>
+      <c r="C2016" t="n">
+        <v>1286</v>
+      </c>
+      <c r="D2016" t="n">
+        <v>1383</v>
+      </c>
+      <c r="E2016" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-germanski-marki-vilhelm-ii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2017">
+      <c r="A2017" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2017" t="inlineStr">
+        <is>
+          <t>Златен Мемориален Суверен Чарлз III Великобритания 2022г.</t>
+        </is>
+      </c>
+      <c r="C2017" t="n">
+        <v>1328</v>
+      </c>
+      <c r="D2017" t="n">
+        <v>1387</v>
+      </c>
+      <c r="E2017" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-memorialen-suveren-charles-iii-2022/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2018">
+      <c r="A2018" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2018" t="inlineStr">
+        <is>
+          <t>Златен Суверен Чарлз III Великобритания</t>
+        </is>
+      </c>
+      <c r="C2018" t="n">
+        <v>1334</v>
+      </c>
+      <c r="D2018" t="n">
+        <v>1393</v>
+      </c>
+      <c r="E2018" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-charles-iii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2019">
+      <c r="A2019" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2019" t="inlineStr">
+        <is>
+          <t>Златен суверен Елизабет II 1957-2021 Великобритания</t>
+        </is>
+      </c>
+      <c r="C2019" t="n">
+        <v>1301</v>
+      </c>
+      <c r="D2019" t="n">
+        <v>1350</v>
+      </c>
+      <c r="E2019" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/suveren-elizabet-ii-velikobritaniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2020">
+      <c r="A2020" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2020" t="inlineStr">
+        <is>
+          <t>Златен суверен Едуард VII Великобритания</t>
+        </is>
+      </c>
+      <c r="C2020" t="n">
+        <v>1301</v>
+      </c>
+      <c r="D2020" t="n">
+        <v>1374</v>
+      </c>
+      <c r="E2020" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-eduard-vii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2021">
+      <c r="A2021" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2021" t="inlineStr">
+        <is>
+          <t>Златен суверен Джордж V Великобритания</t>
+        </is>
+      </c>
+      <c r="C2021" t="n">
+        <v>1301</v>
+      </c>
+      <c r="D2021" t="n">
+        <v>1374</v>
+      </c>
+      <c r="E2021" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-jorge-v/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2022">
+      <c r="A2022" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2022" t="inlineStr">
+        <is>
+          <t>Златен суверен Виктория Великобритания</t>
+        </is>
+      </c>
+      <c r="C2022" t="n">
+        <v>1301</v>
+      </c>
+      <c r="D2022" t="n">
+        <v>1387</v>
+      </c>
+      <c r="E2022" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-viktoriya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2023">
+      <c r="A2023" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2023" t="inlineStr">
+        <is>
+          <t>Британски златен суверен Елизабет II, 2022г.</t>
+        </is>
+      </c>
+      <c r="C2023" t="n">
+        <v>1301</v>
+      </c>
+      <c r="D2023" t="inlineStr"/>
+      <c r="E2023" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-britanski-suveren-elizabet-ii-2022/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2024">
+      <c r="A2024" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2024" t="inlineStr">
+        <is>
+          <t>20 франка златна монета Тунис</t>
+        </is>
+      </c>
+      <c r="C2024" t="n">
+        <v>1048</v>
+      </c>
+      <c r="D2024" t="n">
+        <v>1141</v>
+      </c>
+      <c r="E2024" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-franka-zlatna-moneta-tunis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2025">
+      <c r="A2025" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2025" t="inlineStr">
+        <is>
+          <t>Златна монета 100 турски куруша</t>
+        </is>
+      </c>
+      <c r="C2025" t="n">
+        <v>1048</v>
+      </c>
+      <c r="D2025" t="inlineStr"/>
+      <c r="E2025" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-100-turski-kurusha/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2026">
+      <c r="A2026" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2026" t="inlineStr">
+        <is>
+          <t>Златна монета 50 песос, Мексико</t>
+        </is>
+      </c>
+      <c r="C2026" t="n">
+        <v>6664</v>
+      </c>
+      <c r="D2026" t="n">
+        <v>7071</v>
+      </c>
+      <c r="E2026" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-50-pesos-meksiko/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2027">
+      <c r="A2027" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2027" t="inlineStr">
+        <is>
+          <t>Златна монета 100 австрийски корони Франц Йосиф</t>
+        </is>
+      </c>
+      <c r="C2027" t="n">
+        <v>5336</v>
+      </c>
+      <c r="D2027" t="n">
+        <v>5721</v>
+      </c>
+      <c r="E2027" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-100-avstriyski-koroni-franc-yosif/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2028">
+      <c r="A2028" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2028" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2028" t="n">
+        <v>5438</v>
+      </c>
+      <c r="D2028" t="n">
+        <v>5762</v>
+      </c>
+      <c r="E2028" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2029">
+      <c r="A2029" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2029" t="inlineStr">
+        <is>
+          <t>15 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2029" t="n">
+        <v>2719</v>
+      </c>
+      <c r="D2029" t="n">
+        <v>2974</v>
+      </c>
+      <c r="E2029" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/15-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2030">
+      <c r="A2030" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2030" t="inlineStr">
+        <is>
+          <t>8 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2030" t="n">
+        <v>1450</v>
+      </c>
+      <c r="D2030" t="n">
+        <v>1629</v>
+      </c>
+      <c r="E2030" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2031">
+      <c r="A2031" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2031" t="inlineStr">
+        <is>
+          <t>3 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2031" t="n">
+        <v>544</v>
+      </c>
+      <c r="D2031" t="n">
+        <v>691</v>
+      </c>
+      <c r="E2031" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/3-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2032">
+      <c r="A2032" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2032" t="inlineStr">
+        <is>
+          <t>1 грам златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2032" t="n">
+        <v>181</v>
+      </c>
+      <c r="D2032" t="n">
+        <v>275</v>
+      </c>
+      <c r="E2032" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2033">
+      <c r="A2033" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2033" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Тигъра 2022</t>
+        </is>
+      </c>
+      <c r="C2033" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2033" t="n">
+        <v>8260</v>
+      </c>
+      <c r="E2033" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-oz-australian-lunar-year-of-the-tiger-2022-gold-coin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2034">
+      <c r="A2034" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2034" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Вола 2021</t>
+        </is>
+      </c>
+      <c r="C2034" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2034" t="n">
+        <v>6608</v>
+      </c>
+      <c r="E2034" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-oz-australian-lunar-year-of-the-ox-2021-gold-coin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2035">
+      <c r="A2035" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2035" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийски лунар година на Мишката 2020</t>
+        </is>
+      </c>
+      <c r="C2035" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2035" t="n">
+        <v>6498</v>
+      </c>
+      <c r="E2035" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyski-lunar-godina-mishkata-2020/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2036">
+      <c r="A2036" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2036" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Кучето 2018</t>
+        </is>
+      </c>
+      <c r="C2036" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2036" t="n">
+        <v>6498</v>
+      </c>
+      <c r="E2036" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni38s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-22/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2037">
+      <c r="A2037" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2037" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Петела 2017</t>
+        </is>
+      </c>
+      <c r="C2037" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2037" t="n">
+        <v>6498</v>
+      </c>
+      <c r="E2037" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni40s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-24/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2038">
+      <c r="A2038" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2038" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Маймуната 2016</t>
+        </is>
+      </c>
+      <c r="C2038" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2038" t="n">
+        <v>6498</v>
+      </c>
+      <c r="E2038" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-maimunata-2016/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2039">
+      <c r="A2039" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2039" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Змията 2013</t>
+        </is>
+      </c>
+      <c r="C2039" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2039" t="n">
+        <v>6608</v>
+      </c>
+      <c r="E2039" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlaten-avstraliiski-lunar-godina-na-zmiyata-2013/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2040">
+      <c r="A2040" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2040" t="inlineStr">
+        <is>
+          <t>1 унция австралиисйки лунар година на дракона 2012</t>
+        </is>
+      </c>
+      <c r="C2040" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2040" t="n">
+        <v>6498</v>
+      </c>
+      <c r="E2040" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-drakona-2012/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2041">
+      <c r="A2041" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2041" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Заека 2011</t>
+        </is>
+      </c>
+      <c r="C2041" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2041" t="n">
+        <v>6498</v>
+      </c>
+      <c r="E2041" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-moneta-avstraliiski-lunar-zaek-2011/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2042">
+      <c r="A2042" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2042" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Вола 2009</t>
+        </is>
+      </c>
+      <c r="C2042" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2042" t="n">
+        <v>6498</v>
+      </c>
+      <c r="E2042" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-avstraliiski-lunar-godina-na-vola-2009/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2043">
+      <c r="A2043" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2043" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Мишката 2008</t>
+        </is>
+      </c>
+      <c r="C2043" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2043" t="n">
+        <v>6498</v>
+      </c>
+      <c r="E2043" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-uncia-moneta-lunar-mishka-2008/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2044">
+      <c r="A2044" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2044" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Прасето 2007</t>
+        </is>
+      </c>
+      <c r="C2044" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2044" t="n">
+        <v>6498</v>
+      </c>
+      <c r="E2044" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-avstraliiski-lunar-godina-na-praseto-2007/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2045">
+      <c r="A2045" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2045" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Петела 2005</t>
+        </is>
+      </c>
+      <c r="C2045" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2045" t="n">
+        <v>6498</v>
+      </c>
+      <c r="E2045" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-petela-2005/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2046">
+      <c r="A2046" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2046" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Маймуната 2004</t>
+        </is>
+      </c>
+      <c r="C2046" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2046" t="n">
+        <v>6498</v>
+      </c>
+      <c r="E2046" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-%d1%83%d0%bd%d1%86%d0%b8%d1%8f-%d0%b7%d0%bb%d0%b0%d1%82%d0%b5%d0%bd-%d0%b0%d0%b2%d1%81%d1%82%d1%80%d0%b0%d0%bb%d0%b8%d0%b9%d1%81%d0%ba%d0%b8-%d0%bb%d1%83%d0%bd%d0%b0%d1%80-%d0%b3%d0%be%d0%b4%d0%b8-2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2047">
+      <c r="A2047" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2047" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Козата 2003</t>
+        </is>
+      </c>
+      <c r="C2047" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2047" t="n">
+        <v>6498</v>
+      </c>
+      <c r="E2047" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni38s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-24/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2048">
+      <c r="A2048" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2048" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийки Лунар 2000 година на дракона</t>
+        </is>
+      </c>
+      <c r="C2048" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2048" t="n">
+        <v>7434</v>
+      </c>
+      <c r="E2048" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyki-lunar-2000-godina-drakona/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2049">
+      <c r="A2049" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2049" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Тигъра 2010</t>
+        </is>
+      </c>
+      <c r="C2049" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2049" t="inlineStr"/>
+      <c r="E2049" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-tigura-2010/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2050">
+      <c r="A2050" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2050" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Кучето 2006</t>
+        </is>
+      </c>
+      <c r="C2050" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2050" t="n">
+        <v>6498</v>
+      </c>
+      <c r="E2050" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-kucheto-2006/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2051">
+      <c r="A2051" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2051" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Тигъра 1998</t>
+        </is>
+      </c>
+      <c r="C2051" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2051" t="n">
+        <v>6883</v>
+      </c>
+      <c r="E2051" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliiski-lunar-godinata-na-tigara-1998/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2052">
+      <c r="A2052" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2052" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Вола 1997</t>
+        </is>
+      </c>
+      <c r="C2052" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2052" t="n">
+        <v>6883</v>
+      </c>
+      <c r="E2052" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliiski-lunar-godinata-na-vola-1997/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2053">
+      <c r="A2053" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2053" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Мишката 1996</t>
+        </is>
+      </c>
+      <c r="C2053" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2053" t="inlineStr"/>
+      <c r="E2053" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni42s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2054">
+      <c r="A2054" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2054" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Коня 2014</t>
+        </is>
+      </c>
+      <c r="C2054" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2054" t="inlineStr"/>
+      <c r="E2054" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-konq-2014/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2055">
+      <c r="A2055" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2055" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Argor-Heraeus лунар Дракон 2024</t>
+        </is>
+      </c>
+      <c r="C2055" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2055" t="inlineStr"/>
+      <c r="E2055" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-argor-heraeus-lunar-drakon-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2056">
+      <c r="A2056" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2056" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Argor-Heraeus лунар Дракон 2024</t>
+        </is>
+      </c>
+      <c r="C2056" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2056" t="inlineStr"/>
+      <c r="E2056" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kyulche-argor-heraeus-lunar-drakon-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2057">
+      <c r="A2057" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2057" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2057" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2057" t="inlineStr"/>
+      <c r="E2057" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2058">
+      <c r="A2058" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2058" t="inlineStr">
+        <is>
+          <t>15 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2058" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2058" t="inlineStr"/>
+      <c r="E2058" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/15-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2059">
+      <c r="A2059" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2059" t="inlineStr">
+        <is>
+          <t>8 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2059" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2059" t="inlineStr"/>
+      <c r="E2059" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2060">
+      <c r="A2060" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2060" t="inlineStr">
+        <is>
+          <t>3 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2060" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2060" t="inlineStr"/>
+      <c r="E2060" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/3-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2061">
+      <c r="A2061" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2061" t="inlineStr">
+        <is>
+          <t>1 грам златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2061" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2061" t="inlineStr"/>
+      <c r="E2061" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2062">
+      <c r="A2062" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2062" t="inlineStr">
+        <is>
+          <t>1/2 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C2062" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2062" t="inlineStr"/>
+      <c r="E2062" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-2-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2063">
+      <c r="A2063" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2063" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Драконът на Тюдор 2024г.</t>
+        </is>
+      </c>
+      <c r="C2063" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2063" t="inlineStr"/>
+      <c r="E2063" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-pazitelite-na-tudorite-drakonat-na-tudor-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2064">
+      <c r="A2064" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2064" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Еднорогът на Сиймор 2024 г.</t>
+        </is>
+      </c>
+      <c r="C2064" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2064" t="inlineStr"/>
+      <c r="E2064" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-pazitelite-na-tyudorite-ednorogut-na-siimor-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2065">
+      <c r="A2065" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2065" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Бикът от Кларънс 2023 г.</t>
+        </is>
+      </c>
+      <c r="C2065" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2065" t="inlineStr"/>
+      <c r="E2065" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-pazitelite-na-tyudorite-bikut-ot-klaruns-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2066">
+      <c r="A2066" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2066" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Британия - Елизабет II</t>
+        </is>
+      </c>
+      <c r="C2066" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2066" t="inlineStr"/>
+      <c r="E2066" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-britaniya-elizabet-ii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2067">
+      <c r="A2067" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2067" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Йейлът на Бофорт 2023 г.</t>
+        </is>
+      </c>
+      <c r="C2067" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2067" t="inlineStr"/>
+      <c r="E2067" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-oz-zlatna-moneta-pazitelite-na-tyudorite-yeylut-na-bofort-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2068">
+      <c r="A2068" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2068" t="inlineStr">
+        <is>
+          <t>1/2 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2068" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2068" t="inlineStr"/>
+      <c r="E2068" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-2-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2069">
+      <c r="A2069" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2069" t="inlineStr">
+        <is>
+          <t>1/4 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2069" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2069" t="inlineStr"/>
+      <c r="E2069" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-4-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2070">
+      <c r="A2070" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2070" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C2070" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2070" t="inlineStr"/>
+      <c r="E2070" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-pamp-lunar-drakon-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2071">
+      <c r="A2071" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2071" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2071" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2071" t="inlineStr"/>
+      <c r="E2071" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-pamp-lunar-zaek-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2072">
+      <c r="A2072" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2072" t="inlineStr">
+        <is>
+          <t>1/10 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2072" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2072" t="inlineStr"/>
+      <c r="E2072" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2073">
+      <c r="A2073" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2073" t="inlineStr">
+        <is>
+          <t>15 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2073" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2073" t="inlineStr"/>
+      <c r="E2073" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/15-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2074">
+      <c r="A2074" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2074" t="inlineStr">
+        <is>
+          <t>1/20 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2074" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2074" t="inlineStr"/>
+      <c r="E2074" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-20-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2075">
+      <c r="A2075" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2075" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2075" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2075" t="inlineStr"/>
+      <c r="E2075" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2076">
+      <c r="A2076" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2076" t="inlineStr">
+        <is>
+          <t>8 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2076" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2076" t="inlineStr"/>
+      <c r="E2076" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2077">
+      <c r="A2077" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2077" t="inlineStr">
+        <is>
+          <t>3 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2077" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2077" t="inlineStr"/>
+      <c r="E2077" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/3-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2078">
+      <c r="A2078" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2078" t="inlineStr">
+        <is>
+          <t>1 грам златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2078" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2078" t="inlineStr"/>
+      <c r="E2078" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2079">
+      <c r="A2079" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2079" t="inlineStr">
+        <is>
+          <t>100 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2079" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2079" t="inlineStr"/>
+      <c r="E2079" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/100-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2080">
+      <c r="A2080" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2080" t="inlineStr">
+        <is>
+          <t>50 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2080" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2080" t="inlineStr"/>
+      <c r="E2080" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2081">
+      <c r="A2081" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2081" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2081" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2081" t="inlineStr"/>
+      <c r="E2081" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2082">
+      <c r="A2082" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2082" t="inlineStr">
+        <is>
+          <t>10 крони Кристиян X Дания</t>
+        </is>
+      </c>
+      <c r="C2082" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2082" t="inlineStr"/>
+      <c r="E2082" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-kroni-kristiyan-x-daniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2083">
+      <c r="A2083" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2083" t="inlineStr">
+        <is>
+          <t>10 Гулдена Вилхелм III Холандия</t>
+        </is>
+      </c>
+      <c r="C2083" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2083" t="inlineStr"/>
+      <c r="E2083" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni38s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-9/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2084">
+      <c r="A2084" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2084" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2022</t>
+        </is>
+      </c>
+      <c r="C2084" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2084" t="inlineStr"/>
+      <c r="E2084" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitayska-panda-2022/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2085">
+      <c r="A2085" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2085" t="inlineStr">
+        <is>
+          <t>Златна монета 10 франка Мариана</t>
+        </is>
+      </c>
+      <c r="C2085" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2085" t="inlineStr"/>
+      <c r="E2085" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-frenski-franka-mariana/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2086">
+      <c r="A2086" s="2" t="n">
+        <v>45706.87078163875</v>
+      </c>
+      <c r="B2086" t="inlineStr">
+        <is>
+          <t>1 килограм златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2086" t="n">
+        <v>5693</v>
+      </c>
+      <c r="D2086" t="inlineStr"/>
+      <c r="E2086" t="inlineStr">
         <is>
           <t>https://tavex.bg/zlato/1-kilogram-zlatno-kulche-valcambi/</t>
         </is>

</xml_diff>

<commit_message>
Report 19 02 2025
</commit_message>
<xml_diff>
--- a/price_history_gold.xlsx
+++ b/price_history_gold.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2086"/>
+  <dimension ref="A1:E2225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39884,7 +39884,7 @@
     </row>
     <row r="1948">
       <c r="A1948" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1948" t="inlineStr">
         <is>
@@ -39905,7 +39905,7 @@
     </row>
     <row r="1949">
       <c r="A1949" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1949" t="inlineStr">
         <is>
@@ -39926,7 +39926,7 @@
     </row>
     <row r="1950">
       <c r="A1950" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1950" t="inlineStr">
         <is>
@@ -39947,7 +39947,7 @@
     </row>
     <row r="1951">
       <c r="A1951" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1951" t="inlineStr">
         <is>
@@ -39968,7 +39968,7 @@
     </row>
     <row r="1952">
       <c r="A1952" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1952" t="inlineStr">
         <is>
@@ -39989,7 +39989,7 @@
     </row>
     <row r="1953">
       <c r="A1953" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1953" t="inlineStr">
         <is>
@@ -40010,7 +40010,7 @@
     </row>
     <row r="1954">
       <c r="A1954" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1954" t="inlineStr">
         <is>
@@ -40031,7 +40031,7 @@
     </row>
     <row r="1955">
       <c r="A1955" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1955" t="inlineStr">
         <is>
@@ -40052,7 +40052,7 @@
     </row>
     <row r="1956">
       <c r="A1956" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1956" t="inlineStr">
         <is>
@@ -40073,7 +40073,7 @@
     </row>
     <row r="1957">
       <c r="A1957" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1957" t="inlineStr">
         <is>
@@ -40094,7 +40094,7 @@
     </row>
     <row r="1958">
       <c r="A1958" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1958" t="inlineStr">
         <is>
@@ -40115,7 +40115,7 @@
     </row>
     <row r="1959">
       <c r="A1959" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1959" t="inlineStr">
         <is>
@@ -40136,7 +40136,7 @@
     </row>
     <row r="1960">
       <c r="A1960" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1960" t="inlineStr">
         <is>
@@ -40157,7 +40157,7 @@
     </row>
     <row r="1961">
       <c r="A1961" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1961" t="inlineStr">
         <is>
@@ -40178,7 +40178,7 @@
     </row>
     <row r="1962">
       <c r="A1962" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1962" t="inlineStr">
         <is>
@@ -40199,7 +40199,7 @@
     </row>
     <row r="1963">
       <c r="A1963" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1963" t="inlineStr">
         <is>
@@ -40220,7 +40220,7 @@
     </row>
     <row r="1964">
       <c r="A1964" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1964" t="inlineStr">
         <is>
@@ -40241,7 +40241,7 @@
     </row>
     <row r="1965">
       <c r="A1965" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1965" t="inlineStr">
         <is>
@@ -40262,7 +40262,7 @@
     </row>
     <row r="1966">
       <c r="A1966" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1966" t="inlineStr">
         <is>
@@ -40281,7 +40281,7 @@
     </row>
     <row r="1967">
       <c r="A1967" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1967" t="inlineStr">
         <is>
@@ -40302,7 +40302,7 @@
     </row>
     <row r="1968">
       <c r="A1968" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1968" t="inlineStr">
         <is>
@@ -40323,7 +40323,7 @@
     </row>
     <row r="1969">
       <c r="A1969" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1969" t="inlineStr">
         <is>
@@ -40344,7 +40344,7 @@
     </row>
     <row r="1970">
       <c r="A1970" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1970" t="inlineStr">
         <is>
@@ -40365,7 +40365,7 @@
     </row>
     <row r="1971">
       <c r="A1971" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1971" t="inlineStr">
         <is>
@@ -40386,7 +40386,7 @@
     </row>
     <row r="1972">
       <c r="A1972" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1972" t="inlineStr">
         <is>
@@ -40407,7 +40407,7 @@
     </row>
     <row r="1973">
       <c r="A1973" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1973" t="inlineStr">
         <is>
@@ -40428,7 +40428,7 @@
     </row>
     <row r="1974">
       <c r="A1974" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1974" t="inlineStr">
         <is>
@@ -40449,7 +40449,7 @@
     </row>
     <row r="1975">
       <c r="A1975" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1975" t="inlineStr">
         <is>
@@ -40470,7 +40470,7 @@
     </row>
     <row r="1976">
       <c r="A1976" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1976" t="inlineStr">
         <is>
@@ -40491,7 +40491,7 @@
     </row>
     <row r="1977">
       <c r="A1977" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1977" t="inlineStr">
         <is>
@@ -40512,7 +40512,7 @@
     </row>
     <row r="1978">
       <c r="A1978" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1978" t="inlineStr">
         <is>
@@ -40533,7 +40533,7 @@
     </row>
     <row r="1979">
       <c r="A1979" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1979" t="inlineStr">
         <is>
@@ -40554,7 +40554,7 @@
     </row>
     <row r="1980">
       <c r="A1980" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1980" t="inlineStr">
         <is>
@@ -40575,7 +40575,7 @@
     </row>
     <row r="1981">
       <c r="A1981" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1981" t="inlineStr">
         <is>
@@ -40596,7 +40596,7 @@
     </row>
     <row r="1982">
       <c r="A1982" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1982" t="inlineStr">
         <is>
@@ -40617,7 +40617,7 @@
     </row>
     <row r="1983">
       <c r="A1983" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1983" t="inlineStr">
         <is>
@@ -40638,7 +40638,7 @@
     </row>
     <row r="1984">
       <c r="A1984" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1984" t="inlineStr">
         <is>
@@ -40659,7 +40659,7 @@
     </row>
     <row r="1985">
       <c r="A1985" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1985" t="inlineStr">
         <is>
@@ -40680,7 +40680,7 @@
     </row>
     <row r="1986">
       <c r="A1986" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1986" t="inlineStr">
         <is>
@@ -40701,7 +40701,7 @@
     </row>
     <row r="1987">
       <c r="A1987" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1987" t="inlineStr">
         <is>
@@ -40722,7 +40722,7 @@
     </row>
     <row r="1988">
       <c r="A1988" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1988" t="inlineStr">
         <is>
@@ -40743,7 +40743,7 @@
     </row>
     <row r="1989">
       <c r="A1989" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1989" t="inlineStr">
         <is>
@@ -40764,7 +40764,7 @@
     </row>
     <row r="1990">
       <c r="A1990" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1990" t="inlineStr">
         <is>
@@ -40785,7 +40785,7 @@
     </row>
     <row r="1991">
       <c r="A1991" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1991" t="inlineStr">
         <is>
@@ -40806,7 +40806,7 @@
     </row>
     <row r="1992">
       <c r="A1992" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1992" t="inlineStr">
         <is>
@@ -40827,7 +40827,7 @@
     </row>
     <row r="1993">
       <c r="A1993" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1993" t="inlineStr">
         <is>
@@ -40848,7 +40848,7 @@
     </row>
     <row r="1994">
       <c r="A1994" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1994" t="inlineStr">
         <is>
@@ -40869,7 +40869,7 @@
     </row>
     <row r="1995">
       <c r="A1995" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1995" t="inlineStr">
         <is>
@@ -40890,7 +40890,7 @@
     </row>
     <row r="1996">
       <c r="A1996" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1996" t="inlineStr">
         <is>
@@ -40911,7 +40911,7 @@
     </row>
     <row r="1997">
       <c r="A1997" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1997" t="inlineStr">
         <is>
@@ -40932,7 +40932,7 @@
     </row>
     <row r="1998">
       <c r="A1998" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1998" t="inlineStr">
         <is>
@@ -40953,7 +40953,7 @@
     </row>
     <row r="1999">
       <c r="A1999" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B1999" t="inlineStr">
         <is>
@@ -40974,7 +40974,7 @@
     </row>
     <row r="2000">
       <c r="A2000" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2000" t="inlineStr">
         <is>
@@ -40995,7 +40995,7 @@
     </row>
     <row r="2001">
       <c r="A2001" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2001" t="inlineStr">
         <is>
@@ -41016,7 +41016,7 @@
     </row>
     <row r="2002">
       <c r="A2002" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2002" t="inlineStr">
         <is>
@@ -41037,7 +41037,7 @@
     </row>
     <row r="2003">
       <c r="A2003" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2003" t="inlineStr">
         <is>
@@ -41058,7 +41058,7 @@
     </row>
     <row r="2004">
       <c r="A2004" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2004" t="inlineStr">
         <is>
@@ -41079,7 +41079,7 @@
     </row>
     <row r="2005">
       <c r="A2005" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2005" t="inlineStr">
         <is>
@@ -41100,7 +41100,7 @@
     </row>
     <row r="2006">
       <c r="A2006" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2006" t="inlineStr">
         <is>
@@ -41121,7 +41121,7 @@
     </row>
     <row r="2007">
       <c r="A2007" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2007" t="inlineStr">
         <is>
@@ -41142,7 +41142,7 @@
     </row>
     <row r="2008">
       <c r="A2008" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2008" t="inlineStr">
         <is>
@@ -41163,7 +41163,7 @@
     </row>
     <row r="2009">
       <c r="A2009" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2009" t="inlineStr">
         <is>
@@ -41184,7 +41184,7 @@
     </row>
     <row r="2010">
       <c r="A2010" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2010" t="inlineStr">
         <is>
@@ -41205,7 +41205,7 @@
     </row>
     <row r="2011">
       <c r="A2011" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2011" t="inlineStr">
         <is>
@@ -41226,7 +41226,7 @@
     </row>
     <row r="2012">
       <c r="A2012" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2012" t="inlineStr">
         <is>
@@ -41247,7 +41247,7 @@
     </row>
     <row r="2013">
       <c r="A2013" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2013" t="inlineStr">
         <is>
@@ -41268,7 +41268,7 @@
     </row>
     <row r="2014">
       <c r="A2014" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2014" t="inlineStr">
         <is>
@@ -41289,7 +41289,7 @@
     </row>
     <row r="2015">
       <c r="A2015" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2015" t="inlineStr">
         <is>
@@ -41310,7 +41310,7 @@
     </row>
     <row r="2016">
       <c r="A2016" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2016" t="inlineStr">
         <is>
@@ -41331,7 +41331,7 @@
     </row>
     <row r="2017">
       <c r="A2017" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2017" t="inlineStr">
         <is>
@@ -41352,7 +41352,7 @@
     </row>
     <row r="2018">
       <c r="A2018" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2018" t="inlineStr">
         <is>
@@ -41373,7 +41373,7 @@
     </row>
     <row r="2019">
       <c r="A2019" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2019" t="inlineStr">
         <is>
@@ -41394,7 +41394,7 @@
     </row>
     <row r="2020">
       <c r="A2020" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2020" t="inlineStr">
         <is>
@@ -41415,7 +41415,7 @@
     </row>
     <row r="2021">
       <c r="A2021" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2021" t="inlineStr">
         <is>
@@ -41436,7 +41436,7 @@
     </row>
     <row r="2022">
       <c r="A2022" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2022" t="inlineStr">
         <is>
@@ -41457,7 +41457,7 @@
     </row>
     <row r="2023">
       <c r="A2023" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2023" t="inlineStr">
         <is>
@@ -41476,7 +41476,7 @@
     </row>
     <row r="2024">
       <c r="A2024" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2024" t="inlineStr">
         <is>
@@ -41497,7 +41497,7 @@
     </row>
     <row r="2025">
       <c r="A2025" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2025" t="inlineStr">
         <is>
@@ -41516,7 +41516,7 @@
     </row>
     <row r="2026">
       <c r="A2026" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2026" t="inlineStr">
         <is>
@@ -41537,7 +41537,7 @@
     </row>
     <row r="2027">
       <c r="A2027" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2027" t="inlineStr">
         <is>
@@ -41558,7 +41558,7 @@
     </row>
     <row r="2028">
       <c r="A2028" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2028" t="inlineStr">
         <is>
@@ -41579,7 +41579,7 @@
     </row>
     <row r="2029">
       <c r="A2029" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2029" t="inlineStr">
         <is>
@@ -41600,7 +41600,7 @@
     </row>
     <row r="2030">
       <c r="A2030" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2030" t="inlineStr">
         <is>
@@ -41621,7 +41621,7 @@
     </row>
     <row r="2031">
       <c r="A2031" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2031" t="inlineStr">
         <is>
@@ -41642,7 +41642,7 @@
     </row>
     <row r="2032">
       <c r="A2032" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2032" t="inlineStr">
         <is>
@@ -41663,7 +41663,7 @@
     </row>
     <row r="2033">
       <c r="A2033" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2033" t="inlineStr">
         <is>
@@ -41684,7 +41684,7 @@
     </row>
     <row r="2034">
       <c r="A2034" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2034" t="inlineStr">
         <is>
@@ -41705,7 +41705,7 @@
     </row>
     <row r="2035">
       <c r="A2035" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2035" t="inlineStr">
         <is>
@@ -41726,7 +41726,7 @@
     </row>
     <row r="2036">
       <c r="A2036" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2036" t="inlineStr">
         <is>
@@ -41747,7 +41747,7 @@
     </row>
     <row r="2037">
       <c r="A2037" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2037" t="inlineStr">
         <is>
@@ -41768,7 +41768,7 @@
     </row>
     <row r="2038">
       <c r="A2038" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2038" t="inlineStr">
         <is>
@@ -41789,7 +41789,7 @@
     </row>
     <row r="2039">
       <c r="A2039" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2039" t="inlineStr">
         <is>
@@ -41810,7 +41810,7 @@
     </row>
     <row r="2040">
       <c r="A2040" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2040" t="inlineStr">
         <is>
@@ -41831,7 +41831,7 @@
     </row>
     <row r="2041">
       <c r="A2041" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2041" t="inlineStr">
         <is>
@@ -41852,7 +41852,7 @@
     </row>
     <row r="2042">
       <c r="A2042" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2042" t="inlineStr">
         <is>
@@ -41873,7 +41873,7 @@
     </row>
     <row r="2043">
       <c r="A2043" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2043" t="inlineStr">
         <is>
@@ -41894,7 +41894,7 @@
     </row>
     <row r="2044">
       <c r="A2044" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2044" t="inlineStr">
         <is>
@@ -41915,7 +41915,7 @@
     </row>
     <row r="2045">
       <c r="A2045" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2045" t="inlineStr">
         <is>
@@ -41936,7 +41936,7 @@
     </row>
     <row r="2046">
       <c r="A2046" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2046" t="inlineStr">
         <is>
@@ -41957,7 +41957,7 @@
     </row>
     <row r="2047">
       <c r="A2047" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2047" t="inlineStr">
         <is>
@@ -41978,7 +41978,7 @@
     </row>
     <row r="2048">
       <c r="A2048" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2048" t="inlineStr">
         <is>
@@ -41999,7 +41999,7 @@
     </row>
     <row r="2049">
       <c r="A2049" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2049" t="inlineStr">
         <is>
@@ -42018,7 +42018,7 @@
     </row>
     <row r="2050">
       <c r="A2050" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2050" t="inlineStr">
         <is>
@@ -42039,7 +42039,7 @@
     </row>
     <row r="2051">
       <c r="A2051" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2051" t="inlineStr">
         <is>
@@ -42060,7 +42060,7 @@
     </row>
     <row r="2052">
       <c r="A2052" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2052" t="inlineStr">
         <is>
@@ -42081,7 +42081,7 @@
     </row>
     <row r="2053">
       <c r="A2053" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2053" t="inlineStr">
         <is>
@@ -42100,7 +42100,7 @@
     </row>
     <row r="2054">
       <c r="A2054" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2054" t="inlineStr">
         <is>
@@ -42119,7 +42119,7 @@
     </row>
     <row r="2055">
       <c r="A2055" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2055" t="inlineStr">
         <is>
@@ -42138,7 +42138,7 @@
     </row>
     <row r="2056">
       <c r="A2056" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2056" t="inlineStr">
         <is>
@@ -42157,7 +42157,7 @@
     </row>
     <row r="2057">
       <c r="A2057" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2057" t="inlineStr">
         <is>
@@ -42176,7 +42176,7 @@
     </row>
     <row r="2058">
       <c r="A2058" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2058" t="inlineStr">
         <is>
@@ -42195,7 +42195,7 @@
     </row>
     <row r="2059">
       <c r="A2059" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2059" t="inlineStr">
         <is>
@@ -42214,7 +42214,7 @@
     </row>
     <row r="2060">
       <c r="A2060" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2060" t="inlineStr">
         <is>
@@ -42233,7 +42233,7 @@
     </row>
     <row r="2061">
       <c r="A2061" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2061" t="inlineStr">
         <is>
@@ -42252,7 +42252,7 @@
     </row>
     <row r="2062">
       <c r="A2062" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2062" t="inlineStr">
         <is>
@@ -42271,7 +42271,7 @@
     </row>
     <row r="2063">
       <c r="A2063" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2063" t="inlineStr">
         <is>
@@ -42290,7 +42290,7 @@
     </row>
     <row r="2064">
       <c r="A2064" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2064" t="inlineStr">
         <is>
@@ -42309,7 +42309,7 @@
     </row>
     <row r="2065">
       <c r="A2065" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2065" t="inlineStr">
         <is>
@@ -42328,7 +42328,7 @@
     </row>
     <row r="2066">
       <c r="A2066" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2066" t="inlineStr">
         <is>
@@ -42347,7 +42347,7 @@
     </row>
     <row r="2067">
       <c r="A2067" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2067" t="inlineStr">
         <is>
@@ -42366,7 +42366,7 @@
     </row>
     <row r="2068">
       <c r="A2068" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2068" t="inlineStr">
         <is>
@@ -42385,7 +42385,7 @@
     </row>
     <row r="2069">
       <c r="A2069" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2069" t="inlineStr">
         <is>
@@ -42404,7 +42404,7 @@
     </row>
     <row r="2070">
       <c r="A2070" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2070" t="inlineStr">
         <is>
@@ -42423,7 +42423,7 @@
     </row>
     <row r="2071">
       <c r="A2071" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2071" t="inlineStr">
         <is>
@@ -42442,7 +42442,7 @@
     </row>
     <row r="2072">
       <c r="A2072" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2072" t="inlineStr">
         <is>
@@ -42461,7 +42461,7 @@
     </row>
     <row r="2073">
       <c r="A2073" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2073" t="inlineStr">
         <is>
@@ -42480,7 +42480,7 @@
     </row>
     <row r="2074">
       <c r="A2074" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2074" t="inlineStr">
         <is>
@@ -42499,7 +42499,7 @@
     </row>
     <row r="2075">
       <c r="A2075" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2075" t="inlineStr">
         <is>
@@ -42518,7 +42518,7 @@
     </row>
     <row r="2076">
       <c r="A2076" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2076" t="inlineStr">
         <is>
@@ -42537,7 +42537,7 @@
     </row>
     <row r="2077">
       <c r="A2077" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2077" t="inlineStr">
         <is>
@@ -42556,7 +42556,7 @@
     </row>
     <row r="2078">
       <c r="A2078" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2078" t="inlineStr">
         <is>
@@ -42575,7 +42575,7 @@
     </row>
     <row r="2079">
       <c r="A2079" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2079" t="inlineStr">
         <is>
@@ -42594,7 +42594,7 @@
     </row>
     <row r="2080">
       <c r="A2080" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2080" t="inlineStr">
         <is>
@@ -42613,7 +42613,7 @@
     </row>
     <row r="2081">
       <c r="A2081" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2081" t="inlineStr">
         <is>
@@ -42632,7 +42632,7 @@
     </row>
     <row r="2082">
       <c r="A2082" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2082" t="inlineStr">
         <is>
@@ -42651,7 +42651,7 @@
     </row>
     <row r="2083">
       <c r="A2083" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2083" t="inlineStr">
         <is>
@@ -42670,7 +42670,7 @@
     </row>
     <row r="2084">
       <c r="A2084" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2084" t="inlineStr">
         <is>
@@ -42689,7 +42689,7 @@
     </row>
     <row r="2085">
       <c r="A2085" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2085" t="inlineStr">
         <is>
@@ -42708,7 +42708,7 @@
     </row>
     <row r="2086">
       <c r="A2086" s="2" t="n">
-        <v>45706.87078163875</v>
+        <v>45706.87078164352</v>
       </c>
       <c r="B2086" t="inlineStr">
         <is>
@@ -42720,6 +42720,2847 @@
       </c>
       <c r="D2086" t="inlineStr"/>
       <c r="E2086" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-kilogram-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2087">
+      <c r="A2087" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2087" t="inlineStr">
+        <is>
+          <t>1 грам абонаментно златно кюлче Tavex</t>
+        </is>
+      </c>
+      <c r="C2087" t="n">
+        <v>183</v>
+      </c>
+      <c r="D2087" t="n">
+        <v>203</v>
+      </c>
+      <c r="E2087" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-abonamentno-zlatno-kulche-tavex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2088">
+      <c r="A2088" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2088" t="inlineStr">
+        <is>
+          <t>0,25 грама златно кюлче Tavex</t>
+        </is>
+      </c>
+      <c r="C2088" t="n">
+        <v>49</v>
+      </c>
+      <c r="D2088" t="n">
+        <v>53</v>
+      </c>
+      <c r="E2088" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/0-25-gr-zlatno-kyulche-tavex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2089">
+      <c r="A2089" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2089" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Британия</t>
+        </is>
+      </c>
+      <c r="C2089" t="n">
+        <v>5639</v>
+      </c>
+      <c r="D2089" t="n">
+        <v>5695</v>
+      </c>
+      <c r="E2089" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-britaniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2090">
+      <c r="A2090" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2090" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Виенска Филхармония</t>
+        </is>
+      </c>
+      <c r="C2090" t="n">
+        <v>5639</v>
+      </c>
+      <c r="D2090" t="n">
+        <v>5723</v>
+      </c>
+      <c r="E2090" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-vienska-filharmoniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2091">
+      <c r="A2091" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2091" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Британия</t>
+        </is>
+      </c>
+      <c r="C2091" t="n">
+        <v>583</v>
+      </c>
+      <c r="D2091" t="n">
+        <v>628</v>
+      </c>
+      <c r="E2091" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlatna-moneta-britaniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2092">
+      <c r="A2092" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2092" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Виенска Филхармония</t>
+        </is>
+      </c>
+      <c r="C2092" t="n">
+        <v>583</v>
+      </c>
+      <c r="D2092" t="n">
+        <v>639</v>
+      </c>
+      <c r="E2092" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-%d1%83%d0%bd%d1%86%d0%b8%d1%8f-%d0%b7%d0%bb%d0%b0%d1%82%d0%bd%d0%b0-%d0%b0%d0%b2%d1%81%d1%82%d1%80%d0%b8%d0%b9%d1%81%d0%ba%d0%b0-%d1%84%d0%b8%d0%bb%d1%85%d0%b0%d1%80%d0%bc%d0%be%d0%bd%d0%b8%d1%8f/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2093">
+      <c r="A2093" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2093" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Канадски кленов лист</t>
+        </is>
+      </c>
+      <c r="C2093" t="n">
+        <v>5639</v>
+      </c>
+      <c r="D2093" t="n">
+        <v>5717</v>
+      </c>
+      <c r="E2093" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-kanadski-klenov-list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2094">
+      <c r="A2094" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2094" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийско кенгуру</t>
+        </is>
+      </c>
+      <c r="C2094" t="n">
+        <v>5639</v>
+      </c>
+      <c r="D2094" t="n">
+        <v>5695</v>
+      </c>
+      <c r="E2094" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliysko-kenguru/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2095">
+      <c r="A2095" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2095" t="inlineStr">
+        <is>
+          <t>100 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2095" t="n">
+        <v>17758</v>
+      </c>
+      <c r="D2095" t="n">
+        <v>18046</v>
+      </c>
+      <c r="E2095" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/100-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2096">
+      <c r="A2096" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2096" t="inlineStr">
+        <is>
+          <t>100 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2096" t="n">
+        <v>17758</v>
+      </c>
+      <c r="D2096" t="n">
+        <v>18064</v>
+      </c>
+      <c r="E2096" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/100-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2097">
+      <c r="A2097" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2097" t="inlineStr">
+        <is>
+          <t>0,25 г златно кюлче Tavex, подаръчен пакет</t>
+        </is>
+      </c>
+      <c r="C2097" t="n">
+        <v>49</v>
+      </c>
+      <c r="D2097" t="n">
+        <v>72</v>
+      </c>
+      <c r="E2097" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/0-25-gr-zlatno-kyulche-tavex-podarachen-paket/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2098">
+      <c r="A2098" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2098" t="inlineStr">
+        <is>
+          <t>50 x 1 грам комбинирано кюлче Valcambi Suisse CombiBar</t>
+        </is>
+      </c>
+      <c r="C2098" t="n">
+        <v>9030</v>
+      </c>
+      <c r="D2098" t="n">
+        <v>9348</v>
+      </c>
+      <c r="E2098" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-kombinirano-zlatno-kulche-valcambi-combibar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2099">
+      <c r="A2099" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2099" t="inlineStr">
+        <is>
+          <t>50 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2099" t="n">
+        <v>9030</v>
+      </c>
+      <c r="D2099" t="n">
+        <v>9112</v>
+      </c>
+      <c r="E2099" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2100">
+      <c r="A2100" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2100" t="inlineStr">
+        <is>
+          <t>50 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2100" t="n">
+        <v>9030</v>
+      </c>
+      <c r="D2100" t="n">
+        <v>9121</v>
+      </c>
+      <c r="E2100" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2101">
+      <c r="A2101" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2101" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2101" t="n">
+        <v>5623</v>
+      </c>
+      <c r="D2101" t="n">
+        <v>5673</v>
+      </c>
+      <c r="E2101" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2102">
+      <c r="A2102" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2102" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче PAMP Suisse</t>
+        </is>
+      </c>
+      <c r="C2102" t="n">
+        <v>5623</v>
+      </c>
+      <c r="D2102" t="n">
+        <v>5676</v>
+      </c>
+      <c r="E2102" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatno-kulche-pamp-suisse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2103">
+      <c r="A2103" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2103" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2103" t="n">
+        <v>5623</v>
+      </c>
+      <c r="D2103" t="n">
+        <v>5679</v>
+      </c>
+      <c r="E2103" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2104">
+      <c r="A2104" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2104" t="inlineStr">
+        <is>
+          <t>20 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2104" t="n">
+        <v>3662</v>
+      </c>
+      <c r="D2104" t="n">
+        <v>3712</v>
+      </c>
+      <c r="E2104" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2105">
+      <c r="A2105" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2105" t="inlineStr">
+        <is>
+          <t>20 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2105" t="n">
+        <v>3662</v>
+      </c>
+      <c r="D2105" t="inlineStr"/>
+      <c r="E2105" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2106">
+      <c r="A2106" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2106" t="inlineStr">
+        <is>
+          <t>20 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2106" t="n">
+        <v>3662</v>
+      </c>
+      <c r="D2106" t="n">
+        <v>3719</v>
+      </c>
+      <c r="E2106" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2107">
+      <c r="A2107" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2107" t="inlineStr">
+        <is>
+          <t>10 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2107" t="n">
+        <v>1831</v>
+      </c>
+      <c r="D2107" t="n">
+        <v>1892</v>
+      </c>
+      <c r="E2107" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2108">
+      <c r="A2108" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2108" t="inlineStr">
+        <is>
+          <t>10 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2108" t="n">
+        <v>1831</v>
+      </c>
+      <c r="D2108" t="n">
+        <v>1909</v>
+      </c>
+      <c r="E2108" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2109">
+      <c r="A2109" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2109" t="inlineStr">
+        <is>
+          <t>10 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2109" t="n">
+        <v>1831</v>
+      </c>
+      <c r="D2109" t="n">
+        <v>1893</v>
+      </c>
+      <c r="E2109" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2110">
+      <c r="A2110" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2110" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2110" t="n">
+        <v>924</v>
+      </c>
+      <c r="D2110" t="n">
+        <v>999</v>
+      </c>
+      <c r="E2110" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2111">
+      <c r="A2111" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2111" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2111" t="n">
+        <v>924</v>
+      </c>
+      <c r="D2111" t="n">
+        <v>1014</v>
+      </c>
+      <c r="E2111" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2112">
+      <c r="A2112" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2112" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2112" t="n">
+        <v>924</v>
+      </c>
+      <c r="D2112" t="n">
+        <v>1001</v>
+      </c>
+      <c r="E2112" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2113">
+      <c r="A2113" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2113" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C2113" t="n">
+        <v>960</v>
+      </c>
+      <c r="D2113" t="n">
+        <v>1050</v>
+      </c>
+      <c r="E2113" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-pamp-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2114">
+      <c r="A2114" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2114" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Argor-Heraeus лунар Змия 2025</t>
+        </is>
+      </c>
+      <c r="C2114" t="n">
+        <v>933</v>
+      </c>
+      <c r="D2114" t="n">
+        <v>1036</v>
+      </c>
+      <c r="E2114" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-argor-heraeus-lunar-zmiya-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2115">
+      <c r="A2115" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2115" t="inlineStr">
+        <is>
+          <t>2,5 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2115" t="n">
+        <v>475</v>
+      </c>
+      <c r="D2115" t="n">
+        <v>531</v>
+      </c>
+      <c r="E2115" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/2-5-grama-zlatno-kyulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2116">
+      <c r="A2116" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2116" t="inlineStr">
+        <is>
+          <t>2,5 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2116" t="n">
+        <v>475</v>
+      </c>
+      <c r="D2116" t="n">
+        <v>535</v>
+      </c>
+      <c r="E2116" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/dva-grama-i-polovina-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2117">
+      <c r="A2117" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2117" t="inlineStr">
+        <is>
+          <t>2 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2117" t="n">
+        <v>380</v>
+      </c>
+      <c r="D2117" t="n">
+        <v>425</v>
+      </c>
+      <c r="E2117" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/2-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2118">
+      <c r="A2118" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2118" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2118" t="n">
+        <v>186</v>
+      </c>
+      <c r="D2118" t="n">
+        <v>224</v>
+      </c>
+      <c r="E2118" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2119">
+      <c r="A2119" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2119" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2119" t="n">
+        <v>186</v>
+      </c>
+      <c r="D2119" t="n">
+        <v>225</v>
+      </c>
+      <c r="E2119" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2120">
+      <c r="A2120" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2120" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2120" t="n">
+        <v>186</v>
+      </c>
+      <c r="D2120" t="n">
+        <v>222</v>
+      </c>
+      <c r="E2120" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2121">
+      <c r="A2121" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2121" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Argor-Heraeus лунар Змия 2025</t>
+        </is>
+      </c>
+      <c r="C2121" t="n">
+        <v>213</v>
+      </c>
+      <c r="D2121" t="n">
+        <v>270</v>
+      </c>
+      <c r="E2121" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kyulche-argor-heraeus-lunar-zmiya-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2122">
+      <c r="A2122" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2122" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Американски орел</t>
+        </is>
+      </c>
+      <c r="C2122" t="n">
+        <v>5639</v>
+      </c>
+      <c r="D2122" t="n">
+        <v>5867</v>
+      </c>
+      <c r="E2122" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-uncia-amerikanski-orel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2123">
+      <c r="A2123" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2123" t="inlineStr">
+        <is>
+          <t>20 долара двоен орел лейди Либърти</t>
+        </is>
+      </c>
+      <c r="C2123" t="n">
+        <v>5296</v>
+      </c>
+      <c r="D2123" t="n">
+        <v>6236</v>
+      </c>
+      <c r="E2123" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-dolara-dvoen-orel-lejdi-libarti/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2124">
+      <c r="A2124" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2124" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Американски бизон</t>
+        </is>
+      </c>
+      <c r="C2124" t="n">
+        <v>5722</v>
+      </c>
+      <c r="D2124" t="n">
+        <v>5977</v>
+      </c>
+      <c r="E2124" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-amerikanski-bizon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2125">
+      <c r="A2125" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2125" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Кругерранд, Южна Африка</t>
+        </is>
+      </c>
+      <c r="C2125" t="n">
+        <v>5562</v>
+      </c>
+      <c r="D2125" t="n">
+        <v>5673</v>
+      </c>
+      <c r="E2125" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-krugerrand-yujna-afrika/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2126">
+      <c r="A2126" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2126" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Слон Южна Африка - Големите 5</t>
+        </is>
+      </c>
+      <c r="C2126" t="n">
+        <v>5639</v>
+      </c>
+      <c r="D2126" t="n">
+        <v>5756</v>
+      </c>
+      <c r="E2126" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-slon-yuzhna-afrika-golemite-5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2127">
+      <c r="A2127" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2127" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2127" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2127" t="n">
+        <v>6390</v>
+      </c>
+      <c r="E2127" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2128">
+      <c r="A2128" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2128" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C2128" t="n">
+        <v>5805</v>
+      </c>
+      <c r="D2128" t="n">
+        <v>6092</v>
+      </c>
+      <c r="E2128" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2129">
+      <c r="A2129" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2129" t="inlineStr">
+        <is>
+          <t>1/4 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C2129" t="n">
+        <v>1451</v>
+      </c>
+      <c r="D2129" t="n">
+        <v>1652</v>
+      </c>
+      <c r="E2129" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-4-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2130">
+      <c r="A2130" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2130" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C2130" t="n">
+        <v>581</v>
+      </c>
+      <c r="D2130" t="n">
+        <v>716</v>
+      </c>
+      <c r="E2130" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2131">
+      <c r="A2131" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2131" t="inlineStr">
+        <is>
+          <t>1/20 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C2131" t="n">
+        <v>277</v>
+      </c>
+      <c r="D2131" t="n">
+        <v>405</v>
+      </c>
+      <c r="E2131" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-20-unciya-zlaten-avstraliiski-lunar-godina-na-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2132">
+      <c r="A2132" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2132" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C2132" t="n">
+        <v>5750</v>
+      </c>
+      <c r="D2132" t="n">
+        <v>5867</v>
+      </c>
+      <c r="E2132" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2133">
+      <c r="A2133" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2133" t="inlineStr">
+        <is>
+          <t>1/2 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C2133" t="n">
+        <v>2820</v>
+      </c>
+      <c r="D2133" t="n">
+        <v>3140</v>
+      </c>
+      <c r="E2133" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-2-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2134">
+      <c r="A2134" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2134" t="inlineStr">
+        <is>
+          <t>1/4 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C2134" t="n">
+        <v>1451</v>
+      </c>
+      <c r="D2134" t="n">
+        <v>1625</v>
+      </c>
+      <c r="E2134" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-4-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2135">
+      <c r="A2135" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2135" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C2135" t="n">
+        <v>581</v>
+      </c>
+      <c r="D2135" t="n">
+        <v>705</v>
+      </c>
+      <c r="E2135" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2136">
+      <c r="A2136" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2136" t="inlineStr">
+        <is>
+          <t>1/20 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C2136" t="n">
+        <v>277</v>
+      </c>
+      <c r="D2136" t="n">
+        <v>405</v>
+      </c>
+      <c r="E2136" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-20-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2137">
+      <c r="A2137" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2137" t="inlineStr">
+        <is>
+          <t>Руска златна монета 5 рубли Николай II</t>
+        </is>
+      </c>
+      <c r="C2137" t="n">
+        <v>757</v>
+      </c>
+      <c r="D2137" t="n">
+        <v>993</v>
+      </c>
+      <c r="E2137" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-5-rubli-nikolay-iii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2138">
+      <c r="A2138" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2138" t="inlineStr">
+        <is>
+          <t>10 рубли Николай II Русия</t>
+        </is>
+      </c>
+      <c r="C2138" t="n">
+        <v>1514</v>
+      </c>
+      <c r="D2138" t="n">
+        <v>2057</v>
+      </c>
+      <c r="E2138" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-rubli-nikolai-ii-rusia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2139">
+      <c r="A2139" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2139" t="inlineStr">
+        <is>
+          <t>20 френски франка Наполеон III</t>
+        </is>
+      </c>
+      <c r="C2139" t="n">
+        <v>1053</v>
+      </c>
+      <c r="D2139" t="n">
+        <v>1083</v>
+      </c>
+      <c r="E2139" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-frenski-franka-napoleon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2140">
+      <c r="A2140" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2140" t="inlineStr">
+        <is>
+          <t>20 френски франка златна монета Наполеон III с лавров венец</t>
+        </is>
+      </c>
+      <c r="C2140" t="n">
+        <v>1053</v>
+      </c>
+      <c r="D2140" t="n">
+        <v>1083</v>
+      </c>
+      <c r="E2140" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-%d1%84%d1%80%d0%b0%d0%bd%d0%ba%d0%b0-%d1%84%d1%80%d0%b5%d0%bd%d1%81%d0%ba%d0%b8-%d0%bd%d0%b0%d0%bf%d0%be%d0%bb%d0%b5%d0%be%d0%bd-%d1%81-%d0%bb%d0%b0%d0%b2%d1%80%d0%be%d0%b2-%d0%b2%d0%b5%d0%bd%d0%b5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2141">
+      <c r="A2141" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2141" t="inlineStr">
+        <is>
+          <t>10 франка френски Наполеон III</t>
+        </is>
+      </c>
+      <c r="C2141" t="n">
+        <v>573</v>
+      </c>
+      <c r="D2141" t="n">
+        <v>656</v>
+      </c>
+      <c r="E2141" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-frenski-franka-napoleon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2142">
+      <c r="A2142" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2142" t="inlineStr">
+        <is>
+          <t>10 френски франка златна монета Наполеон III с лавров венец</t>
+        </is>
+      </c>
+      <c r="C2142" t="n">
+        <v>573</v>
+      </c>
+      <c r="D2142" t="inlineStr"/>
+      <c r="E2142" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-frenski-franka-zlatna-moneta-napoleon-iii-s-lavrov-venets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2143">
+      <c r="A2143" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2143" t="inlineStr">
+        <is>
+          <t>Златна монета 20 френски франка Серес</t>
+        </is>
+      </c>
+      <c r="C2143" t="n">
+        <v>1053</v>
+      </c>
+      <c r="D2143" t="n">
+        <v>1083</v>
+      </c>
+      <c r="E2143" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-frenski-franka-seres/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2144">
+      <c r="A2144" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2144" t="inlineStr">
+        <is>
+          <t>20 френски франка златна монета Гениус</t>
+        </is>
+      </c>
+      <c r="C2144" t="n">
+        <v>1053</v>
+      </c>
+      <c r="D2144" t="n">
+        <v>1083</v>
+      </c>
+      <c r="E2144" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-zlatni-frenski-franka-genius/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2145">
+      <c r="A2145" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2145" t="inlineStr">
+        <is>
+          <t>Златна монета 20 франка Мариана</t>
+        </is>
+      </c>
+      <c r="C2145" t="n">
+        <v>1053</v>
+      </c>
+      <c r="D2145" t="n">
+        <v>1083</v>
+      </c>
+      <c r="E2145" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-frenski-franka-mariana/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2146">
+      <c r="A2146" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2146" t="inlineStr">
+        <is>
+          <t>20 белгийски франка златна монета Леополд II</t>
+        </is>
+      </c>
+      <c r="C2146" t="n">
+        <v>1055</v>
+      </c>
+      <c r="D2146" t="n">
+        <v>1085</v>
+      </c>
+      <c r="E2146" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-belgiiski-franka-leopold-ii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2147">
+      <c r="A2147" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2147" t="inlineStr">
+        <is>
+          <t>20 лири Виктор Емануил II Италия</t>
+        </is>
+      </c>
+      <c r="C2147" t="n">
+        <v>1055</v>
+      </c>
+      <c r="D2147" t="n">
+        <v>1101</v>
+      </c>
+      <c r="E2147" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/italian-20lira-emanuele/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2148">
+      <c r="A2148" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2148" t="inlineStr">
+        <is>
+          <t>20 лири златна монета Умберто I, Италия</t>
+        </is>
+      </c>
+      <c r="C2148" t="n">
+        <v>1055</v>
+      </c>
+      <c r="D2148" t="n">
+        <v>1085</v>
+      </c>
+      <c r="E2148" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-liri-zlatna-moneta-umberto-i-italiya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2149">
+      <c r="A2149" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2149" t="inlineStr">
+        <is>
+          <t>4 австрийски дуката златна монета Франц Йосиф</t>
+        </is>
+      </c>
+      <c r="C2149" t="n">
+        <v>2448</v>
+      </c>
+      <c r="D2149" t="n">
+        <v>2646</v>
+      </c>
+      <c r="E2149" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-4-avstriiski-dukata-franc-iosif/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2150">
+      <c r="A2150" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2150" t="inlineStr">
+        <is>
+          <t>1 австрийски дукат златна монета Франц Йосиф</t>
+        </is>
+      </c>
+      <c r="C2150" t="n">
+        <v>630</v>
+      </c>
+      <c r="D2150" t="n">
+        <v>664</v>
+      </c>
+      <c r="E2150" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-1-avstriiski-dukat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2151">
+      <c r="A2151" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2151" t="inlineStr">
+        <is>
+          <t>8 форинта/20 франка Франц Йосиф Унгария</t>
+        </is>
+      </c>
+      <c r="C2151" t="n">
+        <v>1053</v>
+      </c>
+      <c r="D2151" t="n">
+        <v>1111</v>
+      </c>
+      <c r="E2151" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-forinta-20-franka-franc-iosif-ungariia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2152">
+      <c r="A2152" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2152" t="inlineStr">
+        <is>
+          <t>Златна монета 4 флорина/10 франка Франц Йосиф, Австрия</t>
+        </is>
+      </c>
+      <c r="C2152" t="n">
+        <v>552</v>
+      </c>
+      <c r="D2152" t="n">
+        <v>591</v>
+      </c>
+      <c r="E2152" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-4-florina-10-franka-franc-iosif-avstria/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2153">
+      <c r="A2153" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2153" t="inlineStr">
+        <is>
+          <t>20 франка златна монета Швейцария Вренели</t>
+        </is>
+      </c>
+      <c r="C2153" t="n">
+        <v>1053</v>
+      </c>
+      <c r="D2153" t="n">
+        <v>1085</v>
+      </c>
+      <c r="E2153" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-zlatni-franka-shveitsariya-vreneli/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2154">
+      <c r="A2154" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2154" t="inlineStr">
+        <is>
+          <t>10 гулдена Вилхелмина Холандия</t>
+        </is>
+      </c>
+      <c r="C2154" t="n">
+        <v>1071</v>
+      </c>
+      <c r="D2154" t="n">
+        <v>1164</v>
+      </c>
+      <c r="E2154" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-guldena-vilhemina-holandiya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2155">
+      <c r="A2155" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2155" t="inlineStr">
+        <is>
+          <t>20 германски марки Вилхелм II</t>
+        </is>
+      </c>
+      <c r="C2155" t="n">
+        <v>1287</v>
+      </c>
+      <c r="D2155" t="n">
+        <v>1383</v>
+      </c>
+      <c r="E2155" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-germanski-marki-vilhelm-ii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2156">
+      <c r="A2156" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2156" t="inlineStr">
+        <is>
+          <t>Златен Мемориален Суверен Чарлз III Великобритания 2022г.</t>
+        </is>
+      </c>
+      <c r="C2156" t="n">
+        <v>1328</v>
+      </c>
+      <c r="D2156" t="n">
+        <v>1387</v>
+      </c>
+      <c r="E2156" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-memorialen-suveren-charles-iii-2022/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2157">
+      <c r="A2157" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2157" t="inlineStr">
+        <is>
+          <t>Златен Суверен Чарлз III Великобритания</t>
+        </is>
+      </c>
+      <c r="C2157" t="n">
+        <v>1335</v>
+      </c>
+      <c r="D2157" t="n">
+        <v>1394</v>
+      </c>
+      <c r="E2157" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-charles-iii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2158">
+      <c r="A2158" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2158" t="inlineStr">
+        <is>
+          <t>Златен суверен Елизабет II 1957-2021 Великобритания</t>
+        </is>
+      </c>
+      <c r="C2158" t="n">
+        <v>1301</v>
+      </c>
+      <c r="D2158" t="n">
+        <v>1351</v>
+      </c>
+      <c r="E2158" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/suveren-elizabet-ii-velikobritaniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2159">
+      <c r="A2159" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2159" t="inlineStr">
+        <is>
+          <t>Златен суверен Едуард VII Великобритания</t>
+        </is>
+      </c>
+      <c r="C2159" t="n">
+        <v>1301</v>
+      </c>
+      <c r="D2159" t="n">
+        <v>1374</v>
+      </c>
+      <c r="E2159" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-eduard-vii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2160">
+      <c r="A2160" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2160" t="inlineStr">
+        <is>
+          <t>Златен суверен Джордж V Великобритания</t>
+        </is>
+      </c>
+      <c r="C2160" t="n">
+        <v>1301</v>
+      </c>
+      <c r="D2160" t="n">
+        <v>1374</v>
+      </c>
+      <c r="E2160" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-jorge-v/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2161">
+      <c r="A2161" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2161" t="inlineStr">
+        <is>
+          <t>Златен суверен Виктория Великобритания</t>
+        </is>
+      </c>
+      <c r="C2161" t="n">
+        <v>1301</v>
+      </c>
+      <c r="D2161" t="n">
+        <v>1387</v>
+      </c>
+      <c r="E2161" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-viktoriya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2162">
+      <c r="A2162" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2162" t="inlineStr">
+        <is>
+          <t>Британски златен суверен Елизабет II, 2022г.</t>
+        </is>
+      </c>
+      <c r="C2162" t="n">
+        <v>1301</v>
+      </c>
+      <c r="D2162" t="inlineStr"/>
+      <c r="E2162" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-britanski-suveren-elizabet-ii-2022/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2163">
+      <c r="A2163" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2163" t="inlineStr">
+        <is>
+          <t>20 франка златна монета Тунис</t>
+        </is>
+      </c>
+      <c r="C2163" t="n">
+        <v>1048</v>
+      </c>
+      <c r="D2163" t="n">
+        <v>1142</v>
+      </c>
+      <c r="E2163" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-franka-zlatna-moneta-tunis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2164">
+      <c r="A2164" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2164" t="inlineStr">
+        <is>
+          <t>Златна монета 100 турски куруша</t>
+        </is>
+      </c>
+      <c r="C2164" t="n">
+        <v>1048</v>
+      </c>
+      <c r="D2164" t="inlineStr"/>
+      <c r="E2164" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-100-turski-kurusha/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2165">
+      <c r="A2165" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2165" t="inlineStr">
+        <is>
+          <t>Златна монета 50 песос, Мексико</t>
+        </is>
+      </c>
+      <c r="C2165" t="n">
+        <v>6666</v>
+      </c>
+      <c r="D2165" t="n">
+        <v>7073</v>
+      </c>
+      <c r="E2165" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-50-pesos-meksiko/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2166">
+      <c r="A2166" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2166" t="inlineStr">
+        <is>
+          <t>Златна монета 100 австрийски корони Франц Йосиф</t>
+        </is>
+      </c>
+      <c r="C2166" t="n">
+        <v>5338</v>
+      </c>
+      <c r="D2166" t="n">
+        <v>5723</v>
+      </c>
+      <c r="E2166" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-100-avstriyski-koroni-franc-yosif/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2167">
+      <c r="A2167" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2167" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2167" t="n">
+        <v>5439</v>
+      </c>
+      <c r="D2167" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E2167" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2168">
+      <c r="A2168" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2168" t="inlineStr">
+        <is>
+          <t>15 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2168" t="n">
+        <v>2720</v>
+      </c>
+      <c r="D2168" t="n">
+        <v>2975</v>
+      </c>
+      <c r="E2168" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/15-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2169">
+      <c r="A2169" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2169" t="inlineStr">
+        <is>
+          <t>8 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2169" t="n">
+        <v>1450</v>
+      </c>
+      <c r="D2169" t="n">
+        <v>1629</v>
+      </c>
+      <c r="E2169" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2170">
+      <c r="A2170" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2170" t="inlineStr">
+        <is>
+          <t>3 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2170" t="n">
+        <v>544</v>
+      </c>
+      <c r="D2170" t="n">
+        <v>691</v>
+      </c>
+      <c r="E2170" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/3-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2171">
+      <c r="A2171" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2171" t="inlineStr">
+        <is>
+          <t>1 грам златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2171" t="n">
+        <v>181</v>
+      </c>
+      <c r="D2171" t="n">
+        <v>275</v>
+      </c>
+      <c r="E2171" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2172">
+      <c r="A2172" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2172" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Тигъра 2022</t>
+        </is>
+      </c>
+      <c r="C2172" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2172" t="n">
+        <v>8263</v>
+      </c>
+      <c r="E2172" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-oz-australian-lunar-year-of-the-tiger-2022-gold-coin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2173">
+      <c r="A2173" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2173" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Вола 2021</t>
+        </is>
+      </c>
+      <c r="C2173" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2173" t="n">
+        <v>6609</v>
+      </c>
+      <c r="E2173" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-oz-australian-lunar-year-of-the-ox-2021-gold-coin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2174">
+      <c r="A2174" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2174" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийски лунар година на Мишката 2020</t>
+        </is>
+      </c>
+      <c r="C2174" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2174" t="n">
+        <v>6500</v>
+      </c>
+      <c r="E2174" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyski-lunar-godina-mishkata-2020/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2175">
+      <c r="A2175" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2175" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Кучето 2018</t>
+        </is>
+      </c>
+      <c r="C2175" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2175" t="n">
+        <v>6500</v>
+      </c>
+      <c r="E2175" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni38s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-22/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2176">
+      <c r="A2176" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2176" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Петела 2017</t>
+        </is>
+      </c>
+      <c r="C2176" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2176" t="n">
+        <v>6500</v>
+      </c>
+      <c r="E2176" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni40s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-24/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2177">
+      <c r="A2177" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2177" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Маймуната 2016</t>
+        </is>
+      </c>
+      <c r="C2177" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2177" t="n">
+        <v>6500</v>
+      </c>
+      <c r="E2177" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-maimunata-2016/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2178">
+      <c r="A2178" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2178" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Змията 2013</t>
+        </is>
+      </c>
+      <c r="C2178" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2178" t="n">
+        <v>6609</v>
+      </c>
+      <c r="E2178" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlaten-avstraliiski-lunar-godina-na-zmiyata-2013/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2179">
+      <c r="A2179" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2179" t="inlineStr">
+        <is>
+          <t>1 унция австралиисйки лунар година на дракона 2012</t>
+        </is>
+      </c>
+      <c r="C2179" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2179" t="n">
+        <v>6500</v>
+      </c>
+      <c r="E2179" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-drakona-2012/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2180">
+      <c r="A2180" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2180" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Заека 2011</t>
+        </is>
+      </c>
+      <c r="C2180" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2180" t="n">
+        <v>6500</v>
+      </c>
+      <c r="E2180" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-moneta-avstraliiski-lunar-zaek-2011/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2181">
+      <c r="A2181" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2181" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Вола 2009</t>
+        </is>
+      </c>
+      <c r="C2181" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2181" t="n">
+        <v>6500</v>
+      </c>
+      <c r="E2181" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-avstraliiski-lunar-godina-na-vola-2009/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2182">
+      <c r="A2182" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2182" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Мишката 2008</t>
+        </is>
+      </c>
+      <c r="C2182" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2182" t="n">
+        <v>6500</v>
+      </c>
+      <c r="E2182" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-uncia-moneta-lunar-mishka-2008/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2183">
+      <c r="A2183" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2183" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Прасето 2007</t>
+        </is>
+      </c>
+      <c r="C2183" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2183" t="n">
+        <v>6500</v>
+      </c>
+      <c r="E2183" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-avstraliiski-lunar-godina-na-praseto-2007/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2184">
+      <c r="A2184" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2184" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Петела 2005</t>
+        </is>
+      </c>
+      <c r="C2184" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2184" t="n">
+        <v>6500</v>
+      </c>
+      <c r="E2184" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-petela-2005/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2185">
+      <c r="A2185" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2185" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Маймуната 2004</t>
+        </is>
+      </c>
+      <c r="C2185" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2185" t="n">
+        <v>6500</v>
+      </c>
+      <c r="E2185" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-%d1%83%d0%bd%d1%86%d0%b8%d1%8f-%d0%b7%d0%bb%d0%b0%d1%82%d0%b5%d0%bd-%d0%b0%d0%b2%d1%81%d1%82%d1%80%d0%b0%d0%bb%d0%b8%d0%b9%d1%81%d0%ba%d0%b8-%d0%bb%d1%83%d0%bd%d0%b0%d1%80-%d0%b3%d0%be%d0%b4%d0%b8-2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2186">
+      <c r="A2186" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2186" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Козата 2003</t>
+        </is>
+      </c>
+      <c r="C2186" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2186" t="n">
+        <v>6500</v>
+      </c>
+      <c r="E2186" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni38s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-24/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2187">
+      <c r="A2187" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2187" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийки Лунар 2000 година на дракона</t>
+        </is>
+      </c>
+      <c r="C2187" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2187" t="n">
+        <v>7437</v>
+      </c>
+      <c r="E2187" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyki-lunar-2000-godina-drakona/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2188">
+      <c r="A2188" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2188" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Тигъра 2010</t>
+        </is>
+      </c>
+      <c r="C2188" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2188" t="inlineStr"/>
+      <c r="E2188" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-tigura-2010/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2189">
+      <c r="A2189" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2189" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Кучето 2006</t>
+        </is>
+      </c>
+      <c r="C2189" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2189" t="n">
+        <v>6500</v>
+      </c>
+      <c r="E2189" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-kucheto-2006/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2190">
+      <c r="A2190" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2190" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Тигъра 1998</t>
+        </is>
+      </c>
+      <c r="C2190" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2190" t="n">
+        <v>6885</v>
+      </c>
+      <c r="E2190" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliiski-lunar-godinata-na-tigara-1998/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2191">
+      <c r="A2191" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2191" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Вола 1997</t>
+        </is>
+      </c>
+      <c r="C2191" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2191" t="n">
+        <v>6885</v>
+      </c>
+      <c r="E2191" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliiski-lunar-godinata-na-vola-1997/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2192">
+      <c r="A2192" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2192" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Мишката 1996</t>
+        </is>
+      </c>
+      <c r="C2192" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2192" t="inlineStr"/>
+      <c r="E2192" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni42s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2193">
+      <c r="A2193" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2193" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Коня 2014</t>
+        </is>
+      </c>
+      <c r="C2193" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2193" t="inlineStr"/>
+      <c r="E2193" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-konq-2014/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2194">
+      <c r="A2194" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2194" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Argor-Heraeus лунар Дракон 2024</t>
+        </is>
+      </c>
+      <c r="C2194" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2194" t="inlineStr"/>
+      <c r="E2194" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-argor-heraeus-lunar-drakon-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2195">
+      <c r="A2195" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2195" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Argor-Heraeus лунар Дракон 2024</t>
+        </is>
+      </c>
+      <c r="C2195" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2195" t="inlineStr"/>
+      <c r="E2195" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kyulche-argor-heraeus-lunar-drakon-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2196">
+      <c r="A2196" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2196" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2196" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2196" t="inlineStr"/>
+      <c r="E2196" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2197">
+      <c r="A2197" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2197" t="inlineStr">
+        <is>
+          <t>15 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2197" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2197" t="inlineStr"/>
+      <c r="E2197" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/15-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2198">
+      <c r="A2198" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2198" t="inlineStr">
+        <is>
+          <t>8 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2198" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2198" t="inlineStr"/>
+      <c r="E2198" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2199">
+      <c r="A2199" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2199" t="inlineStr">
+        <is>
+          <t>3 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2199" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2199" t="inlineStr"/>
+      <c r="E2199" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/3-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2200">
+      <c r="A2200" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2200" t="inlineStr">
+        <is>
+          <t>1 грам златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2200" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2200" t="inlineStr"/>
+      <c r="E2200" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2201">
+      <c r="A2201" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2201" t="inlineStr">
+        <is>
+          <t>1/2 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C2201" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2201" t="inlineStr"/>
+      <c r="E2201" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-2-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2202">
+      <c r="A2202" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2202" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Драконът на Тюдор 2024г.</t>
+        </is>
+      </c>
+      <c r="C2202" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2202" t="inlineStr"/>
+      <c r="E2202" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-pazitelite-na-tudorite-drakonat-na-tudor-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2203">
+      <c r="A2203" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2203" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Еднорогът на Сиймор 2024 г.</t>
+        </is>
+      </c>
+      <c r="C2203" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2203" t="inlineStr"/>
+      <c r="E2203" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-pazitelite-na-tyudorite-ednorogut-na-siimor-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2204">
+      <c r="A2204" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2204" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Бикът от Кларънс 2023 г.</t>
+        </is>
+      </c>
+      <c r="C2204" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2204" t="inlineStr"/>
+      <c r="E2204" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-pazitelite-na-tyudorite-bikut-ot-klaruns-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2205">
+      <c r="A2205" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2205" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Британия - Елизабет II</t>
+        </is>
+      </c>
+      <c r="C2205" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2205" t="inlineStr"/>
+      <c r="E2205" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-britaniya-elizabet-ii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2206">
+      <c r="A2206" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2206" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Йейлът на Бофорт 2023 г.</t>
+        </is>
+      </c>
+      <c r="C2206" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2206" t="inlineStr"/>
+      <c r="E2206" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-oz-zlatna-moneta-pazitelite-na-tyudorite-yeylut-na-bofort-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2207">
+      <c r="A2207" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2207" t="inlineStr">
+        <is>
+          <t>1/2 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2207" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2207" t="inlineStr"/>
+      <c r="E2207" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-2-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2208">
+      <c r="A2208" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2208" t="inlineStr">
+        <is>
+          <t>1/4 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2208" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2208" t="inlineStr"/>
+      <c r="E2208" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-4-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2209">
+      <c r="A2209" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2209" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C2209" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2209" t="inlineStr"/>
+      <c r="E2209" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-pamp-lunar-drakon-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2210">
+      <c r="A2210" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2210" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2210" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2210" t="inlineStr"/>
+      <c r="E2210" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-pamp-lunar-zaek-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2211">
+      <c r="A2211" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2211" t="inlineStr">
+        <is>
+          <t>1/10 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2211" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2211" t="inlineStr"/>
+      <c r="E2211" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2212">
+      <c r="A2212" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2212" t="inlineStr">
+        <is>
+          <t>15 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2212" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2212" t="inlineStr"/>
+      <c r="E2212" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/15-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2213">
+      <c r="A2213" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2213" t="inlineStr">
+        <is>
+          <t>1/20 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2213" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2213" t="inlineStr"/>
+      <c r="E2213" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-20-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2214">
+      <c r="A2214" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2214" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2214" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2214" t="inlineStr"/>
+      <c r="E2214" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2215">
+      <c r="A2215" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2215" t="inlineStr">
+        <is>
+          <t>8 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2215" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2215" t="inlineStr"/>
+      <c r="E2215" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2216">
+      <c r="A2216" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2216" t="inlineStr">
+        <is>
+          <t>3 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2216" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2216" t="inlineStr"/>
+      <c r="E2216" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/3-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2217">
+      <c r="A2217" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2217" t="inlineStr">
+        <is>
+          <t>1 грам златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2217" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2217" t="inlineStr"/>
+      <c r="E2217" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2218">
+      <c r="A2218" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2218" t="inlineStr">
+        <is>
+          <t>100 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2218" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2218" t="inlineStr"/>
+      <c r="E2218" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/100-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2219">
+      <c r="A2219" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2219" t="inlineStr">
+        <is>
+          <t>50 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2219" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2219" t="inlineStr"/>
+      <c r="E2219" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2220">
+      <c r="A2220" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2220" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2220" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2220" t="inlineStr"/>
+      <c r="E2220" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2221">
+      <c r="A2221" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2221" t="inlineStr">
+        <is>
+          <t>10 крони Кристиян X Дания</t>
+        </is>
+      </c>
+      <c r="C2221" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2221" t="inlineStr"/>
+      <c r="E2221" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-kroni-kristiyan-x-daniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2222">
+      <c r="A2222" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2222" t="inlineStr">
+        <is>
+          <t>10 Гулдена Вилхелм III Холандия</t>
+        </is>
+      </c>
+      <c r="C2222" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2222" t="inlineStr"/>
+      <c r="E2222" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni38s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-9/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2223">
+      <c r="A2223" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2223" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2022</t>
+        </is>
+      </c>
+      <c r="C2223" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2223" t="inlineStr"/>
+      <c r="E2223" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitayska-panda-2022/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2224">
+      <c r="A2224" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2224" t="inlineStr">
+        <is>
+          <t>Златна монета 10 франка Мариана</t>
+        </is>
+      </c>
+      <c r="C2224" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2224" t="inlineStr"/>
+      <c r="E2224" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-frenski-franka-mariana/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2225">
+      <c r="A2225" s="2" t="n">
+        <v>45707.898585527</v>
+      </c>
+      <c r="B2225" t="inlineStr">
+        <is>
+          <t>1 килограм златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2225" t="n">
+        <v>5695</v>
+      </c>
+      <c r="D2225" t="inlineStr"/>
+      <c r="E2225" t="inlineStr">
         <is>
           <t>https://tavex.bg/zlato/1-kilogram-zlatno-kulche-valcambi/</t>
         </is>

</xml_diff>

<commit_message>
Report 20 02 2025
</commit_message>
<xml_diff>
--- a/price_history_gold.xlsx
+++ b/price_history_gold.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2225"/>
+  <dimension ref="A1:E2365"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -42727,7 +42727,7 @@
     </row>
     <row r="2087">
       <c r="A2087" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2087" t="inlineStr">
         <is>
@@ -42748,7 +42748,7 @@
     </row>
     <row r="2088">
       <c r="A2088" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2088" t="inlineStr">
         <is>
@@ -42769,7 +42769,7 @@
     </row>
     <row r="2089">
       <c r="A2089" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2089" t="inlineStr">
         <is>
@@ -42790,7 +42790,7 @@
     </row>
     <row r="2090">
       <c r="A2090" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2090" t="inlineStr">
         <is>
@@ -42811,7 +42811,7 @@
     </row>
     <row r="2091">
       <c r="A2091" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2091" t="inlineStr">
         <is>
@@ -42832,7 +42832,7 @@
     </row>
     <row r="2092">
       <c r="A2092" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2092" t="inlineStr">
         <is>
@@ -42853,7 +42853,7 @@
     </row>
     <row r="2093">
       <c r="A2093" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2093" t="inlineStr">
         <is>
@@ -42874,7 +42874,7 @@
     </row>
     <row r="2094">
       <c r="A2094" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2094" t="inlineStr">
         <is>
@@ -42895,7 +42895,7 @@
     </row>
     <row r="2095">
       <c r="A2095" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2095" t="inlineStr">
         <is>
@@ -42916,7 +42916,7 @@
     </row>
     <row r="2096">
       <c r="A2096" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2096" t="inlineStr">
         <is>
@@ -42937,7 +42937,7 @@
     </row>
     <row r="2097">
       <c r="A2097" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2097" t="inlineStr">
         <is>
@@ -42958,7 +42958,7 @@
     </row>
     <row r="2098">
       <c r="A2098" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2098" t="inlineStr">
         <is>
@@ -42979,7 +42979,7 @@
     </row>
     <row r="2099">
       <c r="A2099" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2099" t="inlineStr">
         <is>
@@ -43000,7 +43000,7 @@
     </row>
     <row r="2100">
       <c r="A2100" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2100" t="inlineStr">
         <is>
@@ -43021,7 +43021,7 @@
     </row>
     <row r="2101">
       <c r="A2101" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2101" t="inlineStr">
         <is>
@@ -43042,7 +43042,7 @@
     </row>
     <row r="2102">
       <c r="A2102" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2102" t="inlineStr">
         <is>
@@ -43063,7 +43063,7 @@
     </row>
     <row r="2103">
       <c r="A2103" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2103" t="inlineStr">
         <is>
@@ -43084,7 +43084,7 @@
     </row>
     <row r="2104">
       <c r="A2104" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2104" t="inlineStr">
         <is>
@@ -43105,7 +43105,7 @@
     </row>
     <row r="2105">
       <c r="A2105" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2105" t="inlineStr">
         <is>
@@ -43124,7 +43124,7 @@
     </row>
     <row r="2106">
       <c r="A2106" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2106" t="inlineStr">
         <is>
@@ -43145,7 +43145,7 @@
     </row>
     <row r="2107">
       <c r="A2107" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2107" t="inlineStr">
         <is>
@@ -43166,7 +43166,7 @@
     </row>
     <row r="2108">
       <c r="A2108" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2108" t="inlineStr">
         <is>
@@ -43187,7 +43187,7 @@
     </row>
     <row r="2109">
       <c r="A2109" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2109" t="inlineStr">
         <is>
@@ -43208,7 +43208,7 @@
     </row>
     <row r="2110">
       <c r="A2110" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2110" t="inlineStr">
         <is>
@@ -43229,7 +43229,7 @@
     </row>
     <row r="2111">
       <c r="A2111" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2111" t="inlineStr">
         <is>
@@ -43250,7 +43250,7 @@
     </row>
     <row r="2112">
       <c r="A2112" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2112" t="inlineStr">
         <is>
@@ -43271,7 +43271,7 @@
     </row>
     <row r="2113">
       <c r="A2113" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2113" t="inlineStr">
         <is>
@@ -43292,7 +43292,7 @@
     </row>
     <row r="2114">
       <c r="A2114" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2114" t="inlineStr">
         <is>
@@ -43313,7 +43313,7 @@
     </row>
     <row r="2115">
       <c r="A2115" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2115" t="inlineStr">
         <is>
@@ -43334,7 +43334,7 @@
     </row>
     <row r="2116">
       <c r="A2116" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2116" t="inlineStr">
         <is>
@@ -43355,7 +43355,7 @@
     </row>
     <row r="2117">
       <c r="A2117" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2117" t="inlineStr">
         <is>
@@ -43376,7 +43376,7 @@
     </row>
     <row r="2118">
       <c r="A2118" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2118" t="inlineStr">
         <is>
@@ -43397,7 +43397,7 @@
     </row>
     <row r="2119">
       <c r="A2119" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2119" t="inlineStr">
         <is>
@@ -43418,7 +43418,7 @@
     </row>
     <row r="2120">
       <c r="A2120" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2120" t="inlineStr">
         <is>
@@ -43439,7 +43439,7 @@
     </row>
     <row r="2121">
       <c r="A2121" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2121" t="inlineStr">
         <is>
@@ -43460,7 +43460,7 @@
     </row>
     <row r="2122">
       <c r="A2122" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2122" t="inlineStr">
         <is>
@@ -43481,7 +43481,7 @@
     </row>
     <row r="2123">
       <c r="A2123" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2123" t="inlineStr">
         <is>
@@ -43502,7 +43502,7 @@
     </row>
     <row r="2124">
       <c r="A2124" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2124" t="inlineStr">
         <is>
@@ -43523,7 +43523,7 @@
     </row>
     <row r="2125">
       <c r="A2125" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2125" t="inlineStr">
         <is>
@@ -43544,7 +43544,7 @@
     </row>
     <row r="2126">
       <c r="A2126" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2126" t="inlineStr">
         <is>
@@ -43565,7 +43565,7 @@
     </row>
     <row r="2127">
       <c r="A2127" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2127" t="inlineStr">
         <is>
@@ -43586,7 +43586,7 @@
     </row>
     <row r="2128">
       <c r="A2128" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2128" t="inlineStr">
         <is>
@@ -43607,7 +43607,7 @@
     </row>
     <row r="2129">
       <c r="A2129" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2129" t="inlineStr">
         <is>
@@ -43628,7 +43628,7 @@
     </row>
     <row r="2130">
       <c r="A2130" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2130" t="inlineStr">
         <is>
@@ -43649,7 +43649,7 @@
     </row>
     <row r="2131">
       <c r="A2131" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2131" t="inlineStr">
         <is>
@@ -43670,7 +43670,7 @@
     </row>
     <row r="2132">
       <c r="A2132" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2132" t="inlineStr">
         <is>
@@ -43691,7 +43691,7 @@
     </row>
     <row r="2133">
       <c r="A2133" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2133" t="inlineStr">
         <is>
@@ -43712,7 +43712,7 @@
     </row>
     <row r="2134">
       <c r="A2134" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2134" t="inlineStr">
         <is>
@@ -43733,7 +43733,7 @@
     </row>
     <row r="2135">
       <c r="A2135" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2135" t="inlineStr">
         <is>
@@ -43754,7 +43754,7 @@
     </row>
     <row r="2136">
       <c r="A2136" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2136" t="inlineStr">
         <is>
@@ -43775,7 +43775,7 @@
     </row>
     <row r="2137">
       <c r="A2137" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2137" t="inlineStr">
         <is>
@@ -43796,7 +43796,7 @@
     </row>
     <row r="2138">
       <c r="A2138" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2138" t="inlineStr">
         <is>
@@ -43817,7 +43817,7 @@
     </row>
     <row r="2139">
       <c r="A2139" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2139" t="inlineStr">
         <is>
@@ -43838,7 +43838,7 @@
     </row>
     <row r="2140">
       <c r="A2140" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2140" t="inlineStr">
         <is>
@@ -43859,7 +43859,7 @@
     </row>
     <row r="2141">
       <c r="A2141" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2141" t="inlineStr">
         <is>
@@ -43880,7 +43880,7 @@
     </row>
     <row r="2142">
       <c r="A2142" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2142" t="inlineStr">
         <is>
@@ -43899,7 +43899,7 @@
     </row>
     <row r="2143">
       <c r="A2143" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2143" t="inlineStr">
         <is>
@@ -43920,7 +43920,7 @@
     </row>
     <row r="2144">
       <c r="A2144" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2144" t="inlineStr">
         <is>
@@ -43941,7 +43941,7 @@
     </row>
     <row r="2145">
       <c r="A2145" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2145" t="inlineStr">
         <is>
@@ -43962,7 +43962,7 @@
     </row>
     <row r="2146">
       <c r="A2146" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2146" t="inlineStr">
         <is>
@@ -43983,7 +43983,7 @@
     </row>
     <row r="2147">
       <c r="A2147" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2147" t="inlineStr">
         <is>
@@ -44004,7 +44004,7 @@
     </row>
     <row r="2148">
       <c r="A2148" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2148" t="inlineStr">
         <is>
@@ -44025,7 +44025,7 @@
     </row>
     <row r="2149">
       <c r="A2149" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2149" t="inlineStr">
         <is>
@@ -44046,7 +44046,7 @@
     </row>
     <row r="2150">
       <c r="A2150" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2150" t="inlineStr">
         <is>
@@ -44067,7 +44067,7 @@
     </row>
     <row r="2151">
       <c r="A2151" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2151" t="inlineStr">
         <is>
@@ -44088,7 +44088,7 @@
     </row>
     <row r="2152">
       <c r="A2152" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2152" t="inlineStr">
         <is>
@@ -44109,7 +44109,7 @@
     </row>
     <row r="2153">
       <c r="A2153" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2153" t="inlineStr">
         <is>
@@ -44130,7 +44130,7 @@
     </row>
     <row r="2154">
       <c r="A2154" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2154" t="inlineStr">
         <is>
@@ -44151,7 +44151,7 @@
     </row>
     <row r="2155">
       <c r="A2155" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2155" t="inlineStr">
         <is>
@@ -44172,7 +44172,7 @@
     </row>
     <row r="2156">
       <c r="A2156" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2156" t="inlineStr">
         <is>
@@ -44193,7 +44193,7 @@
     </row>
     <row r="2157">
       <c r="A2157" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2157" t="inlineStr">
         <is>
@@ -44214,7 +44214,7 @@
     </row>
     <row r="2158">
       <c r="A2158" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2158" t="inlineStr">
         <is>
@@ -44235,7 +44235,7 @@
     </row>
     <row r="2159">
       <c r="A2159" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2159" t="inlineStr">
         <is>
@@ -44256,7 +44256,7 @@
     </row>
     <row r="2160">
       <c r="A2160" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2160" t="inlineStr">
         <is>
@@ -44277,7 +44277,7 @@
     </row>
     <row r="2161">
       <c r="A2161" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2161" t="inlineStr">
         <is>
@@ -44298,7 +44298,7 @@
     </row>
     <row r="2162">
       <c r="A2162" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2162" t="inlineStr">
         <is>
@@ -44317,7 +44317,7 @@
     </row>
     <row r="2163">
       <c r="A2163" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2163" t="inlineStr">
         <is>
@@ -44338,7 +44338,7 @@
     </row>
     <row r="2164">
       <c r="A2164" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2164" t="inlineStr">
         <is>
@@ -44357,7 +44357,7 @@
     </row>
     <row r="2165">
       <c r="A2165" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2165" t="inlineStr">
         <is>
@@ -44378,7 +44378,7 @@
     </row>
     <row r="2166">
       <c r="A2166" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2166" t="inlineStr">
         <is>
@@ -44399,7 +44399,7 @@
     </row>
     <row r="2167">
       <c r="A2167" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2167" t="inlineStr">
         <is>
@@ -44420,7 +44420,7 @@
     </row>
     <row r="2168">
       <c r="A2168" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2168" t="inlineStr">
         <is>
@@ -44441,7 +44441,7 @@
     </row>
     <row r="2169">
       <c r="A2169" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2169" t="inlineStr">
         <is>
@@ -44462,7 +44462,7 @@
     </row>
     <row r="2170">
       <c r="A2170" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2170" t="inlineStr">
         <is>
@@ -44483,7 +44483,7 @@
     </row>
     <row r="2171">
       <c r="A2171" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2171" t="inlineStr">
         <is>
@@ -44504,7 +44504,7 @@
     </row>
     <row r="2172">
       <c r="A2172" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2172" t="inlineStr">
         <is>
@@ -44525,7 +44525,7 @@
     </row>
     <row r="2173">
       <c r="A2173" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2173" t="inlineStr">
         <is>
@@ -44546,7 +44546,7 @@
     </row>
     <row r="2174">
       <c r="A2174" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2174" t="inlineStr">
         <is>
@@ -44567,7 +44567,7 @@
     </row>
     <row r="2175">
       <c r="A2175" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2175" t="inlineStr">
         <is>
@@ -44588,7 +44588,7 @@
     </row>
     <row r="2176">
       <c r="A2176" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2176" t="inlineStr">
         <is>
@@ -44609,7 +44609,7 @@
     </row>
     <row r="2177">
       <c r="A2177" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2177" t="inlineStr">
         <is>
@@ -44630,7 +44630,7 @@
     </row>
     <row r="2178">
       <c r="A2178" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2178" t="inlineStr">
         <is>
@@ -44651,7 +44651,7 @@
     </row>
     <row r="2179">
       <c r="A2179" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2179" t="inlineStr">
         <is>
@@ -44672,7 +44672,7 @@
     </row>
     <row r="2180">
       <c r="A2180" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2180" t="inlineStr">
         <is>
@@ -44693,7 +44693,7 @@
     </row>
     <row r="2181">
       <c r="A2181" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2181" t="inlineStr">
         <is>
@@ -44714,7 +44714,7 @@
     </row>
     <row r="2182">
       <c r="A2182" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2182" t="inlineStr">
         <is>
@@ -44735,7 +44735,7 @@
     </row>
     <row r="2183">
       <c r="A2183" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2183" t="inlineStr">
         <is>
@@ -44756,7 +44756,7 @@
     </row>
     <row r="2184">
       <c r="A2184" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2184" t="inlineStr">
         <is>
@@ -44777,7 +44777,7 @@
     </row>
     <row r="2185">
       <c r="A2185" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2185" t="inlineStr">
         <is>
@@ -44798,7 +44798,7 @@
     </row>
     <row r="2186">
       <c r="A2186" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2186" t="inlineStr">
         <is>
@@ -44819,7 +44819,7 @@
     </row>
     <row r="2187">
       <c r="A2187" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2187" t="inlineStr">
         <is>
@@ -44840,7 +44840,7 @@
     </row>
     <row r="2188">
       <c r="A2188" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2188" t="inlineStr">
         <is>
@@ -44859,7 +44859,7 @@
     </row>
     <row r="2189">
       <c r="A2189" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2189" t="inlineStr">
         <is>
@@ -44880,7 +44880,7 @@
     </row>
     <row r="2190">
       <c r="A2190" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2190" t="inlineStr">
         <is>
@@ -44901,7 +44901,7 @@
     </row>
     <row r="2191">
       <c r="A2191" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2191" t="inlineStr">
         <is>
@@ -44922,7 +44922,7 @@
     </row>
     <row r="2192">
       <c r="A2192" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2192" t="inlineStr">
         <is>
@@ -44941,7 +44941,7 @@
     </row>
     <row r="2193">
       <c r="A2193" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2193" t="inlineStr">
         <is>
@@ -44960,7 +44960,7 @@
     </row>
     <row r="2194">
       <c r="A2194" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2194" t="inlineStr">
         <is>
@@ -44979,7 +44979,7 @@
     </row>
     <row r="2195">
       <c r="A2195" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2195" t="inlineStr">
         <is>
@@ -44998,7 +44998,7 @@
     </row>
     <row r="2196">
       <c r="A2196" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2196" t="inlineStr">
         <is>
@@ -45017,7 +45017,7 @@
     </row>
     <row r="2197">
       <c r="A2197" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2197" t="inlineStr">
         <is>
@@ -45036,7 +45036,7 @@
     </row>
     <row r="2198">
       <c r="A2198" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2198" t="inlineStr">
         <is>
@@ -45055,7 +45055,7 @@
     </row>
     <row r="2199">
       <c r="A2199" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2199" t="inlineStr">
         <is>
@@ -45074,7 +45074,7 @@
     </row>
     <row r="2200">
       <c r="A2200" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2200" t="inlineStr">
         <is>
@@ -45093,7 +45093,7 @@
     </row>
     <row r="2201">
       <c r="A2201" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2201" t="inlineStr">
         <is>
@@ -45112,7 +45112,7 @@
     </row>
     <row r="2202">
       <c r="A2202" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2202" t="inlineStr">
         <is>
@@ -45131,7 +45131,7 @@
     </row>
     <row r="2203">
       <c r="A2203" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2203" t="inlineStr">
         <is>
@@ -45150,7 +45150,7 @@
     </row>
     <row r="2204">
       <c r="A2204" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2204" t="inlineStr">
         <is>
@@ -45169,7 +45169,7 @@
     </row>
     <row r="2205">
       <c r="A2205" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2205" t="inlineStr">
         <is>
@@ -45188,7 +45188,7 @@
     </row>
     <row r="2206">
       <c r="A2206" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2206" t="inlineStr">
         <is>
@@ -45207,7 +45207,7 @@
     </row>
     <row r="2207">
       <c r="A2207" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2207" t="inlineStr">
         <is>
@@ -45226,7 +45226,7 @@
     </row>
     <row r="2208">
       <c r="A2208" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2208" t="inlineStr">
         <is>
@@ -45245,7 +45245,7 @@
     </row>
     <row r="2209">
       <c r="A2209" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2209" t="inlineStr">
         <is>
@@ -45264,7 +45264,7 @@
     </row>
     <row r="2210">
       <c r="A2210" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2210" t="inlineStr">
         <is>
@@ -45283,7 +45283,7 @@
     </row>
     <row r="2211">
       <c r="A2211" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2211" t="inlineStr">
         <is>
@@ -45302,7 +45302,7 @@
     </row>
     <row r="2212">
       <c r="A2212" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2212" t="inlineStr">
         <is>
@@ -45321,7 +45321,7 @@
     </row>
     <row r="2213">
       <c r="A2213" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2213" t="inlineStr">
         <is>
@@ -45340,7 +45340,7 @@
     </row>
     <row r="2214">
       <c r="A2214" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2214" t="inlineStr">
         <is>
@@ -45359,7 +45359,7 @@
     </row>
     <row r="2215">
       <c r="A2215" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2215" t="inlineStr">
         <is>
@@ -45378,7 +45378,7 @@
     </row>
     <row r="2216">
       <c r="A2216" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2216" t="inlineStr">
         <is>
@@ -45397,7 +45397,7 @@
     </row>
     <row r="2217">
       <c r="A2217" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2217" t="inlineStr">
         <is>
@@ -45416,7 +45416,7 @@
     </row>
     <row r="2218">
       <c r="A2218" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2218" t="inlineStr">
         <is>
@@ -45435,7 +45435,7 @@
     </row>
     <row r="2219">
       <c r="A2219" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2219" t="inlineStr">
         <is>
@@ -45454,7 +45454,7 @@
     </row>
     <row r="2220">
       <c r="A2220" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2220" t="inlineStr">
         <is>
@@ -45473,7 +45473,7 @@
     </row>
     <row r="2221">
       <c r="A2221" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2221" t="inlineStr">
         <is>
@@ -45492,7 +45492,7 @@
     </row>
     <row r="2222">
       <c r="A2222" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2222" t="inlineStr">
         <is>
@@ -45511,7 +45511,7 @@
     </row>
     <row r="2223">
       <c r="A2223" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2223" t="inlineStr">
         <is>
@@ -45530,7 +45530,7 @@
     </row>
     <row r="2224">
       <c r="A2224" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2224" t="inlineStr">
         <is>
@@ -45549,7 +45549,7 @@
     </row>
     <row r="2225">
       <c r="A2225" s="2" t="n">
-        <v>45707.898585527</v>
+        <v>45707.89858553241</v>
       </c>
       <c r="B2225" t="inlineStr">
         <is>
@@ -45561,6 +45561,2868 @@
       </c>
       <c r="D2225" t="inlineStr"/>
       <c r="E2225" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-kilogram-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2226">
+      <c r="A2226" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2226" t="inlineStr">
+        <is>
+          <t>1 грам абонаментно златно кюлче Tavex</t>
+        </is>
+      </c>
+      <c r="C2226" t="n">
+        <v>182</v>
+      </c>
+      <c r="D2226" t="n">
+        <v>202</v>
+      </c>
+      <c r="E2226" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-abonamentno-zlatno-kulche-tavex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2227">
+      <c r="A2227" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2227" t="inlineStr">
+        <is>
+          <t>0,25 грама златно кюлче Tavex</t>
+        </is>
+      </c>
+      <c r="C2227" t="n">
+        <v>48</v>
+      </c>
+      <c r="D2227" t="n">
+        <v>53</v>
+      </c>
+      <c r="E2227" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/0-25-gr-zlatno-kyulche-tavex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2228">
+      <c r="A2228" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2228" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Британия</t>
+        </is>
+      </c>
+      <c r="C2228" t="n">
+        <v>5625</v>
+      </c>
+      <c r="D2228" t="n">
+        <v>5682</v>
+      </c>
+      <c r="E2228" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-britaniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2229">
+      <c r="A2229" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2229" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Виенска Филхармония</t>
+        </is>
+      </c>
+      <c r="C2229" t="n">
+        <v>5625</v>
+      </c>
+      <c r="D2229" t="n">
+        <v>5709</v>
+      </c>
+      <c r="E2229" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-vienska-filharmoniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2230">
+      <c r="A2230" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2230" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Британия</t>
+        </is>
+      </c>
+      <c r="C2230" t="n">
+        <v>582</v>
+      </c>
+      <c r="D2230" t="n">
+        <v>627</v>
+      </c>
+      <c r="E2230" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlatna-moneta-britaniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2231">
+      <c r="A2231" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2231" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Виенска Филхармония</t>
+        </is>
+      </c>
+      <c r="C2231" t="n">
+        <v>582</v>
+      </c>
+      <c r="D2231" t="n">
+        <v>638</v>
+      </c>
+      <c r="E2231" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-%d1%83%d0%bd%d1%86%d0%b8%d1%8f-%d0%b7%d0%bb%d0%b0%d1%82%d0%bd%d0%b0-%d0%b0%d0%b2%d1%81%d1%82%d1%80%d0%b8%d0%b9%d1%81%d0%ba%d0%b0-%d1%84%d0%b8%d0%bb%d1%85%d0%b0%d1%80%d0%bc%d0%be%d0%bd%d0%b8%d1%8f/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2232">
+      <c r="A2232" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2232" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Канадски кленов лист</t>
+        </is>
+      </c>
+      <c r="C2232" t="n">
+        <v>5625</v>
+      </c>
+      <c r="D2232" t="n">
+        <v>5704</v>
+      </c>
+      <c r="E2232" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-kanadski-klenov-list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2233">
+      <c r="A2233" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2233" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийско кенгуру</t>
+        </is>
+      </c>
+      <c r="C2233" t="n">
+        <v>5625</v>
+      </c>
+      <c r="D2233" t="n">
+        <v>5682</v>
+      </c>
+      <c r="E2233" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliysko-kenguru/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2234">
+      <c r="A2234" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2234" t="inlineStr">
+        <is>
+          <t>100 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2234" t="n">
+        <v>17713</v>
+      </c>
+      <c r="D2234" t="n">
+        <v>18003</v>
+      </c>
+      <c r="E2234" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/100-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2235">
+      <c r="A2235" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2235" t="inlineStr">
+        <is>
+          <t>100 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2235" t="n">
+        <v>17713</v>
+      </c>
+      <c r="D2235" t="n">
+        <v>18021</v>
+      </c>
+      <c r="E2235" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/100-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2236">
+      <c r="A2236" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2236" t="inlineStr">
+        <is>
+          <t>0,25 г златно кюлче Tavex, подаръчен пакет</t>
+        </is>
+      </c>
+      <c r="C2236" t="n">
+        <v>48</v>
+      </c>
+      <c r="D2236" t="n">
+        <v>72</v>
+      </c>
+      <c r="E2236" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/0-25-gr-zlatno-kyulche-tavex-podarachen-paket/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2237">
+      <c r="A2237" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2237" t="inlineStr">
+        <is>
+          <t>50 x 1 грам комбинирано кюлче Valcambi Suisse CombiBar</t>
+        </is>
+      </c>
+      <c r="C2237" t="n">
+        <v>9007</v>
+      </c>
+      <c r="D2237" t="n">
+        <v>9326</v>
+      </c>
+      <c r="E2237" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-kombinirano-zlatno-kulche-valcambi-combibar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2238">
+      <c r="A2238" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2238" t="inlineStr">
+        <is>
+          <t>50 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2238" t="n">
+        <v>9007</v>
+      </c>
+      <c r="D2238" t="n">
+        <v>9090</v>
+      </c>
+      <c r="E2238" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2239">
+      <c r="A2239" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2239" t="inlineStr">
+        <is>
+          <t>50 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2239" t="n">
+        <v>9007</v>
+      </c>
+      <c r="D2239" t="n">
+        <v>9099</v>
+      </c>
+      <c r="E2239" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2240">
+      <c r="A2240" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2240" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2240" t="n">
+        <v>5609</v>
+      </c>
+      <c r="D2240" t="n">
+        <v>5660</v>
+      </c>
+      <c r="E2240" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2241">
+      <c r="A2241" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2241" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче PAMP Suisse</t>
+        </is>
+      </c>
+      <c r="C2241" t="n">
+        <v>5609</v>
+      </c>
+      <c r="D2241" t="n">
+        <v>5663</v>
+      </c>
+      <c r="E2241" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatno-kulche-pamp-suisse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2242">
+      <c r="A2242" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2242" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2242" t="n">
+        <v>5609</v>
+      </c>
+      <c r="D2242" t="n">
+        <v>5665</v>
+      </c>
+      <c r="E2242" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2243">
+      <c r="A2243" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2243" t="inlineStr">
+        <is>
+          <t>20 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2243" t="n">
+        <v>3653</v>
+      </c>
+      <c r="D2243" t="n">
+        <v>3703</v>
+      </c>
+      <c r="E2243" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2244">
+      <c r="A2244" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2244" t="inlineStr">
+        <is>
+          <t>20 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2244" t="n">
+        <v>3653</v>
+      </c>
+      <c r="D2244" t="inlineStr"/>
+      <c r="E2244" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2245">
+      <c r="A2245" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2245" t="inlineStr">
+        <is>
+          <t>20 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2245" t="n">
+        <v>3653</v>
+      </c>
+      <c r="D2245" t="n">
+        <v>3710</v>
+      </c>
+      <c r="E2245" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2246">
+      <c r="A2246" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2246" t="inlineStr">
+        <is>
+          <t>10 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2246" t="n">
+        <v>1827</v>
+      </c>
+      <c r="D2246" t="n">
+        <v>1887</v>
+      </c>
+      <c r="E2246" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2247">
+      <c r="A2247" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2247" t="inlineStr">
+        <is>
+          <t>10 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2247" t="n">
+        <v>1827</v>
+      </c>
+      <c r="D2247" t="n">
+        <v>1905</v>
+      </c>
+      <c r="E2247" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2248">
+      <c r="A2248" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2248" t="inlineStr">
+        <is>
+          <t>10 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2248" t="n">
+        <v>1827</v>
+      </c>
+      <c r="D2248" t="n">
+        <v>1889</v>
+      </c>
+      <c r="E2248" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2249">
+      <c r="A2249" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2249" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2249" t="n">
+        <v>922</v>
+      </c>
+      <c r="D2249" t="n">
+        <v>997</v>
+      </c>
+      <c r="E2249" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2250">
+      <c r="A2250" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2250" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2250" t="n">
+        <v>922</v>
+      </c>
+      <c r="D2250" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E2250" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2251">
+      <c r="A2251" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2251" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2251" t="n">
+        <v>922</v>
+      </c>
+      <c r="D2251" t="n">
+        <v>998</v>
+      </c>
+      <c r="E2251" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2252">
+      <c r="A2252" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2252" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C2252" t="n">
+        <v>957</v>
+      </c>
+      <c r="D2252" t="n">
+        <v>1047</v>
+      </c>
+      <c r="E2252" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-pamp-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2253">
+      <c r="A2253" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2253" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Argor-Heraeus лунар Змия 2025</t>
+        </is>
+      </c>
+      <c r="C2253" t="n">
+        <v>931</v>
+      </c>
+      <c r="D2253" t="n">
+        <v>1034</v>
+      </c>
+      <c r="E2253" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-argor-heraeus-lunar-zmiya-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2254">
+      <c r="A2254" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2254" t="inlineStr">
+        <is>
+          <t>2,5 грама златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2254" t="n">
+        <v>474</v>
+      </c>
+      <c r="D2254" t="n">
+        <v>530</v>
+      </c>
+      <c r="E2254" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/2-5-grama-zlatno-kyulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2255">
+      <c r="A2255" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2255" t="inlineStr">
+        <is>
+          <t>2,5 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2255" t="n">
+        <v>474</v>
+      </c>
+      <c r="D2255" t="n">
+        <v>534</v>
+      </c>
+      <c r="E2255" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/dva-grama-i-polovina-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2256">
+      <c r="A2256" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2256" t="inlineStr">
+        <is>
+          <t>2 грама златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2256" t="n">
+        <v>379</v>
+      </c>
+      <c r="D2256" t="n">
+        <v>424</v>
+      </c>
+      <c r="E2256" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/2-grama-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2257">
+      <c r="A2257" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2257" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2257" t="n">
+        <v>186</v>
+      </c>
+      <c r="D2257" t="n">
+        <v>223</v>
+      </c>
+      <c r="E2257" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kulche-valcambi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2258">
+      <c r="A2258" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2258" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2258" t="n">
+        <v>186</v>
+      </c>
+      <c r="D2258" t="n">
+        <v>225</v>
+      </c>
+      <c r="E2258" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2259">
+      <c r="A2259" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2259" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Argor-Heraeus</t>
+        </is>
+      </c>
+      <c r="C2259" t="n">
+        <v>186</v>
+      </c>
+      <c r="D2259" t="n">
+        <v>221</v>
+      </c>
+      <c r="E2259" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kyulche-argor-heraeus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2260">
+      <c r="A2260" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2260" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Argor-Heraeus лунар Змия 2025</t>
+        </is>
+      </c>
+      <c r="C2260" t="n">
+        <v>212</v>
+      </c>
+      <c r="D2260" t="n">
+        <v>269</v>
+      </c>
+      <c r="E2260" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kyulche-argor-heraeus-lunar-zmiya-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2261">
+      <c r="A2261" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2261" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Американски орел</t>
+        </is>
+      </c>
+      <c r="C2261" t="n">
+        <v>5625</v>
+      </c>
+      <c r="D2261" t="n">
+        <v>5853</v>
+      </c>
+      <c r="E2261" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-uncia-amerikanski-orel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2262">
+      <c r="A2262" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2262" t="inlineStr">
+        <is>
+          <t>20 долара двоен орел лейди Либърти</t>
+        </is>
+      </c>
+      <c r="C2262" t="n">
+        <v>5282</v>
+      </c>
+      <c r="D2262" t="n">
+        <v>6221</v>
+      </c>
+      <c r="E2262" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-dolara-dvoen-orel-lejdi-libarti/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2263">
+      <c r="A2263" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2263" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Американски бизон</t>
+        </is>
+      </c>
+      <c r="C2263" t="n">
+        <v>5708</v>
+      </c>
+      <c r="D2263" t="n">
+        <v>5962</v>
+      </c>
+      <c r="E2263" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-amerikanski-bizon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2264">
+      <c r="A2264" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2264" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Кругерранд, Южна Африка</t>
+        </is>
+      </c>
+      <c r="C2264" t="n">
+        <v>5548</v>
+      </c>
+      <c r="D2264" t="n">
+        <v>5660</v>
+      </c>
+      <c r="E2264" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-krugerrand-yujna-afrika/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2265">
+      <c r="A2265" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2265" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Слон Южна Африка - Големите 5</t>
+        </is>
+      </c>
+      <c r="C2265" t="n">
+        <v>5625</v>
+      </c>
+      <c r="D2265" t="n">
+        <v>5742</v>
+      </c>
+      <c r="E2265" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-slon-yuzhna-afrika-golemite-5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2266">
+      <c r="A2266" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2266" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите Пантерата на Кралицата</t>
+        </is>
+      </c>
+      <c r="C2266" t="n">
+        <v>5653</v>
+      </c>
+      <c r="D2266" t="n">
+        <v>5831</v>
+      </c>
+      <c r="E2266" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-untsiya-zlatna-moneta-pazitelite-na-tyudorite-panterata-na-kralitsata/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2267">
+      <c r="A2267" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2267" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2267" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2267" t="n">
+        <v>6375</v>
+      </c>
+      <c r="E2267" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2268">
+      <c r="A2268" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2268" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C2268" t="n">
+        <v>5790</v>
+      </c>
+      <c r="D2268" t="n">
+        <v>6078</v>
+      </c>
+      <c r="E2268" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2269">
+      <c r="A2269" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2269" t="inlineStr">
+        <is>
+          <t>1/4 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C2269" t="n">
+        <v>1447</v>
+      </c>
+      <c r="D2269" t="n">
+        <v>1648</v>
+      </c>
+      <c r="E2269" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-4-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2270">
+      <c r="A2270" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2270" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C2270" t="n">
+        <v>579</v>
+      </c>
+      <c r="D2270" t="n">
+        <v>715</v>
+      </c>
+      <c r="E2270" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2271">
+      <c r="A2271" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2271" t="inlineStr">
+        <is>
+          <t>1/20 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C2271" t="n">
+        <v>276</v>
+      </c>
+      <c r="D2271" t="n">
+        <v>404</v>
+      </c>
+      <c r="E2271" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-20-unciya-zlaten-avstraliiski-lunar-godina-na-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2272">
+      <c r="A2272" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2272" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C2272" t="n">
+        <v>5736</v>
+      </c>
+      <c r="D2272" t="n">
+        <v>5853</v>
+      </c>
+      <c r="E2272" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2273">
+      <c r="A2273" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2273" t="inlineStr">
+        <is>
+          <t>1/2 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C2273" t="n">
+        <v>2813</v>
+      </c>
+      <c r="D2273" t="n">
+        <v>3132</v>
+      </c>
+      <c r="E2273" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-2-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2274">
+      <c r="A2274" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2274" t="inlineStr">
+        <is>
+          <t>1/4 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C2274" t="n">
+        <v>1447</v>
+      </c>
+      <c r="D2274" t="n">
+        <v>1621</v>
+      </c>
+      <c r="E2274" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-4-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2275">
+      <c r="A2275" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2275" t="inlineStr">
+        <is>
+          <t>1/10 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C2275" t="n">
+        <v>579</v>
+      </c>
+      <c r="D2275" t="n">
+        <v>704</v>
+      </c>
+      <c r="E2275" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2276">
+      <c r="A2276" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2276" t="inlineStr">
+        <is>
+          <t>1/20 унция златна монета Австралийски лунар година на Змията 2025</t>
+        </is>
+      </c>
+      <c r="C2276" t="n">
+        <v>276</v>
+      </c>
+      <c r="D2276" t="n">
+        <v>404</v>
+      </c>
+      <c r="E2276" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-20-unciya-zlatna-moneta-avstraliyski-lunar-godina-zmiyata-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2277">
+      <c r="A2277" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2277" t="inlineStr">
+        <is>
+          <t>Руска златна монета 5 рубли Николай II</t>
+        </is>
+      </c>
+      <c r="C2277" t="n">
+        <v>755</v>
+      </c>
+      <c r="D2277" t="n">
+        <v>991</v>
+      </c>
+      <c r="E2277" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-5-rubli-nikolay-iii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2278">
+      <c r="A2278" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2278" t="inlineStr">
+        <is>
+          <t>10 рубли Николай II Русия</t>
+        </is>
+      </c>
+      <c r="C2278" t="n">
+        <v>1510</v>
+      </c>
+      <c r="D2278" t="n">
+        <v>2052</v>
+      </c>
+      <c r="E2278" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-rubli-nikolai-ii-rusia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2279">
+      <c r="A2279" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2279" t="inlineStr">
+        <is>
+          <t>20 френски франка Наполеон III</t>
+        </is>
+      </c>
+      <c r="C2279" t="n">
+        <v>1050</v>
+      </c>
+      <c r="D2279" t="n">
+        <v>1081</v>
+      </c>
+      <c r="E2279" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-frenski-franka-napoleon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2280">
+      <c r="A2280" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2280" t="inlineStr">
+        <is>
+          <t>20 френски франка златна монета Наполеон III с лавров венец</t>
+        </is>
+      </c>
+      <c r="C2280" t="n">
+        <v>1050</v>
+      </c>
+      <c r="D2280" t="n">
+        <v>1081</v>
+      </c>
+      <c r="E2280" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-%d1%84%d1%80%d0%b0%d0%bd%d0%ba%d0%b0-%d1%84%d1%80%d0%b5%d0%bd%d1%81%d0%ba%d0%b8-%d0%bd%d0%b0%d0%bf%d0%be%d0%bb%d0%b5%d0%be%d0%bd-%d1%81-%d0%bb%d0%b0%d0%b2%d1%80%d0%be%d0%b2-%d0%b2%d0%b5%d0%bd%d0%b5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2281">
+      <c r="A2281" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2281" t="inlineStr">
+        <is>
+          <t>10 франка френски Наполеон III</t>
+        </is>
+      </c>
+      <c r="C2281" t="n">
+        <v>571</v>
+      </c>
+      <c r="D2281" t="n">
+        <v>654</v>
+      </c>
+      <c r="E2281" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-frenski-franka-napoleon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2282">
+      <c r="A2282" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2282" t="inlineStr">
+        <is>
+          <t>10 френски франка златна монета Наполеон III с лавров венец</t>
+        </is>
+      </c>
+      <c r="C2282" t="n">
+        <v>571</v>
+      </c>
+      <c r="D2282" t="inlineStr"/>
+      <c r="E2282" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-frenski-franka-zlatna-moneta-napoleon-iii-s-lavrov-venets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2283">
+      <c r="A2283" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2283" t="inlineStr">
+        <is>
+          <t>Златна монета 20 френски франка Серес</t>
+        </is>
+      </c>
+      <c r="C2283" t="n">
+        <v>1050</v>
+      </c>
+      <c r="D2283" t="n">
+        <v>1081</v>
+      </c>
+      <c r="E2283" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-frenski-franka-seres/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2284">
+      <c r="A2284" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2284" t="inlineStr">
+        <is>
+          <t>20 френски франка златна монета Гениус</t>
+        </is>
+      </c>
+      <c r="C2284" t="n">
+        <v>1050</v>
+      </c>
+      <c r="D2284" t="n">
+        <v>1081</v>
+      </c>
+      <c r="E2284" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-zlatni-frenski-franka-genius/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2285">
+      <c r="A2285" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2285" t="inlineStr">
+        <is>
+          <t>Златна монета 20 франка Мариана</t>
+        </is>
+      </c>
+      <c r="C2285" t="n">
+        <v>1050</v>
+      </c>
+      <c r="D2285" t="n">
+        <v>1081</v>
+      </c>
+      <c r="E2285" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-frenski-franka-mariana/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2286">
+      <c r="A2286" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2286" t="inlineStr">
+        <is>
+          <t>20 белгийски франка златна монета Леополд II</t>
+        </is>
+      </c>
+      <c r="C2286" t="n">
+        <v>1052</v>
+      </c>
+      <c r="D2286" t="n">
+        <v>1083</v>
+      </c>
+      <c r="E2286" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-belgiiski-franka-leopold-ii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2287">
+      <c r="A2287" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2287" t="inlineStr">
+        <is>
+          <t>20 лири Виктор Емануил II Италия</t>
+        </is>
+      </c>
+      <c r="C2287" t="n">
+        <v>1052</v>
+      </c>
+      <c r="D2287" t="n">
+        <v>1098</v>
+      </c>
+      <c r="E2287" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/italian-20lira-emanuele/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2288">
+      <c r="A2288" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2288" t="inlineStr">
+        <is>
+          <t>20 лири златна монета Умберто I, Италия</t>
+        </is>
+      </c>
+      <c r="C2288" t="n">
+        <v>1052</v>
+      </c>
+      <c r="D2288" t="n">
+        <v>1083</v>
+      </c>
+      <c r="E2288" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-liri-zlatna-moneta-umberto-i-italiya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2289">
+      <c r="A2289" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2289" t="inlineStr">
+        <is>
+          <t>4 австрийски дуката златна монета Франц Йосиф</t>
+        </is>
+      </c>
+      <c r="C2289" t="n">
+        <v>2442</v>
+      </c>
+      <c r="D2289" t="n">
+        <v>2640</v>
+      </c>
+      <c r="E2289" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-4-avstriiski-dukata-franc-iosif/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2290">
+      <c r="A2290" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2290" t="inlineStr">
+        <is>
+          <t>1 австрийски дукат златна монета Франц Йосиф</t>
+        </is>
+      </c>
+      <c r="C2290" t="n">
+        <v>628</v>
+      </c>
+      <c r="D2290" t="n">
+        <v>663</v>
+      </c>
+      <c r="E2290" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-1-avstriiski-dukat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2291">
+      <c r="A2291" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2291" t="inlineStr">
+        <is>
+          <t>8 форинта/20 франка Франц Йосиф Унгария</t>
+        </is>
+      </c>
+      <c r="C2291" t="n">
+        <v>1050</v>
+      </c>
+      <c r="D2291" t="n">
+        <v>1108</v>
+      </c>
+      <c r="E2291" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-forinta-20-franka-franc-iosif-ungariia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2292">
+      <c r="A2292" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2292" t="inlineStr">
+        <is>
+          <t>Златна монета 4 флорина/10 франка Франц Йосиф, Австрия</t>
+        </is>
+      </c>
+      <c r="C2292" t="n">
+        <v>551</v>
+      </c>
+      <c r="D2292" t="n">
+        <v>589</v>
+      </c>
+      <c r="E2292" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-4-florina-10-franka-franc-iosif-avstria/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2293">
+      <c r="A2293" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2293" t="inlineStr">
+        <is>
+          <t>20 франка златна монета Швейцария Вренели</t>
+        </is>
+      </c>
+      <c r="C2293" t="n">
+        <v>1050</v>
+      </c>
+      <c r="D2293" t="n">
+        <v>1083</v>
+      </c>
+      <c r="E2293" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-zlatni-franka-shveitsariya-vreneli/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2294">
+      <c r="A2294" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2294" t="inlineStr">
+        <is>
+          <t>10 гулдена Вилхелмина Холандия</t>
+        </is>
+      </c>
+      <c r="C2294" t="n">
+        <v>1069</v>
+      </c>
+      <c r="D2294" t="n">
+        <v>1161</v>
+      </c>
+      <c r="E2294" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-guldena-vilhemina-holandiya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2295">
+      <c r="A2295" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2295" t="inlineStr">
+        <is>
+          <t>20 германски марки Вилхелм II</t>
+        </is>
+      </c>
+      <c r="C2295" t="n">
+        <v>1283</v>
+      </c>
+      <c r="D2295" t="n">
+        <v>1380</v>
+      </c>
+      <c r="E2295" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-germanski-marki-vilhelm-ii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2296">
+      <c r="A2296" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2296" t="inlineStr">
+        <is>
+          <t>Златен Мемориален Суверен Чарлз III Великобритания 2022г.</t>
+        </is>
+      </c>
+      <c r="C2296" t="n">
+        <v>1325</v>
+      </c>
+      <c r="D2296" t="n">
+        <v>1384</v>
+      </c>
+      <c r="E2296" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-memorialen-suveren-charles-iii-2022/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2297">
+      <c r="A2297" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2297" t="inlineStr">
+        <is>
+          <t>Златен Суверен Чарлз III Великобритания</t>
+        </is>
+      </c>
+      <c r="C2297" t="n">
+        <v>1331</v>
+      </c>
+      <c r="D2297" t="n">
+        <v>1390</v>
+      </c>
+      <c r="E2297" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-charles-iii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2298">
+      <c r="A2298" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2298" t="inlineStr">
+        <is>
+          <t>Златен суверен Елизабет II 1957-2021 Великобритания</t>
+        </is>
+      </c>
+      <c r="C2298" t="n">
+        <v>1298</v>
+      </c>
+      <c r="D2298" t="n">
+        <v>1348</v>
+      </c>
+      <c r="E2298" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/suveren-elizabet-ii-velikobritaniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2299">
+      <c r="A2299" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2299" t="inlineStr">
+        <is>
+          <t>Златен суверен Едуард VII Великобритания</t>
+        </is>
+      </c>
+      <c r="C2299" t="n">
+        <v>1298</v>
+      </c>
+      <c r="D2299" t="n">
+        <v>1371</v>
+      </c>
+      <c r="E2299" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-eduard-vii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2300">
+      <c r="A2300" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2300" t="inlineStr">
+        <is>
+          <t>Златен суверен Джордж V Великобритания</t>
+        </is>
+      </c>
+      <c r="C2300" t="n">
+        <v>1298</v>
+      </c>
+      <c r="D2300" t="n">
+        <v>1371</v>
+      </c>
+      <c r="E2300" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-jorge-v/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2301">
+      <c r="A2301" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2301" t="inlineStr">
+        <is>
+          <t>Златен суверен Виктория Великобритания</t>
+        </is>
+      </c>
+      <c r="C2301" t="n">
+        <v>1298</v>
+      </c>
+      <c r="D2301" t="n">
+        <v>1384</v>
+      </c>
+      <c r="E2301" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-suveren-viktoriya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2302">
+      <c r="A2302" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2302" t="inlineStr">
+        <is>
+          <t>Британски златен суверен Елизабет II, 2022г.</t>
+        </is>
+      </c>
+      <c r="C2302" t="n">
+        <v>1298</v>
+      </c>
+      <c r="D2302" t="inlineStr"/>
+      <c r="E2302" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlaten-britanski-suveren-elizabet-ii-2022/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2303">
+      <c r="A2303" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2303" t="inlineStr">
+        <is>
+          <t>20 франка златна монета Тунис</t>
+        </is>
+      </c>
+      <c r="C2303" t="n">
+        <v>1045</v>
+      </c>
+      <c r="D2303" t="n">
+        <v>1139</v>
+      </c>
+      <c r="E2303" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/20-franka-zlatna-moneta-tunis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2304">
+      <c r="A2304" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2304" t="inlineStr">
+        <is>
+          <t>Златна монета 100 турски куруша</t>
+        </is>
+      </c>
+      <c r="C2304" t="n">
+        <v>1045</v>
+      </c>
+      <c r="D2304" t="inlineStr"/>
+      <c r="E2304" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-100-turski-kurusha/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2305">
+      <c r="A2305" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2305" t="inlineStr">
+        <is>
+          <t>Златна монета 50 песос, Мексико</t>
+        </is>
+      </c>
+      <c r="C2305" t="n">
+        <v>6649</v>
+      </c>
+      <c r="D2305" t="n">
+        <v>7056</v>
+      </c>
+      <c r="E2305" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-50-pesos-meksiko/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2306">
+      <c r="A2306" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2306" t="inlineStr">
+        <is>
+          <t>Златна монета 100 австрийски корони Франц Йосиф</t>
+        </is>
+      </c>
+      <c r="C2306" t="n">
+        <v>5324</v>
+      </c>
+      <c r="D2306" t="n">
+        <v>5709</v>
+      </c>
+      <c r="E2306" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/zlatna-moneta-100-avstriyski-koroni-franc-yosif/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2307">
+      <c r="A2307" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2307" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2307" t="n">
+        <v>5426</v>
+      </c>
+      <c r="D2307" t="n">
+        <v>5750</v>
+      </c>
+      <c r="E2307" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2308">
+      <c r="A2308" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2308" t="inlineStr">
+        <is>
+          <t>15 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2308" t="n">
+        <v>2713</v>
+      </c>
+      <c r="D2308" t="n">
+        <v>2968</v>
+      </c>
+      <c r="E2308" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/15-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2309">
+      <c r="A2309" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2309" t="inlineStr">
+        <is>
+          <t>8 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2309" t="n">
+        <v>1447</v>
+      </c>
+      <c r="D2309" t="n">
+        <v>1625</v>
+      </c>
+      <c r="E2309" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2310">
+      <c r="A2310" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2310" t="inlineStr">
+        <is>
+          <t>3 грама златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2310" t="n">
+        <v>543</v>
+      </c>
+      <c r="D2310" t="n">
+        <v>689</v>
+      </c>
+      <c r="E2310" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/3-grama-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2311">
+      <c r="A2311" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2311" t="inlineStr">
+        <is>
+          <t>1 грам златна монета Китайска панда 2025</t>
+        </is>
+      </c>
+      <c r="C2311" t="n">
+        <v>181</v>
+      </c>
+      <c r="D2311" t="n">
+        <v>274</v>
+      </c>
+      <c r="E2311" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatna-moneta-kitaiska-panda-2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2312">
+      <c r="A2312" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2312" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Тигъра 2022</t>
+        </is>
+      </c>
+      <c r="C2312" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2312" t="n">
+        <v>8243</v>
+      </c>
+      <c r="E2312" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-oz-australian-lunar-year-of-the-tiger-2022-gold-coin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2313">
+      <c r="A2313" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2313" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Вола 2021</t>
+        </is>
+      </c>
+      <c r="C2313" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2313" t="n">
+        <v>6594</v>
+      </c>
+      <c r="E2313" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-oz-australian-lunar-year-of-the-ox-2021-gold-coin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2314">
+      <c r="A2314" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2314" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Австралийски лунар година на Мишката 2020</t>
+        </is>
+      </c>
+      <c r="C2314" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2314" t="n">
+        <v>6484</v>
+      </c>
+      <c r="E2314" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyski-lunar-godina-mishkata-2020/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2315">
+      <c r="A2315" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2315" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Кучето 2018</t>
+        </is>
+      </c>
+      <c r="C2315" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2315" t="n">
+        <v>6484</v>
+      </c>
+      <c r="E2315" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni38s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-22/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2316">
+      <c r="A2316" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2316" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Петела 2017</t>
+        </is>
+      </c>
+      <c r="C2316" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2316" t="n">
+        <v>6484</v>
+      </c>
+      <c r="E2316" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni40s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-24/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2317">
+      <c r="A2317" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2317" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Маймуната 2016</t>
+        </is>
+      </c>
+      <c r="C2317" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2317" t="n">
+        <v>6484</v>
+      </c>
+      <c r="E2317" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-maimunata-2016/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2318">
+      <c r="A2318" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2318" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Змията 2013</t>
+        </is>
+      </c>
+      <c r="C2318" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2318" t="n">
+        <v>6594</v>
+      </c>
+      <c r="E2318" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlaten-avstraliiski-lunar-godina-na-zmiyata-2013/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2319">
+      <c r="A2319" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2319" t="inlineStr">
+        <is>
+          <t>1 унция австралиисйки лунар година на дракона 2012</t>
+        </is>
+      </c>
+      <c r="C2319" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2319" t="n">
+        <v>6484</v>
+      </c>
+      <c r="E2319" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-drakona-2012/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2320">
+      <c r="A2320" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2320" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Заека 2011</t>
+        </is>
+      </c>
+      <c r="C2320" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2320" t="n">
+        <v>6484</v>
+      </c>
+      <c r="E2320" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-moneta-avstraliiski-lunar-zaek-2011/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2321">
+      <c r="A2321" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2321" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Вола 2009</t>
+        </is>
+      </c>
+      <c r="C2321" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2321" t="n">
+        <v>6484</v>
+      </c>
+      <c r="E2321" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-avstraliiski-lunar-godina-na-vola-2009/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2322">
+      <c r="A2322" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2322" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Мишката 2008</t>
+        </is>
+      </c>
+      <c r="C2322" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2322" t="n">
+        <v>6484</v>
+      </c>
+      <c r="E2322" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-uncia-moneta-lunar-mishka-2008/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2323">
+      <c r="A2323" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2323" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Прасето 2007</t>
+        </is>
+      </c>
+      <c r="C2323" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2323" t="n">
+        <v>6484</v>
+      </c>
+      <c r="E2323" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-avstraliiski-lunar-godina-na-praseto-2007/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2324">
+      <c r="A2324" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2324" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Петела 2005</t>
+        </is>
+      </c>
+      <c r="C2324" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2324" t="n">
+        <v>6484</v>
+      </c>
+      <c r="E2324" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-petela-2005/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2325">
+      <c r="A2325" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2325" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийски лунар година на Маймуната 2004</t>
+        </is>
+      </c>
+      <c r="C2325" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2325" t="n">
+        <v>6484</v>
+      </c>
+      <c r="E2325" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-%d1%83%d0%bd%d1%86%d0%b8%d1%8f-%d0%b7%d0%bb%d0%b0%d1%82%d0%b5%d0%bd-%d0%b0%d0%b2%d1%81%d1%82%d1%80%d0%b0%d0%bb%d0%b8%d0%b9%d1%81%d0%ba%d0%b8-%d0%bb%d1%83%d0%bd%d0%b0%d1%80-%d0%b3%d0%be%d0%b4%d0%b8-2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2326">
+      <c r="A2326" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2326" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Козата 2003</t>
+        </is>
+      </c>
+      <c r="C2326" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2326" t="n">
+        <v>6484</v>
+      </c>
+      <c r="E2326" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni38s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-24/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2327">
+      <c r="A2327" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2327" t="inlineStr">
+        <is>
+          <t>1 унция златна монета австралийки Лунар 2000 година на дракона</t>
+        </is>
+      </c>
+      <c r="C2327" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2327" t="n">
+        <v>7419</v>
+      </c>
+      <c r="E2327" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliyki-lunar-2000-godina-drakona/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2328">
+      <c r="A2328" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2328" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Тигъра 2010</t>
+        </is>
+      </c>
+      <c r="C2328" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2328" t="inlineStr"/>
+      <c r="E2328" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-tigura-2010/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2329">
+      <c r="A2329" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2329" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Кучето 2006</t>
+        </is>
+      </c>
+      <c r="C2329" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2329" t="n">
+        <v>6484</v>
+      </c>
+      <c r="E2329" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-kucheto-2006/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2330">
+      <c r="A2330" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2330" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Тигъра 1998</t>
+        </is>
+      </c>
+      <c r="C2330" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2330" t="n">
+        <v>6869</v>
+      </c>
+      <c r="E2330" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliiski-lunar-godinata-na-tigara-1998/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2331">
+      <c r="A2331" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2331" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Вола 1997</t>
+        </is>
+      </c>
+      <c r="C2331" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2331" t="n">
+        <v>6869</v>
+      </c>
+      <c r="E2331" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-avstraliiski-lunar-godinata-na-vola-1997/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2332">
+      <c r="A2332" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2332" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Мишката 1996</t>
+        </is>
+      </c>
+      <c r="C2332" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2332" t="inlineStr"/>
+      <c r="E2332" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni42s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2333">
+      <c r="A2333" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2333" t="inlineStr">
+        <is>
+          <t>1 унция златен австралийски лунар година на Коня 2014</t>
+        </is>
+      </c>
+      <c r="C2333" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2333" t="inlineStr"/>
+      <c r="E2333" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciq-avstraliiski-lunar-godina-na-konq-2014/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2334">
+      <c r="A2334" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2334" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче Argor-Heraeus лунар Дракон 2024</t>
+        </is>
+      </c>
+      <c r="C2334" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2334" t="inlineStr"/>
+      <c r="E2334" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-argor-heraeus-lunar-drakon-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2335">
+      <c r="A2335" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2335" t="inlineStr">
+        <is>
+          <t>1 грам златно кюлче Argor-Heraeus лунар Дракон 2024</t>
+        </is>
+      </c>
+      <c r="C2335" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2335" t="inlineStr"/>
+      <c r="E2335" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatno-kyulche-argor-heraeus-lunar-drakon-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2336">
+      <c r="A2336" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2336" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2336" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2336" t="inlineStr"/>
+      <c r="E2336" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2337">
+      <c r="A2337" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2337" t="inlineStr">
+        <is>
+          <t>15 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2337" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2337" t="inlineStr"/>
+      <c r="E2337" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/15-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2338">
+      <c r="A2338" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2338" t="inlineStr">
+        <is>
+          <t>8 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2338" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2338" t="inlineStr"/>
+      <c r="E2338" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2339">
+      <c r="A2339" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2339" t="inlineStr">
+        <is>
+          <t>3 грама златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2339" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2339" t="inlineStr"/>
+      <c r="E2339" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/3-grama-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2340">
+      <c r="A2340" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2340" t="inlineStr">
+        <is>
+          <t>1 грам златна монета Китайска панда 2024</t>
+        </is>
+      </c>
+      <c r="C2340" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2340" t="inlineStr"/>
+      <c r="E2340" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatna-moneta-kitayska-panda-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2341">
+      <c r="A2341" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2341" t="inlineStr">
+        <is>
+          <t>1/2 унция златна монета Австралийски лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C2341" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2341" t="inlineStr"/>
+      <c r="E2341" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-2-unciya-zlatna-moneta-avstraliyski-lunar-godina-drakona-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2342">
+      <c r="A2342" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2342" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Драконът на Тюдор 2024г.</t>
+        </is>
+      </c>
+      <c r="C2342" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2342" t="inlineStr"/>
+      <c r="E2342" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-pazitelite-na-tudorite-drakonat-na-tudor-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2343">
+      <c r="A2343" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2343" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Еднорогът на Сиймор 2024 г.</t>
+        </is>
+      </c>
+      <c r="C2343" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2343" t="inlineStr"/>
+      <c r="E2343" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-pazitelite-na-tyudorite-ednorogut-na-siimor-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2344">
+      <c r="A2344" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2344" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Бикът от Кларънс 2023 г.</t>
+        </is>
+      </c>
+      <c r="C2344" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2344" t="inlineStr"/>
+      <c r="E2344" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-pazitelite-na-tyudorite-bikut-ot-klaruns-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2345">
+      <c r="A2345" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2345" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Британия - Елизабет II</t>
+        </is>
+      </c>
+      <c r="C2345" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2345" t="inlineStr"/>
+      <c r="E2345" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatna-moneta-britaniya-elizabet-ii/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2346">
+      <c r="A2346" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2346" t="inlineStr">
+        <is>
+          <t>1 унция златна монета Пазителите на Тюдорите - Йейлът на Бофорт 2023 г.</t>
+        </is>
+      </c>
+      <c r="C2346" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2346" t="inlineStr"/>
+      <c r="E2346" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-oz-zlatna-moneta-pazitelite-na-tyudorite-yeylut-na-bofort-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2347">
+      <c r="A2347" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2347" t="inlineStr">
+        <is>
+          <t>1/2 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2347" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2347" t="inlineStr"/>
+      <c r="E2347" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-2-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2348">
+      <c r="A2348" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2348" t="inlineStr">
+        <is>
+          <t>1/4 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2348" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2348" t="inlineStr"/>
+      <c r="E2348" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-4-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2349">
+      <c r="A2349" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2349" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP лунар година на Дракона 2024</t>
+        </is>
+      </c>
+      <c r="C2349" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2349" t="inlineStr"/>
+      <c r="E2349" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-pamp-lunar-drakon-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2350">
+      <c r="A2350" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2350" t="inlineStr">
+        <is>
+          <t>5 грама златно кюлче PAMP лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2350" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2350" t="inlineStr"/>
+      <c r="E2350" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/5-grama-zlatno-kyulche-pamp-lunar-zaek-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2351">
+      <c r="A2351" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2351" t="inlineStr">
+        <is>
+          <t>1/10 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2351" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2351" t="inlineStr"/>
+      <c r="E2351" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-10-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2352">
+      <c r="A2352" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2352" t="inlineStr">
+        <is>
+          <t>15 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2352" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2352" t="inlineStr"/>
+      <c r="E2352" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/15-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2353">
+      <c r="A2353" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2353" t="inlineStr">
+        <is>
+          <t>1/20 унция златен австралийски лунар година на Заека 2023</t>
+        </is>
+      </c>
+      <c r="C2353" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2353" t="inlineStr"/>
+      <c r="E2353" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-20-unciya-zlaten-avstraliiski-lunar-godina-na-zaeka-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2354">
+      <c r="A2354" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2354" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2354" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2354" t="inlineStr"/>
+      <c r="E2354" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2355">
+      <c r="A2355" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2355" t="inlineStr">
+        <is>
+          <t>8 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2355" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2355" t="inlineStr"/>
+      <c r="E2355" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/8-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2356">
+      <c r="A2356" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2356" t="inlineStr">
+        <is>
+          <t>3 грама златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2356" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2356" t="inlineStr"/>
+      <c r="E2356" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/3-grama-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2357">
+      <c r="A2357" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2357" t="inlineStr">
+        <is>
+          <t>1 грам златна монета Китайска панда 2023</t>
+        </is>
+      </c>
+      <c r="C2357" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2357" t="inlineStr"/>
+      <c r="E2357" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-gram-zlatna-moneta-kitayska-panda-2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2358">
+      <c r="A2358" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2358" t="inlineStr">
+        <is>
+          <t>100 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2358" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2358" t="inlineStr"/>
+      <c r="E2358" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/100-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2359">
+      <c r="A2359" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2359" t="inlineStr">
+        <is>
+          <t>50 грама златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2359" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2359" t="inlineStr"/>
+      <c r="E2359" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/50-grama-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2360">
+      <c r="A2360" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2360" t="inlineStr">
+        <is>
+          <t>1 унция златно кюлче PAMP Фортуна</t>
+        </is>
+      </c>
+      <c r="C2360" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2360" t="inlineStr"/>
+      <c r="E2360" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/1-unciya-zlatno-kulche-pamp-fortuna/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2361">
+      <c r="A2361" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2361" t="inlineStr">
+        <is>
+          <t>10 крони Кристиян X Дания</t>
+        </is>
+      </c>
+      <c r="C2361" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2361" t="inlineStr"/>
+      <c r="E2361" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-kroni-kristiyan-x-daniya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2362">
+      <c r="A2362" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2362" t="inlineStr">
+        <is>
+          <t>10 Гулдена Вилхелм III Холандия</t>
+        </is>
+      </c>
+      <c r="C2362" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2362" t="inlineStr"/>
+      <c r="E2362" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/a5s12listpositioni38s12attributekeys12slug_seo_urls13attributenames47%d0%bf%d1%8a%d1%82-%d0%b4%d0%be-%d1%81%d1%82%d1%80%d0%b0%d0%bd%d1%86%d0%b8%d1%82%d0%b0%d1%82%d0%b0-seo-9/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2363">
+      <c r="A2363" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2363" t="inlineStr">
+        <is>
+          <t>30 грама златна монета Китайска панда 2022</t>
+        </is>
+      </c>
+      <c r="C2363" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2363" t="inlineStr"/>
+      <c r="E2363" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/30-grama-zlatna-moneta-kitayska-panda-2022/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2364">
+      <c r="A2364" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2364" t="inlineStr">
+        <is>
+          <t>Златна монета 10 франка Мариана</t>
+        </is>
+      </c>
+      <c r="C2364" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2364" t="inlineStr"/>
+      <c r="E2364" t="inlineStr">
+        <is>
+          <t>https://tavex.bg/zlato/10-frenski-franka-mariana/</t>
+        </is>
+      </c>
+    </row>
+    <row r="2365">
+      <c r="A2365" s="2" t="n">
+        <v>45708.85989896983</v>
+      </c>
+      <c r="B2365" t="inlineStr">
+        <is>
+          <t>1 килограм златно кюлче Valcambi</t>
+        </is>
+      </c>
+      <c r="C2365" t="n">
+        <v>5681</v>
+      </c>
+      <c r="D2365" t="inlineStr"/>
+      <c r="E2365" t="inlineStr">
         <is>
           <t>https://tavex.bg/zlato/1-kilogram-zlatno-kulche-valcambi/</t>
         </is>

</xml_diff>